<commit_message>
Update structure of equipment element
</commit_message>
<xml_diff>
--- a/Examples/DCC_temperature.xlsx
+++ b/Examples/DCC_temperature.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tesla\Data\MS\4006-03 AI metrologi\Software\DCCtables\master\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\MS\4006-03 AI metrologi\Software\DCCtables\master\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D4232B-A177-4672-AA2F-092B15AC6CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="34320" windowHeight="19680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21396" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -23,10 +22,11 @@
     <sheet name="Software" sheetId="8" state="hidden" r:id="rId8"/>
     <sheet name="Locations" sheetId="13" state="hidden" r:id="rId9"/>
     <sheet name="Equipment" sheetId="12" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
   <definedNames>
     <definedName name="ColType" localSheetId="3">[1]Definitions!$A$2:$A$6</definedName>
@@ -41,7 +41,7 @@
     <definedName name="statementCategories">Definitions!$F$2:$F$10</definedName>
     <definedName name="UsedReference">metaDataType</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="524">
   <si>
     <t>customerTag</t>
   </si>
@@ -364,9 +364,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>swRef</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -1042,9 +1039,6 @@
     <t>\zepto</t>
   </si>
   <si>
-    <t>nan</t>
-  </si>
-  <si>
     <t>Customer Tags</t>
   </si>
   <si>
@@ -1054,9 +1048,6 @@
     <t>TempCal</t>
   </si>
   <si>
-    <t>NN32</t>
-  </si>
-  <si>
     <t>Amitek</t>
   </si>
   <si>
@@ -1117,9 +1108,6 @@
     <t>DANAK</t>
   </si>
   <si>
-    <t>itemID1 itemID2</t>
-  </si>
-  <si>
     <t>itemRef</t>
   </si>
   <si>
@@ -1159,9 +1147,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>itemID2</t>
-  </si>
-  <si>
     <t>NN14</t>
   </si>
   <si>
@@ -1192,21 +1177,9 @@
     <t>productNumber</t>
   </si>
   <si>
-    <t>serialNumber</t>
-  </si>
-  <si>
-    <t>customerId</t>
-  </si>
-  <si>
-    <t>itemID3</t>
-  </si>
-  <si>
     <t>another display unit</t>
   </si>
   <si>
-    <t>NN15</t>
-  </si>
-  <si>
     <t>silver edition</t>
   </si>
   <si>
@@ -1238,18 +1211,6 @@
   </si>
   <si>
     <t>Equipment Categories</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>equipID4</t>
-  </si>
-  <si>
-    <t>DFM 1542</t>
   </si>
   <si>
     <t>StreetNo</t>
@@ -1560,9 +1521,6 @@
     <t>Chino</t>
   </si>
   <si>
-    <t>R800-2</t>
-  </si>
-  <si>
     <t>RS927-5</t>
   </si>
   <si>
@@ -1582,12 +1540,111 @@
   </si>
   <si>
     <t>DFM9511</t>
+  </si>
+  <si>
+    <t>item1</t>
+  </si>
+  <si>
+    <t>item2</t>
+  </si>
+  <si>
+    <t>item3</t>
+  </si>
+  <si>
+    <t>equip1</t>
+  </si>
+  <si>
+    <t>item1 item2</t>
+  </si>
+  <si>
+    <t>Temparatursensor</t>
+  </si>
+  <si>
+    <t>Visningsenhed</t>
+  </si>
+  <si>
+    <t>Ekstra visningsenhed</t>
+  </si>
+  <si>
+    <t>DFMs hovedrefererence</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>item01</t>
+  </si>
+  <si>
+    <t>product name</t>
+  </si>
+  <si>
+    <t>prodcut number</t>
+  </si>
+  <si>
+    <t>issuer</t>
+  </si>
+  <si>
+    <t>id1</t>
+  </si>
+  <si>
+    <t>id1 heading lang1</t>
+  </si>
+  <si>
+    <t>id1 issuer</t>
+  </si>
+  <si>
+    <t>id1 heading lang2</t>
+  </si>
+  <si>
+    <t>NN12</t>
+  </si>
+  <si>
+    <t>NN13</t>
+  </si>
+  <si>
+    <t>DFM 432</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>DFM no</t>
+  </si>
+  <si>
+    <t>Client label</t>
+  </si>
+  <si>
+    <t>Kundens id</t>
+  </si>
+  <si>
+    <t>DFMnummer</t>
+  </si>
+  <si>
+    <t>id2 issuer</t>
+  </si>
+  <si>
+    <t>id2</t>
+  </si>
+  <si>
+    <t>id2 heading lang1</t>
+  </si>
+  <si>
+    <t>Serienummer</t>
+  </si>
+  <si>
+    <t>Serial number</t>
+  </si>
+  <si>
+    <t>id2 heading lang2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1660,7 +1717,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1724,6 +1781,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1806,7 +1869,7 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -1918,6 +1981,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
@@ -2014,11 +2079,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Definitions"/>
       <sheetName val="AdministrativeData"/>
@@ -2865,7 +2927,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Januar"/>
@@ -3017,71 +3079,77 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DCFE7457-6089-422F-AE8B-F93B5CC6D5E3}" name="Table135" displayName="Table135" ref="C1:G8" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="C1:G8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table135" displayName="Table135" ref="C1:G8" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="C1:G8"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B6460555-0E0D-4889-8643-C5F57DB2E042}" name="id"/>
-    <tableColumn id="3" xr3:uid="{C1C3BF6A-959C-4D7D-AC99-517770D89042}" name="heading lang1"/>
-    <tableColumn id="4" xr3:uid="{82EC8405-575B-45C9-97A5-B2BE0DFA2511}" name="body lang1" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{19BCF9E6-A96F-4617-BFC8-5BA713CC7CF5}" name="heading lang2"/>
-    <tableColumn id="6" xr3:uid="{EC9151B2-0AB3-48BB-A419-43898218651D}" name="body lang2" dataDxfId="3"/>
+    <tableColumn id="1" name="id"/>
+    <tableColumn id="3" name="heading lang1"/>
+    <tableColumn id="4" name="body lang1" dataDxfId="4"/>
+    <tableColumn id="5" name="heading lang2"/>
+    <tableColumn id="6" name="body lang2" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table14" displayName="Table14" ref="A1:H6" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:H6" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:H6" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:H6"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="swID"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="release "/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="type"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="description"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="content"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="file"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="formula"/>
+    <tableColumn id="1" name="swID"/>
+    <tableColumn id="2" name="name"/>
+    <tableColumn id="3" name="release "/>
+    <tableColumn id="4" name="type"/>
+    <tableColumn id="5" name="description"/>
+    <tableColumn id="6" name="content"/>
+    <tableColumn id="7" name="file"/>
+    <tableColumn id="8" name="formula"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1BBFECBA-56D4-4850-A69E-DDD8D8846A58}" name="Table167" displayName="Table167" ref="A1:M6" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:M6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table167" displayName="Table167" ref="A1:M6" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:M6"/>
   <tableColumns count="13">
-    <tableColumn id="11" xr3:uid="{04D47612-4EBB-4C61-8AA2-577AC8EF81C5}" name="Category"/>
-    <tableColumn id="1" xr3:uid="{1806EC44-C85B-49CD-AF40-4809015F8B91}" name="id"/>
-    <tableColumn id="10" xr3:uid="{037FC876-FCB0-4BD8-B949-CCDFEF3DB5C3}" name="Name1"/>
-    <tableColumn id="13" xr3:uid="{059EB501-42EB-481D-BD96-60B1F9F8E0BF}" name="Name2"/>
-    <tableColumn id="2" xr3:uid="{4B415654-8F7A-40C8-BE3F-C07A4342B8A8}" name="Street1"/>
-    <tableColumn id="3" xr3:uid="{8C44E7BB-FF2E-44D7-8032-0F3A17D4F953}" name="StreetNo"/>
-    <tableColumn id="14" xr3:uid="{D59D5E06-76EA-4FBE-A02E-AB131783E17F}" name="Column1"/>
-    <tableColumn id="4" xr3:uid="{A708A527-4B82-4729-94A7-E36DC2AB792E}" name="City"/>
-    <tableColumn id="5" xr3:uid="{F5A5DD0D-3003-45A9-975B-5FFE69D70DD2}" name="PostCode"/>
-    <tableColumn id="6" xr3:uid="{907E8258-546A-4ED6-80F0-FF4C0BB84D88}" name="PO-BOX"/>
-    <tableColumn id="7" xr3:uid="{18EA1B9E-9FA2-4BB9-B5B5-C58EAD2FEB62}" name="CountryCode"/>
-    <tableColumn id="8" xr3:uid="{BD63A030-E943-4AE2-BD22-F3A03E64E7FD}" name="further"/>
-    <tableColumn id="9" xr3:uid="{7E706009-4E8A-4143-8D41-18D74C7EFA47}" name="p"/>
+    <tableColumn id="11" name="Category"/>
+    <tableColumn id="1" name="id"/>
+    <tableColumn id="10" name="Name1"/>
+    <tableColumn id="13" name="Name2"/>
+    <tableColumn id="2" name="Street1"/>
+    <tableColumn id="3" name="StreetNo"/>
+    <tableColumn id="14" name="Column1"/>
+    <tableColumn id="4" name="City"/>
+    <tableColumn id="5" name="PostCode"/>
+    <tableColumn id="6" name="PO-BOX"/>
+    <tableColumn id="7" name="CountryCode"/>
+    <tableColumn id="8" name="further"/>
+    <tableColumn id="9" name="p"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B838957E-BA60-4601-B76A-05754E31F1D4}" name="Table16" displayName="Table16" ref="B1:J6" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B1:J6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="9">
-    <tableColumn id="11" xr3:uid="{2F03DDC1-5525-47DB-9C7A-78876A716A29}" name="category"/>
-    <tableColumn id="1" xr3:uid="{EA082D58-1E08-4AD3-BFAF-E947B2336921}" name="id"/>
-    <tableColumn id="2" xr3:uid="{B3FE107D-F1F8-4BA2-84D0-A4D664DA995B}" name="customerId"/>
-    <tableColumn id="4" xr3:uid="{257C57BA-5D0B-43F6-8D17-14F18E0B544F}" name="description"/>
-    <tableColumn id="5" xr3:uid="{8AA00CC2-F293-4BB3-A2C4-3B7F057C76DC}" name="swRef"/>
-    <tableColumn id="6" xr3:uid="{7A627269-42D2-425E-AC8C-45EC7EDF2E8C}" name="manufacturer"/>
-    <tableColumn id="7" xr3:uid="{62A0306E-96DA-4535-9CFB-48AF217F6E8E}" name="productName"/>
-    <tableColumn id="8" xr3:uid="{B1BA2124-70A6-4015-9AF1-FE74E51C0115}" name="productNumber"/>
-    <tableColumn id="9" xr3:uid="{B433F7BB-298D-4183-A3D7-5EC8642DEF72}" name="serialNumber"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="B1:P6" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B1:P6"/>
+  <tableColumns count="15">
+    <tableColumn id="11" name="category"/>
+    <tableColumn id="1" name="id"/>
+    <tableColumn id="4" name="heading lang1"/>
+    <tableColumn id="3" name="heading lang2"/>
+    <tableColumn id="6" name="manufacturer"/>
+    <tableColumn id="7" name="productName"/>
+    <tableColumn id="8" name="productNumber"/>
+    <tableColumn id="10" name="id1"/>
+    <tableColumn id="12" name="id1 issuer"/>
+    <tableColumn id="13" name="id1 heading lang1"/>
+    <tableColumn id="14" name="id1 heading lang2"/>
+    <tableColumn id="15" name="id2"/>
+    <tableColumn id="16" name="id2 issuer"/>
+    <tableColumn id="17" name="id2 heading lang1"/>
+    <tableColumn id="18" name="id2 heading lang2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3383,23 +3451,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" customWidth="1"/>
+    <col min="2" max="2" width="32.5546875" customWidth="1"/>
     <col min="3" max="3" width="62" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3420,36 +3488,36 @@
         <v>98</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="B2" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="D2" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="F2" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="G2" t="s">
-        <v>392</v>
+        <v>367</v>
       </c>
       <c r="I2" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="L2" s="2"/>
     </row>
@@ -3461,19 +3529,19 @@
         <v>24</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G3" t="s">
-        <v>393</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="L3" s="2"/>
     </row>
@@ -3485,16 +3553,16 @@
         <v>23</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F4" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="I4" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="L4" s="2"/>
     </row>
@@ -3503,37 +3571,37 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F5" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="I5" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F6" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="I6" t="s">
         <v>0</v>
@@ -3543,16 +3611,16 @@
     <row r="7" spans="1:12">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="I7" t="s">
         <v>19</v>
@@ -3564,16 +3632,16 @@
         <v>3</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F8" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="I8" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
       <c r="L8" s="2"/>
     </row>
@@ -3582,16 +3650,16 @@
         <v>4</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F9" t="s">
-        <v>431</v>
+        <v>418</v>
       </c>
       <c r="I9" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="L9" s="2"/>
     </row>
@@ -3600,16 +3668,16 @@
         <v>5</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F10" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
       <c r="I10" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="L10" s="2"/>
     </row>
@@ -3618,13 +3686,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I11" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="L11" s="2"/>
     </row>
@@ -3633,10 +3701,10 @@
         <v>22</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L12" s="2"/>
     </row>
@@ -3645,10 +3713,10 @@
         <v>39</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L13" s="2"/>
     </row>
@@ -3657,10 +3725,10 @@
         <v>40</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L14" s="2"/>
     </row>
@@ -3669,113 +3737,113 @@
         <v>43</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12">
       <c r="C16" s="30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="3:4">
       <c r="C17" s="30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="3:4">
       <c r="C18" s="30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="3:4">
       <c r="C19" s="30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="20" spans="3:4">
       <c r="C20" s="30" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
       <c r="D20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="3:4">
       <c r="C21" s="30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="3:4">
       <c r="C22" s="30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="3:4">
       <c r="C23" s="30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="24" spans="3:4">
       <c r="C24" s="30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="25" spans="3:4">
       <c r="C25" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="26" spans="3:4">
       <c r="C26" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="27" spans="3:4">
       <c r="C27" s="30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D27" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="28" spans="3:4">
       <c r="C28" s="30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D28" t="s">
         <v>28</v>
@@ -3783,39 +3851,39 @@
     </row>
     <row r="29" spans="3:4">
       <c r="C29" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="30" spans="3:4">
       <c r="C30" s="30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="31" spans="3:4">
       <c r="C31" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D31" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="32" spans="3:4">
       <c r="C32" s="30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D32" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="33" spans="3:4">
       <c r="C33" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D33" t="s">
         <v>27</v>
@@ -3823,771 +3891,771 @@
     </row>
     <row r="34" spans="3:4">
       <c r="C34" s="30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35" spans="3:4">
       <c r="C35" s="30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D35" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="36" spans="3:4">
       <c r="C36" s="30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D36" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="37" spans="3:4">
       <c r="C37" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D37" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="38" spans="3:4">
       <c r="C38" s="30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D38" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="39" spans="3:4">
       <c r="C39" s="30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D39" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="40" spans="3:4">
       <c r="C40" s="30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D40" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="41" spans="3:4">
       <c r="C41" s="30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D41" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="42" spans="3:4">
       <c r="C42" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D42" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="43" spans="3:4">
       <c r="C43" s="30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D43" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="44" spans="3:4">
       <c r="C44" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D44" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="45" spans="3:4">
       <c r="C45" s="30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D45" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="46" spans="3:4">
       <c r="C46" s="30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D46" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="47" spans="3:4">
       <c r="C47" s="30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D47" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="48" spans="3:4">
       <c r="C48" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D48" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="49" spans="3:4">
       <c r="C49" s="30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D49" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="50" spans="3:4">
       <c r="C50" s="30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D50" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="51" spans="3:4">
       <c r="C51" s="30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D51" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="52" spans="3:4">
       <c r="C52" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D52" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="53" spans="3:4">
       <c r="C53" s="30" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D53" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="54" spans="3:4">
       <c r="C54" s="30" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D54" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="55" spans="3:4">
       <c r="C55" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D55" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="56" spans="3:4">
       <c r="C56" s="30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D56" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="57" spans="3:4">
       <c r="C57" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D57" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="58" spans="3:4">
       <c r="C58" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D58" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="59" spans="3:4">
       <c r="C59" s="30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D59" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="60" spans="3:4">
       <c r="C60" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D60" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="61" spans="3:4">
       <c r="C61" s="30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D61" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="62" spans="3:4">
       <c r="C62" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D62" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="63" spans="3:4">
       <c r="C63" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D63" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="64" spans="3:4">
       <c r="C64" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="65" spans="3:4">
       <c r="C65" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D65" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="66" spans="3:4">
       <c r="C66" s="30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D66" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="67" spans="3:4">
       <c r="C67" s="30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D67" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="68" spans="3:4">
       <c r="C68" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="69" spans="3:4">
       <c r="C69" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="70" spans="3:4">
       <c r="C70" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="72" spans="3:4">
       <c r="C72" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="74" spans="3:4">
       <c r="C74" s="30" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="75" spans="3:4">
       <c r="C75" s="30" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="76" spans="3:4">
       <c r="C76" s="30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="77" spans="3:4">
       <c r="C77" s="30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="80" spans="3:4">
       <c r="C80" s="30" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81" s="30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="82" spans="3:3">
       <c r="C82" s="30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83" s="30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84" s="30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86" s="30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87" s="30" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="88" spans="3:3">
       <c r="C88" s="30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89" s="30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="90" spans="3:3">
       <c r="C90" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="91" spans="3:3">
       <c r="C91" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92" s="30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93" s="30" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="94" spans="3:3">
       <c r="C94" s="30" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="95" spans="3:3">
       <c r="C95" s="30" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="96" spans="3:3">
       <c r="C96" s="30" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="97" spans="3:3">
       <c r="C97" s="30" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="98" spans="3:3">
       <c r="C98" s="30" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="99" spans="3:3">
       <c r="C99" s="30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="100" spans="3:3">
       <c r="C100" s="30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="101" spans="3:3">
       <c r="C101" s="30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="102" spans="3:3">
       <c r="C102" s="30" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="103" spans="3:3">
       <c r="C103" s="30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="104" spans="3:3">
       <c r="C104" s="30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="105" spans="3:3">
       <c r="C105" s="30" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="106" spans="3:3">
       <c r="C106" s="30" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="107" spans="3:3">
       <c r="C107" s="30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="108" spans="3:3">
       <c r="C108" s="30" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="109" spans="3:3">
       <c r="C109" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="110" spans="3:3">
       <c r="C110" s="30" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="111" spans="3:3">
       <c r="C111" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="112" spans="3:3">
       <c r="C112" s="30" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="113" spans="3:3">
       <c r="C113" s="30" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="114" spans="3:3">
       <c r="C114" s="30" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="115" spans="3:3">
       <c r="C115" s="30" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="116" spans="3:3">
       <c r="C116" s="30" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="117" spans="3:3">
       <c r="C117" s="30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="118" spans="3:3">
       <c r="C118" s="30" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="119" spans="3:3">
       <c r="C119" s="30" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="120" spans="3:3">
       <c r="C120" s="30" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="121" spans="3:3">
       <c r="C121" s="30" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="122" spans="3:3">
       <c r="C122" s="30" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="123" spans="3:3">
       <c r="C123" s="30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="124" spans="3:3">
       <c r="C124" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="125" spans="3:3">
       <c r="C125" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="126" spans="3:3">
       <c r="C126" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="127" spans="3:3">
       <c r="C127" s="30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="128" spans="3:3">
       <c r="C128" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="129" spans="3:3">
       <c r="C129" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="130" spans="3:3">
       <c r="C130" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="131" spans="3:3">
       <c r="C131" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="132" spans="3:3">
       <c r="C132" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="133" spans="3:3">
       <c r="C133" s="30" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="134" spans="3:3">
       <c r="C134" s="30" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
     </row>
     <row r="135" spans="3:3">
       <c r="C135" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="136" spans="3:3">
       <c r="C136" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="137" spans="3:3">
       <c r="C137" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="138" spans="3:3">
       <c r="C138" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="139" spans="3:3">
       <c r="C139" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="https://www.metrology.net/wiki/testprocess-measure-conductance/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId2" display="https://www.metrology.net/wiki/testprocess-measure-conductivity/" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C5" r:id="rId3" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac/" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C6" r:id="rId4" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C7" r:id="rId5" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-squarewave/" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C8" r:id="rId6" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-trianglewave/" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C9" r:id="rId7" display="https://www.metrology.net/wiki/testprocess-measure-current-dc/" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C10" r:id="rId8" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-gas/" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C11" r:id="rId9" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-liquid/" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C12" r:id="rId10" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-solid/" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C13" r:id="rId11" display="https://www.metrology.net/wiki/testprocess-measure-force/" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="C14" r:id="rId12" display="https://www.metrology.net/wiki/testprocess-measure-frequency/" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="C15" r:id="rId13" display="https://www.metrology.net/wiki/testprocess-measure-frequency-amplitudemodulation-rate/" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="C16" r:id="rId14" display="https://www.metrology.net/wiki/testprocess-measure-frequency-frequencymodulation-deviation/" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="C17" r:id="rId15" display="https://www.metrology.net/wiki/testprocess-measure-frequency-frequencymodulation-rate/" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="C18" r:id="rId16" display="https://www.metrology.net/wiki/testprocess-measure-frequency-phasemodulation-rate/" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="C19" r:id="rId17" display="https://www.metrology.net/wiki/testprocess-measure-humidity-absolute/" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="C21" r:id="rId18" display="https://www.metrology.net/wiki/testprocess-measure-impedance/" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="C22" r:id="rId19" display="https://www.metrology.net/wiki/testprocess-measure-inductance/" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="C23" r:id="rId20" display="https://www.metrology.net/wiki/testprocess-measure-length/" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="C24" r:id="rId21" display="https://www.metrology.net/wiki/testprocess-measure-length-circumference/" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C25" r:id="rId22" display="https://www.metrology.net/wiki/testprocess-measure-length-diameter/" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="C26" r:id="rId23" display="https://www.metrology.net/wiki/testprocess-measure-length-form-flatness/" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="C27" r:id="rId24" display="https://www.metrology.net/wiki/testprocess-measure-length-form-parallelism/" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="C28" r:id="rId25" display="https://www.metrology.net/wiki/testprocess-measure-length-form-perpendicularity/" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="C29" r:id="rId26" display="https://www.metrology.net/wiki/testprocess-measure-length-form-roughness/" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="C30" r:id="rId27" display="https://www.metrology.net/wiki/testprocess-measure-length-form-roundness/" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C31" r:id="rId28" display="https://www.metrology.net/wiki/testprocess-measure-length-form-sphericity/" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="C32" r:id="rId29" display="https://www.metrology.net/wiki/testprocess-measure-length-form-straightness-axis/" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C33" r:id="rId30" display="https://www.metrology.net/wiki/testprocess-measure-length-form-straightness-surface/" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="C34" r:id="rId31" display="https://www.metrology.net/wiki/testprocess-measure-length-radius/" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="C35" r:id="rId32" display="https://www.metrology.net/wiki/testprocess-measure-mass-apparent/" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C36" r:id="rId33" display="https://www.metrology.net/wiki/testprocess-measure-mass-conventional/" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C37" r:id="rId34" display="https://www.metrology.net/wiki/testprocess-measure-mass-true/" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="C38" r:id="rId35" display="https://www.metrology.net/wiki/testprocess-measure-phase-phasemodulation/" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="C39" r:id="rId36" display="https://www.metrology.net/wiki/testprocess-measure-phase-reflectioncoefficent-rf/" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="C40" r:id="rId37" display="https://www.metrology.net/wiki/testprocess-measure-phase-reflectioncoefficent/" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="C41" r:id="rId38" display="https://www.metrology.net/wiki/testprocess-measure-phasenoise-sideband/" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="C42" r:id="rId39" display="https://www.metrology.net/wiki/testprocess-measure-power-rf-sinewave/" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="C43" r:id="rId40" display="https://www.metrology.net/wiki/testprocess-measure-pressure-hydraulic-static/" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="C44" r:id="rId41" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-absolute-static/" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="C45" r:id="rId42" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-differential-static/" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="C46" r:id="rId43" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-gage-static/" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="C47" r:id="rId44" display="https://www.metrology.net/wiki/testprocess-measure-ratio-amplitudemodulation/" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="C48" r:id="rId45" display="https://www.metrology.net/wiki/testprocess-measure-ratio-density-mass/" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="C49" r:id="rId46" display="https://www.metrology.net/wiki/testprocess-measure-ratio-humidity-relative/" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="C50" r:id="rId47" display="https://www.metrology.net/wiki/testprocess-measure-ratio-humidity-specific/" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="C51" r:id="rId48" display="https://www.metrology.net/wiki/testprocess-measure-ratio-reflectioncoefficent-rf/" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="C52" r:id="rId49" display="https://www.metrology.net/wiki/testprocess-measure-ratio-power-rf-sinewave-delta-frequency/" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="C53" r:id="rId50" display="https://www.metrology.net/wiki/testprocess-measure-ratio-power-rf-sinewave-delta-power/" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="C54" r:id="rId51" display="https://www.metrology.net/wiki/testprocess-measure-ratio-transmissioncoefficent/" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="C55" r:id="rId52" display="https://www.metrology.net/wiki/testprocess-measure-ratio-torque/" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="C56" r:id="rId53" display="https://www.metrology.net/wiki/testprocess-measure-ratio-voltage-ac-ripple-ondc/" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="C57" r:id="rId54" display="https://www.metrology.net/wiki/testprocess-measure-ratio-voltage-ac-sinewave-delta-frequency/" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="C58" r:id="rId55" display="https://www.metrology.net/wiki/testprocess-measure-ratio-volts-ac-sinewave-delta-volts/" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="C59" r:id="rId56" display="https://www.metrology.net/wiki/testprocess-measure-ohms/" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="C60" r:id="rId57" display="https://www.metrology.net/wiki/testprocess-measure-temperature/" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="C61" r:id="rId58" display="https://www.metrology.net/wiki/testprocess-measure-temperature-radiometric/" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="C62" r:id="rId59" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-prt/" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="C63" r:id="rId60" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-rtd/" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="C64" r:id="rId61" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-thermocouple/" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="C65" r:id="rId62" display="https://www.metrology.net/wiki/testprocess-measure-time-pulsetransition/" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="C66" r:id="rId63" display="https://www.metrology.net/wiki/testprocess-measure-time-absolute/" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="C67" r:id="rId64" display="https://www.metrology.net/wiki/testprocess-measure-torque/" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="C68" r:id="rId65" display="https://www.metrology.net/wiki/testprocess-measure-torque-hydraulicpressure/" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="C69" r:id="rId66" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac/" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="C70" r:id="rId67" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-noise-ondc/" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="C71" r:id="rId68" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="C72" r:id="rId69" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-squarewave/" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="C73" r:id="rId70" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-trianglewave/" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="C74" r:id="rId71" display="https://www.metrology.net/wiki/testprocess-measure-voltage-dc/" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="C75" r:id="rId72" display="https://www.metrology.net/wiki/testprocess-measure-weight/" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="C76" r:id="rId73" display="https://www.metrology.net/wiki/testprocess-source-capacitance/" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="C77" r:id="rId74" display="https://www.metrology.net/wiki/testprocess-source-conductance/" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="C78" r:id="rId75" display="https://www.metrology.net/wiki/testprocess-source-conductivity/" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="C79" r:id="rId76" display="https://www.metrology.net/wiki/testprocess-source-current-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="C80" r:id="rId77" display="https://www.metrology.net/wiki/testprocess-source-current-ac-squarewave/" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="C81" r:id="rId78" display="https://www.metrology.net/wiki/testprocess-source-current-ac-triangle/" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="C82" r:id="rId79" display="https://www.metrology.net/wiki/testprocess-source-current-dc/" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="C83" r:id="rId80" display="https://www.metrology.net/wiki/testprocess-source-density-mass-gas/" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="C84" r:id="rId81" display="https://www.metrology.net/wiki/testprocess-source-density-mass-liquid/" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="C85" r:id="rId82" display="https://www.metrology.net/wiki/testprocess-source-density-mass-solid/" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="C86" r:id="rId83" display="https://www.metrology.net/wiki/testprocess-source-force/" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="C87" r:id="rId84" display="https://www.metrology.net/wiki/testprocess-source-frequency-ac-squarewave/" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="C88" r:id="rId85" display="https://www.metrology.net/wiki/testprocess-source-frequency-arbitrary-cardiograph/" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="C89" r:id="rId86" display="https://www.metrology.net/wiki/testprocess-source-humidity-absolute/" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="C90" r:id="rId87" display="https://www.metrology.net/wiki/testprocess-source-impedance/" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="C91" r:id="rId88" display="https://www.metrology.net/wiki/testprocess-source-inductance/" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="C92" r:id="rId89" display="https://www.metrology.net/wiki/testprocess-source-length/" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="C93" r:id="rId90" display="https://www.metrology.net/wiki/testprocess-source-length-circumference/" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="C94" r:id="rId91" display="https://www.metrology.net/wiki/testprocess-source-length-diameter/" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="C95" r:id="rId92" display="https://www.metrology.net/wiki/testprocess-source-length-form-perpendicularity/" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="C96" r:id="rId93" display="https://www.metrology.net/wiki/testprocess-source-length-form-roundness/" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="C97" r:id="rId94" display="https://www.metrology.net/wiki/testprocess-source-length-form-sphericity/" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="C98" r:id="rId95" display="https://www.metrology.net/wiki/testprocess-source-length-form-straightness-surrface/" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="C99" r:id="rId96" display="https://www.metrology.net/wiki/testprocess-source-length-radius/" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="C100" r:id="rId97" display="https://www.metrology.net/wiki/testprocess-source-mass-apparent/" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="C101" r:id="rId98" display="https://www.metrology.net/wiki/testprocess-source-mass-conventional/" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="C102" r:id="rId99" display="https://www.metrology.net/wiki/testprocess-source-mass-true/" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="C103" r:id="rId100" display="https://www.metrology.net/wiki/testprocess-source-period-marker/" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="C104" r:id="rId101" display="https://www.metrology.net/wiki/testprocess-source-period-squarewave/" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="C105" r:id="rId102" display="https://www.metrology.net/wiki/testprocess-source-power-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="C106" r:id="rId103" display="https://www.metrology.net/wiki/testprocess-source-power-ac-sinewave-simulated/" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="C107" r:id="rId104" display="https://www.metrology.net/wiki/testprocess-source-power-dc-simulated/" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="C108" r:id="rId105" display="https://www.metrology.net/wiki/testprocess-source-power-noise-terminated/" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="C109" r:id="rId106" display="https://www.metrology.net/wiki/testprocess-source-power-rf-sinewave/" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="C110" r:id="rId107" display="https://www.metrology.net/wiki/testprocess-source-pressure-hydraulic-static/" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="C111" r:id="rId108" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-absolute-static/" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="C112" r:id="rId109" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-differential-static/" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="C113" r:id="rId110" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-gage-static/" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="C114" r:id="rId111" display="https://www.metrology.net/wiki/testprocess-source-ratio-amplitudemodulation/" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="C115" r:id="rId112" display="https://www.metrology.net/wiki/testprocess-source-ratio-humidity-relative/" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="C116" r:id="rId113" display="https://www.metrology.net/wiki/testprocess-source-ratio-humidity-specific/" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="C117" r:id="rId114" display="https://www.metrology.net/wiki/testprocess-source-ratio-rf-sinusoidal-delta-frequency/" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="C118" r:id="rId115" display="https://www.metrology.net/wiki/source-voltage-ac-sinewave-delta-frequency/" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="C119" r:id="rId116" display="https://www.metrology.net/wiki/testprocess-source-voltage-ac-sinewave-delta-voltage/" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="C120" r:id="rId117" display="https://www.metrology.net/wiki/testprocess-source-resistance/" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="C121" r:id="rId118" display="https://www.metrology.net/wiki/testprocess-source-temperature/" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="C122" r:id="rId119" display="https://www.metrology.net/wiki/testprocess-source-temperature-fixedpoint/" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="C123" r:id="rId120" display="https://www.metrology.net/wiki/testprocess-source-temperature-radiometric/" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="C124" r:id="rId121" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-prt/" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="C125" r:id="rId122" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-rtd/" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="C126" r:id="rId123" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-thermocouple/" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="C127" r:id="rId124" display="https://www.metrology.net/wiki/source-time-marker/" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="C128" r:id="rId125" display="https://www.metrology.net/wiki/testprocess-source-torque/" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="C129" r:id="rId126" display="https://www.metrology.net/wiki/source-voltage-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="C130" r:id="rId127" display="https://www.metrology.net/wiki/testprocess-source-voltage-dc/" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="C131" r:id="rId128" display="https://www.metrology.net/wiki/source-voltage-dc-delta/" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="C132" r:id="rId129" display="https://www.metrology.net/wiki/testprocess-source-voltage-noise-terminated/" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="C133" r:id="rId130" display="https://www.metrology.net/wiki/testprocess-source-voltage-shorted/" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="C134" r:id="rId131" display="https://www.metrology.net/wiki/testprocess-source-weight/" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="C20" r:id="rId132" display="https://www.metrology.net/wiki/testprocess-measure-humidity-absolute/" xr:uid="{606A194B-BA4C-4BE1-987D-8A8739C26FA4}"/>
+    <hyperlink ref="C3" r:id="rId1" display="https://www.metrology.net/wiki/testprocess-measure-conductance/"/>
+    <hyperlink ref="C4" r:id="rId2" display="https://www.metrology.net/wiki/testprocess-measure-conductivity/"/>
+    <hyperlink ref="C5" r:id="rId3" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac/"/>
+    <hyperlink ref="C6" r:id="rId4" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-sinewave/"/>
+    <hyperlink ref="C7" r:id="rId5" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-squarewave/"/>
+    <hyperlink ref="C8" r:id="rId6" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-trianglewave/"/>
+    <hyperlink ref="C9" r:id="rId7" display="https://www.metrology.net/wiki/testprocess-measure-current-dc/"/>
+    <hyperlink ref="C10" r:id="rId8" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-gas/"/>
+    <hyperlink ref="C11" r:id="rId9" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-liquid/"/>
+    <hyperlink ref="C12" r:id="rId10" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-solid/"/>
+    <hyperlink ref="C13" r:id="rId11" display="https://www.metrology.net/wiki/testprocess-measure-force/"/>
+    <hyperlink ref="C14" r:id="rId12" display="https://www.metrology.net/wiki/testprocess-measure-frequency/"/>
+    <hyperlink ref="C15" r:id="rId13" display="https://www.metrology.net/wiki/testprocess-measure-frequency-amplitudemodulation-rate/"/>
+    <hyperlink ref="C16" r:id="rId14" display="https://www.metrology.net/wiki/testprocess-measure-frequency-frequencymodulation-deviation/"/>
+    <hyperlink ref="C17" r:id="rId15" display="https://www.metrology.net/wiki/testprocess-measure-frequency-frequencymodulation-rate/"/>
+    <hyperlink ref="C18" r:id="rId16" display="https://www.metrology.net/wiki/testprocess-measure-frequency-phasemodulation-rate/"/>
+    <hyperlink ref="C19" r:id="rId17" display="https://www.metrology.net/wiki/testprocess-measure-humidity-absolute/"/>
+    <hyperlink ref="C21" r:id="rId18" display="https://www.metrology.net/wiki/testprocess-measure-impedance/"/>
+    <hyperlink ref="C22" r:id="rId19" display="https://www.metrology.net/wiki/testprocess-measure-inductance/"/>
+    <hyperlink ref="C23" r:id="rId20" display="https://www.metrology.net/wiki/testprocess-measure-length/"/>
+    <hyperlink ref="C24" r:id="rId21" display="https://www.metrology.net/wiki/testprocess-measure-length-circumference/"/>
+    <hyperlink ref="C25" r:id="rId22" display="https://www.metrology.net/wiki/testprocess-measure-length-diameter/"/>
+    <hyperlink ref="C26" r:id="rId23" display="https://www.metrology.net/wiki/testprocess-measure-length-form-flatness/"/>
+    <hyperlink ref="C27" r:id="rId24" display="https://www.metrology.net/wiki/testprocess-measure-length-form-parallelism/"/>
+    <hyperlink ref="C28" r:id="rId25" display="https://www.metrology.net/wiki/testprocess-measure-length-form-perpendicularity/"/>
+    <hyperlink ref="C29" r:id="rId26" display="https://www.metrology.net/wiki/testprocess-measure-length-form-roughness/"/>
+    <hyperlink ref="C30" r:id="rId27" display="https://www.metrology.net/wiki/testprocess-measure-length-form-roundness/"/>
+    <hyperlink ref="C31" r:id="rId28" display="https://www.metrology.net/wiki/testprocess-measure-length-form-sphericity/"/>
+    <hyperlink ref="C32" r:id="rId29" display="https://www.metrology.net/wiki/testprocess-measure-length-form-straightness-axis/"/>
+    <hyperlink ref="C33" r:id="rId30" display="https://www.metrology.net/wiki/testprocess-measure-length-form-straightness-surface/"/>
+    <hyperlink ref="C34" r:id="rId31" display="https://www.metrology.net/wiki/testprocess-measure-length-radius/"/>
+    <hyperlink ref="C35" r:id="rId32" display="https://www.metrology.net/wiki/testprocess-measure-mass-apparent/"/>
+    <hyperlink ref="C36" r:id="rId33" display="https://www.metrology.net/wiki/testprocess-measure-mass-conventional/"/>
+    <hyperlink ref="C37" r:id="rId34" display="https://www.metrology.net/wiki/testprocess-measure-mass-true/"/>
+    <hyperlink ref="C38" r:id="rId35" display="https://www.metrology.net/wiki/testprocess-measure-phase-phasemodulation/"/>
+    <hyperlink ref="C39" r:id="rId36" display="https://www.metrology.net/wiki/testprocess-measure-phase-reflectioncoefficent-rf/"/>
+    <hyperlink ref="C40" r:id="rId37" display="https://www.metrology.net/wiki/testprocess-measure-phase-reflectioncoefficent/"/>
+    <hyperlink ref="C41" r:id="rId38" display="https://www.metrology.net/wiki/testprocess-measure-phasenoise-sideband/"/>
+    <hyperlink ref="C42" r:id="rId39" display="https://www.metrology.net/wiki/testprocess-measure-power-rf-sinewave/"/>
+    <hyperlink ref="C43" r:id="rId40" display="https://www.metrology.net/wiki/testprocess-measure-pressure-hydraulic-static/"/>
+    <hyperlink ref="C44" r:id="rId41" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-absolute-static/"/>
+    <hyperlink ref="C45" r:id="rId42" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-differential-static/"/>
+    <hyperlink ref="C46" r:id="rId43" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-gage-static/"/>
+    <hyperlink ref="C47" r:id="rId44" display="https://www.metrology.net/wiki/testprocess-measure-ratio-amplitudemodulation/"/>
+    <hyperlink ref="C48" r:id="rId45" display="https://www.metrology.net/wiki/testprocess-measure-ratio-density-mass/"/>
+    <hyperlink ref="C49" r:id="rId46" display="https://www.metrology.net/wiki/testprocess-measure-ratio-humidity-relative/"/>
+    <hyperlink ref="C50" r:id="rId47" display="https://www.metrology.net/wiki/testprocess-measure-ratio-humidity-specific/"/>
+    <hyperlink ref="C51" r:id="rId48" display="https://www.metrology.net/wiki/testprocess-measure-ratio-reflectioncoefficent-rf/"/>
+    <hyperlink ref="C52" r:id="rId49" display="https://www.metrology.net/wiki/testprocess-measure-ratio-power-rf-sinewave-delta-frequency/"/>
+    <hyperlink ref="C53" r:id="rId50" display="https://www.metrology.net/wiki/testprocess-measure-ratio-power-rf-sinewave-delta-power/"/>
+    <hyperlink ref="C54" r:id="rId51" display="https://www.metrology.net/wiki/testprocess-measure-ratio-transmissioncoefficent/"/>
+    <hyperlink ref="C55" r:id="rId52" display="https://www.metrology.net/wiki/testprocess-measure-ratio-torque/"/>
+    <hyperlink ref="C56" r:id="rId53" display="https://www.metrology.net/wiki/testprocess-measure-ratio-voltage-ac-ripple-ondc/"/>
+    <hyperlink ref="C57" r:id="rId54" display="https://www.metrology.net/wiki/testprocess-measure-ratio-voltage-ac-sinewave-delta-frequency/"/>
+    <hyperlink ref="C58" r:id="rId55" display="https://www.metrology.net/wiki/testprocess-measure-ratio-volts-ac-sinewave-delta-volts/"/>
+    <hyperlink ref="C59" r:id="rId56" display="https://www.metrology.net/wiki/testprocess-measure-ohms/"/>
+    <hyperlink ref="C60" r:id="rId57" display="https://www.metrology.net/wiki/testprocess-measure-temperature/"/>
+    <hyperlink ref="C61" r:id="rId58" display="https://www.metrology.net/wiki/testprocess-measure-temperature-radiometric/"/>
+    <hyperlink ref="C62" r:id="rId59" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-prt/"/>
+    <hyperlink ref="C63" r:id="rId60" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-rtd/"/>
+    <hyperlink ref="C64" r:id="rId61" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-thermocouple/"/>
+    <hyperlink ref="C65" r:id="rId62" display="https://www.metrology.net/wiki/testprocess-measure-time-pulsetransition/"/>
+    <hyperlink ref="C66" r:id="rId63" display="https://www.metrology.net/wiki/testprocess-measure-time-absolute/"/>
+    <hyperlink ref="C67" r:id="rId64" display="https://www.metrology.net/wiki/testprocess-measure-torque/"/>
+    <hyperlink ref="C68" r:id="rId65" display="https://www.metrology.net/wiki/testprocess-measure-torque-hydraulicpressure/"/>
+    <hyperlink ref="C69" r:id="rId66" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac/"/>
+    <hyperlink ref="C70" r:id="rId67" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-noise-ondc/"/>
+    <hyperlink ref="C71" r:id="rId68" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-sinewave/"/>
+    <hyperlink ref="C72" r:id="rId69" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-squarewave/"/>
+    <hyperlink ref="C73" r:id="rId70" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-trianglewave/"/>
+    <hyperlink ref="C74" r:id="rId71" display="https://www.metrology.net/wiki/testprocess-measure-voltage-dc/"/>
+    <hyperlink ref="C75" r:id="rId72" display="https://www.metrology.net/wiki/testprocess-measure-weight/"/>
+    <hyperlink ref="C76" r:id="rId73" display="https://www.metrology.net/wiki/testprocess-source-capacitance/"/>
+    <hyperlink ref="C77" r:id="rId74" display="https://www.metrology.net/wiki/testprocess-source-conductance/"/>
+    <hyperlink ref="C78" r:id="rId75" display="https://www.metrology.net/wiki/testprocess-source-conductivity/"/>
+    <hyperlink ref="C79" r:id="rId76" display="https://www.metrology.net/wiki/testprocess-source-current-ac-sinewave/"/>
+    <hyperlink ref="C80" r:id="rId77" display="https://www.metrology.net/wiki/testprocess-source-current-ac-squarewave/"/>
+    <hyperlink ref="C81" r:id="rId78" display="https://www.metrology.net/wiki/testprocess-source-current-ac-triangle/"/>
+    <hyperlink ref="C82" r:id="rId79" display="https://www.metrology.net/wiki/testprocess-source-current-dc/"/>
+    <hyperlink ref="C83" r:id="rId80" display="https://www.metrology.net/wiki/testprocess-source-density-mass-gas/"/>
+    <hyperlink ref="C84" r:id="rId81" display="https://www.metrology.net/wiki/testprocess-source-density-mass-liquid/"/>
+    <hyperlink ref="C85" r:id="rId82" display="https://www.metrology.net/wiki/testprocess-source-density-mass-solid/"/>
+    <hyperlink ref="C86" r:id="rId83" display="https://www.metrology.net/wiki/testprocess-source-force/"/>
+    <hyperlink ref="C87" r:id="rId84" display="https://www.metrology.net/wiki/testprocess-source-frequency-ac-squarewave/"/>
+    <hyperlink ref="C88" r:id="rId85" display="https://www.metrology.net/wiki/testprocess-source-frequency-arbitrary-cardiograph/"/>
+    <hyperlink ref="C89" r:id="rId86" display="https://www.metrology.net/wiki/testprocess-source-humidity-absolute/"/>
+    <hyperlink ref="C90" r:id="rId87" display="https://www.metrology.net/wiki/testprocess-source-impedance/"/>
+    <hyperlink ref="C91" r:id="rId88" display="https://www.metrology.net/wiki/testprocess-source-inductance/"/>
+    <hyperlink ref="C92" r:id="rId89" display="https://www.metrology.net/wiki/testprocess-source-length/"/>
+    <hyperlink ref="C93" r:id="rId90" display="https://www.metrology.net/wiki/testprocess-source-length-circumference/"/>
+    <hyperlink ref="C94" r:id="rId91" display="https://www.metrology.net/wiki/testprocess-source-length-diameter/"/>
+    <hyperlink ref="C95" r:id="rId92" display="https://www.metrology.net/wiki/testprocess-source-length-form-perpendicularity/"/>
+    <hyperlink ref="C96" r:id="rId93" display="https://www.metrology.net/wiki/testprocess-source-length-form-roundness/"/>
+    <hyperlink ref="C97" r:id="rId94" display="https://www.metrology.net/wiki/testprocess-source-length-form-sphericity/"/>
+    <hyperlink ref="C98" r:id="rId95" display="https://www.metrology.net/wiki/testprocess-source-length-form-straightness-surrface/"/>
+    <hyperlink ref="C99" r:id="rId96" display="https://www.metrology.net/wiki/testprocess-source-length-radius/"/>
+    <hyperlink ref="C100" r:id="rId97" display="https://www.metrology.net/wiki/testprocess-source-mass-apparent/"/>
+    <hyperlink ref="C101" r:id="rId98" display="https://www.metrology.net/wiki/testprocess-source-mass-conventional/"/>
+    <hyperlink ref="C102" r:id="rId99" display="https://www.metrology.net/wiki/testprocess-source-mass-true/"/>
+    <hyperlink ref="C103" r:id="rId100" display="https://www.metrology.net/wiki/testprocess-source-period-marker/"/>
+    <hyperlink ref="C104" r:id="rId101" display="https://www.metrology.net/wiki/testprocess-source-period-squarewave/"/>
+    <hyperlink ref="C105" r:id="rId102" display="https://www.metrology.net/wiki/testprocess-source-power-ac-sinewave/"/>
+    <hyperlink ref="C106" r:id="rId103" display="https://www.metrology.net/wiki/testprocess-source-power-ac-sinewave-simulated/"/>
+    <hyperlink ref="C107" r:id="rId104" display="https://www.metrology.net/wiki/testprocess-source-power-dc-simulated/"/>
+    <hyperlink ref="C108" r:id="rId105" display="https://www.metrology.net/wiki/testprocess-source-power-noise-terminated/"/>
+    <hyperlink ref="C109" r:id="rId106" display="https://www.metrology.net/wiki/testprocess-source-power-rf-sinewave/"/>
+    <hyperlink ref="C110" r:id="rId107" display="https://www.metrology.net/wiki/testprocess-source-pressure-hydraulic-static/"/>
+    <hyperlink ref="C111" r:id="rId108" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-absolute-static/"/>
+    <hyperlink ref="C112" r:id="rId109" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-differential-static/"/>
+    <hyperlink ref="C113" r:id="rId110" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-gage-static/"/>
+    <hyperlink ref="C114" r:id="rId111" display="https://www.metrology.net/wiki/testprocess-source-ratio-amplitudemodulation/"/>
+    <hyperlink ref="C115" r:id="rId112" display="https://www.metrology.net/wiki/testprocess-source-ratio-humidity-relative/"/>
+    <hyperlink ref="C116" r:id="rId113" display="https://www.metrology.net/wiki/testprocess-source-ratio-humidity-specific/"/>
+    <hyperlink ref="C117" r:id="rId114" display="https://www.metrology.net/wiki/testprocess-source-ratio-rf-sinusoidal-delta-frequency/"/>
+    <hyperlink ref="C118" r:id="rId115" display="https://www.metrology.net/wiki/source-voltage-ac-sinewave-delta-frequency/"/>
+    <hyperlink ref="C119" r:id="rId116" display="https://www.metrology.net/wiki/testprocess-source-voltage-ac-sinewave-delta-voltage/"/>
+    <hyperlink ref="C120" r:id="rId117" display="https://www.metrology.net/wiki/testprocess-source-resistance/"/>
+    <hyperlink ref="C121" r:id="rId118" display="https://www.metrology.net/wiki/testprocess-source-temperature/"/>
+    <hyperlink ref="C122" r:id="rId119" display="https://www.metrology.net/wiki/testprocess-source-temperature-fixedpoint/"/>
+    <hyperlink ref="C123" r:id="rId120" display="https://www.metrology.net/wiki/testprocess-source-temperature-radiometric/"/>
+    <hyperlink ref="C124" r:id="rId121" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-prt/"/>
+    <hyperlink ref="C125" r:id="rId122" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-rtd/"/>
+    <hyperlink ref="C126" r:id="rId123" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-thermocouple/"/>
+    <hyperlink ref="C127" r:id="rId124" display="https://www.metrology.net/wiki/source-time-marker/"/>
+    <hyperlink ref="C128" r:id="rId125" display="https://www.metrology.net/wiki/testprocess-source-torque/"/>
+    <hyperlink ref="C129" r:id="rId126" display="https://www.metrology.net/wiki/source-voltage-ac-sinewave/"/>
+    <hyperlink ref="C130" r:id="rId127" display="https://www.metrology.net/wiki/testprocess-source-voltage-dc/"/>
+    <hyperlink ref="C131" r:id="rId128" display="https://www.metrology.net/wiki/source-voltage-dc-delta/"/>
+    <hyperlink ref="C132" r:id="rId129" display="https://www.metrology.net/wiki/testprocess-source-voltage-noise-terminated/"/>
+    <hyperlink ref="C133" r:id="rId130" display="https://www.metrology.net/wiki/testprocess-source-voltage-shorted/"/>
+    <hyperlink ref="C134" r:id="rId131" display="https://www.metrology.net/wiki/testprocess-source-weight/"/>
+    <hyperlink ref="C20" r:id="rId132" display="https://www.metrology.net/wiki/testprocess-measure-humidity-absolute/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId133"/>
@@ -4595,194 +4663,356 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC584196-9739-4B08-B7A7-EF0413D9DC9F}">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="5" width="25.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="10" max="10" width="27.33203125" customWidth="1"/>
+    <col min="11" max="11" width="21.77734375" customWidth="1"/>
+    <col min="12" max="12" width="31" customWidth="1"/>
+    <col min="13" max="13" width="14.21875" customWidth="1"/>
+    <col min="14" max="14" width="26" customWidth="1"/>
+    <col min="15" max="15" width="19.109375" customWidth="1"/>
+    <col min="16" max="16" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:16">
       <c r="A1" s="3" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>377</v>
+        <v>414</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>99</v>
+        <v>415</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>100</v>
+        <v>368</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="I1" s="43" t="s">
+        <v>506</v>
+      </c>
+      <c r="J1" s="43" t="s">
+        <v>508</v>
+      </c>
+      <c r="K1" s="43" t="s">
+        <v>507</v>
+      </c>
+      <c r="L1" s="43" t="s">
+        <v>509</v>
+      </c>
+      <c r="M1" s="44" t="s">
+        <v>519</v>
+      </c>
+      <c r="N1" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="O1" s="44" t="s">
+        <v>520</v>
+      </c>
+      <c r="P1" s="44" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>463</v>
+      </c>
+      <c r="B2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C2" t="s">
+        <v>491</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>496</v>
+      </c>
+      <c r="F2" t="s">
+        <v>328</v>
+      </c>
+      <c r="G2" t="s">
+        <v>329</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>500</v>
+      </c>
+      <c r="I2" t="s">
+        <v>510</v>
+      </c>
+      <c r="J2" t="s">
+        <v>513</v>
+      </c>
+      <c r="K2" t="s">
+        <v>515</v>
+      </c>
+      <c r="L2" t="s">
+        <v>516</v>
+      </c>
+      <c r="M2" t="s">
+        <v>330</v>
+      </c>
+      <c r="N2" t="s">
+        <v>368</v>
+      </c>
+      <c r="O2" t="s">
+        <v>522</v>
+      </c>
+      <c r="P2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>463</v>
+      </c>
+      <c r="B3" t="s">
+        <v>367</v>
+      </c>
+      <c r="C3" t="s">
+        <v>492</v>
+      </c>
+      <c r="D3" t="s">
+        <v>362</v>
+      </c>
+      <c r="E3" t="s">
+        <v>497</v>
+      </c>
+      <c r="F3" t="s">
+        <v>328</v>
+      </c>
+      <c r="G3" t="s">
+        <v>363</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>501</v>
+      </c>
+      <c r="I3" t="s">
+        <v>511</v>
+      </c>
+      <c r="J3" t="s">
+        <v>513</v>
+      </c>
+      <c r="K3" t="s">
+        <v>515</v>
+      </c>
+      <c r="L3" t="s">
+        <v>516</v>
+      </c>
+      <c r="M3" t="s">
+        <v>364</v>
+      </c>
+      <c r="N3" t="s">
+        <v>368</v>
+      </c>
+      <c r="O3" t="s">
+        <v>522</v>
+      </c>
+      <c r="P3" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>463</v>
+      </c>
+      <c r="B4" t="s">
+        <v>367</v>
+      </c>
+      <c r="C4" t="s">
+        <v>493</v>
+      </c>
+      <c r="D4" t="s">
+        <v>371</v>
+      </c>
+      <c r="E4" t="s">
+        <v>498</v>
+      </c>
+      <c r="F4" t="s">
+        <v>328</v>
+      </c>
+      <c r="G4" t="s">
+        <v>372</v>
+      </c>
+      <c r="H4" t="s">
         <v>373</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I4" t="s">
+        <v>361</v>
+      </c>
+      <c r="J4" t="s">
+        <v>513</v>
+      </c>
+      <c r="K4" t="s">
+        <v>515</v>
+      </c>
+      <c r="L4" t="s">
+        <v>516</v>
+      </c>
+      <c r="M4" t="s">
         <v>374</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>476</v>
-      </c>
-      <c r="B2" t="s">
-        <v>372</v>
-      </c>
-      <c r="C2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D2" t="s">
-        <v>330</v>
-      </c>
-      <c r="E2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" t="s">
-        <v>326</v>
-      </c>
-      <c r="G2" t="s">
-        <v>331</v>
-      </c>
-      <c r="H2" t="s">
-        <v>332</v>
-      </c>
-      <c r="I2">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>476</v>
-      </c>
-      <c r="B3" t="s">
-        <v>372</v>
-      </c>
-      <c r="C3" t="s">
-        <v>365</v>
-      </c>
-      <c r="D3" t="s">
-        <v>366</v>
-      </c>
-      <c r="E3" t="s">
-        <v>367</v>
-      </c>
-      <c r="G3" t="s">
-        <v>331</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="N4" t="s">
         <v>368</v>
       </c>
-      <c r="I3">
-        <v>13</v>
-      </c>
-      <c r="J3" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>476</v>
-      </c>
-      <c r="B4" t="s">
-        <v>372</v>
-      </c>
-      <c r="C4" t="s">
-        <v>378</v>
-      </c>
-      <c r="D4" t="s">
-        <v>380</v>
-      </c>
-      <c r="E4" t="s">
-        <v>379</v>
-      </c>
-      <c r="G4" t="s">
-        <v>331</v>
-      </c>
-      <c r="H4" t="s">
-        <v>381</v>
-      </c>
-      <c r="I4" t="s">
-        <v>382</v>
-      </c>
-      <c r="J4" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="O4" t="s">
+        <v>522</v>
+      </c>
+      <c r="P4" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="B5" t="s">
-        <v>393</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>394</v>
+        <v>494</v>
       </c>
       <c r="D5" t="s">
-        <v>395</v>
+        <v>482</v>
       </c>
       <c r="E5" t="s">
-        <v>495</v>
-      </c>
-      <c r="G5" t="s">
-        <v>496</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>498</v>
+        <v>499</v>
+      </c>
+      <c r="F5" t="s">
+        <v>483</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>484</v>
       </c>
       <c r="I5" t="s">
-        <v>497</v>
+        <v>512</v>
       </c>
       <c r="J5" t="s">
-        <v>504</v>
+        <v>513</v>
+      </c>
+      <c r="K5" t="s">
+        <v>514</v>
+      </c>
+      <c r="L5" t="s">
+        <v>517</v>
+      </c>
+      <c r="M5" t="s">
+        <v>490</v>
+      </c>
+      <c r="N5" t="s">
+        <v>368</v>
+      </c>
+      <c r="O5" t="s">
+        <v>522</v>
+      </c>
+      <c r="P5" t="s">
+        <v>521</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6" xr:uid="{948C0099-BC74-4A90-BEFC-CB4A50D83A3C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6 I6 M6">
       <formula1>EquipmentCategories</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" t="s">
+        <v>502</v>
+      </c>
+      <c r="C2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E2" t="s">
+        <v>368</v>
+      </c>
+      <c r="F2" t="s">
+        <v>503</v>
+      </c>
+      <c r="G2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5" t="s">
+        <v>360</v>
+      </c>
+      <c r="C5" t="s">
+        <v>414</v>
+      </c>
+      <c r="D5" t="s">
+        <v>415</v>
+      </c>
+      <c r="E5" t="s">
+        <v>505</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D49"/>
   <sheetViews>
@@ -4790,23 +5020,23 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4814,10 +5044,10 @@
         <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="D2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4828,7 +5058,7 @@
         <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4836,10 +5066,10 @@
         <v>53</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4850,7 +5080,7 @@
         <v>55</v>
       </c>
       <c r="D5" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4861,7 +5091,7 @@
         <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4872,7 +5102,7 @@
         <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4883,29 +5113,29 @@
         <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D9" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D10" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4916,7 +5146,7 @@
         <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4927,7 +5157,7 @@
         <v>66</v>
       </c>
       <c r="D12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -4938,7 +5168,7 @@
         <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4949,7 +5179,7 @@
         <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4960,7 +5190,7 @@
         <v>72</v>
       </c>
       <c r="D15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -4971,7 +5201,7 @@
         <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -4979,10 +5209,10 @@
         <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -4993,7 +5223,7 @@
         <v>77</v>
       </c>
       <c r="D18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -5004,7 +5234,7 @@
         <v>79</v>
       </c>
       <c r="D19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -5015,7 +5245,7 @@
         <v>81</v>
       </c>
       <c r="D20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -5026,7 +5256,7 @@
         <v>83</v>
       </c>
       <c r="D21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -5037,7 +5267,7 @@
         <v>96</v>
       </c>
       <c r="D22" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -5048,18 +5278,18 @@
         <v>85</v>
       </c>
       <c r="D23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>472</v>
+        <v>459</v>
       </c>
       <c r="D24" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
     </row>
     <row r="25" spans="2:4">
@@ -5070,7 +5300,7 @@
         <v>87</v>
       </c>
       <c r="D25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -5081,7 +5311,7 @@
         <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -5092,7 +5322,7 @@
         <v>90</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="2:4">
@@ -5103,7 +5333,7 @@
         <v>92</v>
       </c>
       <c r="D28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="2:4">
@@ -5114,16 +5344,16 @@
         <v>94</v>
       </c>
       <c r="D29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="B30" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C30" s="27"/>
       <c r="D30" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
     </row>
     <row r="31" spans="2:4">
@@ -5131,12 +5361,12 @@
         <v>97</v>
       </c>
       <c r="C31" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="B32" s="3" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="C32" t="s">
         <v>72</v>
@@ -5144,15 +5374,15 @@
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="3" t="s">
-        <v>433</v>
+        <v>420</v>
       </c>
       <c r="C33" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="34" spans="2:3">
       <c r="B34" s="3" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
       <c r="C34">
         <v>255</v>
@@ -5160,7 +5390,7 @@
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="3" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
       <c r="C35">
         <v>17025</v>
@@ -5168,7 +5398,7 @@
     </row>
     <row r="36" spans="2:3">
       <c r="B36" s="3" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -5200,56 +5430,56 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C18" r:id="rId1" display="www.dfm.dk" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="C12" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="C19" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="C23" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="C18" r:id="rId1" display="www.dfm.dk"/>
+    <hyperlink ref="C12" r:id="rId2"/>
+    <hyperlink ref="C19" r:id="rId3"/>
+    <hyperlink ref="C23" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6EB6A2-D607-49A1-9D65-9E8022B0E74E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="56.28515625" style="33" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="68.140625" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="56.33203125" style="33" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="68.109375" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>97</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="H1" s="3"/>
     </row>
@@ -5257,183 +5487,183 @@
       <c r="B2" s="36"/>
       <c r="G2" s="33"/>
     </row>
-    <row r="3" spans="1:8" ht="30">
+    <row r="3" spans="1:8" ht="28.8">
       <c r="A3" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="B3" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="C3" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="D3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="111.75" customHeight="1">
       <c r="A4" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="C4" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
       <c r="D4" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="E4" s="37" t="s">
+        <v>400</v>
+      </c>
+      <c r="F4" t="s">
+        <v>401</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8">
+      <c r="A5" t="s">
+        <v>463</v>
+      </c>
+      <c r="B5" t="s">
+        <v>378</v>
+      </c>
+      <c r="C5" t="s">
+        <v>411</v>
+      </c>
+      <c r="D5" t="s">
+        <v>412</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>470</v>
+      </c>
+      <c r="F5" t="s">
         <v>413</v>
       </c>
-      <c r="F4" t="s">
-        <v>414</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30">
-      <c r="A5" t="s">
-        <v>476</v>
-      </c>
-      <c r="B5" t="s">
-        <v>387</v>
-      </c>
-      <c r="C5" t="s">
-        <v>424</v>
-      </c>
-      <c r="D5" t="s">
-        <v>425</v>
-      </c>
-      <c r="E5" s="33" t="s">
-        <v>483</v>
-      </c>
-      <c r="F5" t="s">
-        <v>426</v>
-      </c>
       <c r="G5" s="33" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="60">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="57.6">
       <c r="A6" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="C6" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>491</v>
+        <v>478</v>
       </c>
       <c r="F6" t="s">
-        <v>490</v>
+        <v>477</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="45">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="43.2">
       <c r="A7" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="B7" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C7" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
       <c r="D7" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F7" t="s">
-        <v>480</v>
+        <v>467</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>481</v>
+        <v>468</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="C8" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="G8" s="33"/>
     </row>
-    <row r="9" spans="1:8" ht="255">
+    <row r="9" spans="1:8" ht="230.4">
       <c r="A9" s="38" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="B9" s="38" t="s">
+        <v>418</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>425</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>427</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>433</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>428</v>
+      </c>
+      <c r="G9" s="39" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8">
+      <c r="A10" s="38" t="s">
+        <v>463</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>424</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>426</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>429</v>
+      </c>
+      <c r="E10" s="39" t="s">
         <v>431</v>
       </c>
-      <c r="C9" s="38" t="s">
-        <v>438</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>440</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>446</v>
-      </c>
-      <c r="F9" s="38" t="s">
-        <v>441</v>
-      </c>
-      <c r="G9" s="39" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="45">
-      <c r="A10" s="38" t="s">
-        <v>476</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>437</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>439</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>442</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>444</v>
-      </c>
       <c r="F10" s="39" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="G10" s="39" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B10" xr:uid="{0EF2E425-2B27-4C14-9F80-FC65046930C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B10">
       <formula1>statementCategories</formula1>
     </dataValidation>
   </dataValidations>
@@ -5446,77 +5676,77 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{164255F3-93CF-4992-BB4A-5F2B2030CF33}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="55.28515625" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="55.33203125" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="B1" t="s">
         <v>97</v>
       </c>
       <c r="C1" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="D1" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="E1" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="F1" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="G1" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
       <c r="H1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="I1" t="s">
         <v>31</v>
       </c>
       <c r="J1" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="B2" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C2" t="s">
-        <v>499</v>
+        <v>485</v>
       </c>
       <c r="D2" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
       <c r="E2" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="F2" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="G2" t="s">
-        <v>503</v>
+        <v>489</v>
       </c>
       <c r="H2">
         <v>-0.5</v>
@@ -5529,51 +5759,51 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D53FE5-FD05-490B-BD2B-60774A285524}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="3" width="24.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="72.5703125" customWidth="1"/>
-    <col min="7" max="7" width="25.85546875" customWidth="1"/>
+    <col min="1" max="3" width="24.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="72.5546875" customWidth="1"/>
+    <col min="7" max="7" width="25.88671875" customWidth="1"/>
     <col min="8" max="8" width="75" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="26.85546875" customWidth="1"/>
+    <col min="10" max="10" width="26.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>433</v>
+        <v>420</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="B2" t="str">
         <f>AdministrativeData!C31</f>
@@ -5607,7 +5837,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:S26"/>
   <sheetViews>
@@ -5615,22 +5845,22 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -5638,7 +5868,7 @@
         <v>29</v>
       </c>
       <c r="G1" s="42" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="H1" s="42"/>
       <c r="I1" s="42"/>
@@ -5647,26 +5877,26 @@
     </row>
     <row r="2" spans="1:19" ht="17.25" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>470</v>
+        <v>457</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="26" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="26" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>469</v>
+        <v>456</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -5694,12 +5924,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="23.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>21</v>
@@ -5726,39 +5956,39 @@
         <v>18</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="P9" s="12" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="R9" s="12" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="23.25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="21.6">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>23</v>
@@ -5782,10 +6012,10 @@
         <v>39</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="L10" s="12" t="s">
         <v>24</v>
@@ -5812,181 +6042,181 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="45.75">
+    <row r="11" spans="1:19" ht="42">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="P11" s="11" t="s">
         <v>453</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>462</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>462</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>462</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>462</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>462</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>462</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>462</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>462</v>
-      </c>
-      <c r="K11" s="11" t="s">
+      <c r="Q11" s="11" t="s">
         <v>453</v>
       </c>
-      <c r="L11" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="M11" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="N11" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="O11" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="P11" s="11" t="s">
-        <v>466</v>
-      </c>
-      <c r="Q11" s="11" t="s">
-        <v>466</v>
-      </c>
       <c r="R11" s="11" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="S11" s="11" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="23.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="21.6">
       <c r="A12" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
       <c r="M12" s="15" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="Q12" s="14" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="R12" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="S12" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="35" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="I13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="L13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="M13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="N13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="O13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="P13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="Q13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="R13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="S13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -5994,7 +6224,7 @@
         <v>30</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
@@ -6019,7 +6249,7 @@
         <v>32</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
       <c r="C15" s="17">
         <v>1000</v>
@@ -6046,7 +6276,7 @@
         <v>33</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="C16" s="17">
         <v>5000</v>
@@ -6073,7 +6303,7 @@
         <v>34</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="C17" s="17">
         <v>10000</v>
@@ -6133,16 +6363,16 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:S11" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:S11">
       <formula1>MeasurandType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:S9" xr:uid="{00000000-0002-0000-0500-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:S9">
       <formula1>ColType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:S10" xr:uid="{00000000-0002-0000-0500-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:S10">
       <formula1>MetaType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:S13" xr:uid="{FB1CB67C-7785-4D42-8012-3FA40F22C35C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:S13">
       <formula1>metaDataType</formula1>
     </dataValidation>
   </dataValidations>
@@ -6152,28 +6382,28 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A4AA81-4554-458B-9882-6962A642879C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="12" width="14.5703125" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" customWidth="1"/>
+    <col min="10" max="12" width="14.5546875" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" customWidth="1"/>
+    <col min="14" max="14" width="16.88671875" customWidth="1"/>
+    <col min="17" max="17" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -6181,7 +6411,7 @@
         <v>29</v>
       </c>
       <c r="G1" s="42" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="H1" s="42"/>
       <c r="I1" s="42"/>
@@ -6191,26 +6421,26 @@
     </row>
     <row r="2" spans="1:17" ht="17.25" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="26" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>351</v>
+        <v>495</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="26" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -6243,7 +6473,7 @@
         <v>44</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>20</v>
@@ -6279,24 +6509,24 @@
         <v>21</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="P9" s="11" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="23.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="21.6">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>23</v>
@@ -6323,7 +6553,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="L10" s="11" t="s">
         <v>4</v>
@@ -6332,7 +6562,7 @@
         <v>5</v>
       </c>
       <c r="N10" s="11" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="O10" s="11" t="s">
         <v>39</v>
@@ -6344,65 +6574,65 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="23.25">
+    <row r="11" spans="1:17" ht="21.6">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M11" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="O11" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="N11" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="O11" s="11" t="s">
-        <v>190</v>
-      </c>
       <c r="P11" s="11" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="23.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>27</v>
@@ -6432,83 +6662,83 @@
         <v>27</v>
       </c>
       <c r="L12" s="14" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="M12" s="15" t="s">
         <v>28</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="Q12" s="14" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="23.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="35" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="I13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="L13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="M13" s="34" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="N13" s="34" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
       <c r="O13" s="34" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="P13" s="34" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="Q13" s="34" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="34.5">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="31.8">
       <c r="A14" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>17</v>
@@ -6532,10 +6762,10 @@
         <v>42</v>
       </c>
       <c r="J14" s="22" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
       <c r="K14" s="22" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
       <c r="L14" s="22" t="s">
         <v>4</v>
@@ -6544,16 +6774,16 @@
         <v>47</v>
       </c>
       <c r="N14" s="22" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
       <c r="O14" s="22" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="P14" s="22" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="Q14" s="22" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -6599,16 +6829,16 @@
         <v>1</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
       <c r="P15" s="9" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>394</v>
+        <v>494</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -6654,16 +6884,16 @@
         <v>2</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="P16" s="9" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="Q16" s="9" t="s">
-        <v>394</v>
+        <v>494</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -6709,16 +6939,16 @@
         <v>3</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="P17" s="9" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>394</v>
+        <v>494</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -6764,16 +6994,16 @@
         <v>4</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
       <c r="P18" s="9" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>394</v>
+        <v>494</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -6819,16 +7049,16 @@
         <v>5</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>394</v>
+        <v>494</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -6868,17 +7098,18 @@
   <mergeCells count="1">
     <mergeCell ref="G1:K1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:Q13" xr:uid="{D96066D6-C857-4588-9E3A-454C48CCC700}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:Q13">
       <formula1>metaDataType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:Q10" xr:uid="{987BDDAD-B799-4310-BFFA-0DF53682893C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:Q10">
       <formula1>MetaType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:Q9" xr:uid="{C503BAA3-1675-4542-B242-F824FDB8945B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:Q9">
       <formula1>ColType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:Q11" xr:uid="{53630EEB-53E9-40E4-923B-B05023339B5D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:Q11">
       <formula1>MeasurandType</formula1>
     </dataValidation>
   </dataValidations>
@@ -6888,7 +7119,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -6896,42 +7127,42 @@
       <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>99</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="I1" s="3"/>
     </row>
@@ -6944,83 +7175,83 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6D6EC4-A3DC-42B4-ABAF-F3EE7418B168}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="6" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" customWidth="1"/>
+    <col min="2" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="6" max="7" width="21.6640625" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" customWidth="1"/>
+    <col min="13" max="13" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="3" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>400</v>
+        <v>387</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" ht="43.2">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
         <v>402</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>404</v>
-      </c>
-      <c r="N1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" ht="45">
-      <c r="A2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" t="s">
-        <v>415</v>
-      </c>
       <c r="C2" s="33" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="E2" t="s">
         <v>92</v>
       </c>
       <c r="F2" t="s">
-        <v>421</v>
+        <v>408</v>
       </c>
       <c r="H2" t="s">
         <v>87</v>
@@ -7034,16 +7265,16 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="C3" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
       <c r="E3" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="F3">
         <v>5</v>
@@ -7060,18 +7291,18 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>418</v>
+        <v>405</v>
       </c>
       <c r="M5">
         <v>1</v>

</xml_diff>

<commit_message>
Add multilingual headings in columns
</commit_message>
<xml_diff>
--- a/Examples/DCC_temperature.xlsx
+++ b/Examples/DCC_temperature.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21396" activeTab="9"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21396" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -18,10 +18,10 @@
     <sheet name="Settings" sheetId="9" r:id="rId4"/>
     <sheet name="Accreditation" sheetId="11" r:id="rId5"/>
     <sheet name="Table2" sheetId="5" state="hidden" r:id="rId6"/>
-    <sheet name="Table_TempCal" sheetId="14" r:id="rId7"/>
-    <sheet name="Software" sheetId="8" state="hidden" r:id="rId8"/>
-    <sheet name="Locations" sheetId="13" state="hidden" r:id="rId9"/>
-    <sheet name="Equipment" sheetId="12" r:id="rId10"/>
+    <sheet name="Equipment" sheetId="12" r:id="rId7"/>
+    <sheet name="Table_TempCal" sheetId="14" r:id="rId8"/>
+    <sheet name="Software" sheetId="8" state="hidden" r:id="rId9"/>
+    <sheet name="Locations" sheetId="13" state="hidden" r:id="rId10"/>
     <sheet name="Sheet1" sheetId="15" r:id="rId11"/>
   </sheets>
   <externalReferences>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="536">
   <si>
     <t>customerTag</t>
   </si>
@@ -214,144 +214,69 @@
     <t>dataCategoryType</t>
   </si>
   <si>
-    <t>DFM_Software_Name</t>
-  </si>
-  <si>
-    <t>DFM_Software_Version</t>
-  </si>
-  <si>
     <t>v0.0.1</t>
   </si>
   <si>
-    <t>DFM_Unique_ID</t>
-  </si>
-  <si>
-    <t>DFM_OrderNo</t>
-  </si>
-  <si>
     <t>8000650430</t>
   </si>
   <si>
-    <t>DFM_ArrivalDate</t>
-  </si>
-  <si>
     <t>2022-02-18</t>
   </si>
   <si>
-    <t>DFM_StartDate</t>
-  </si>
-  <si>
     <t>2022-02-21</t>
   </si>
   <si>
-    <t>DFM_EndDate</t>
-  </si>
-  <si>
     <t>2022-02-22</t>
   </si>
   <si>
     <t>Temperature sensor</t>
   </si>
   <si>
-    <t>DFM_CalLab_CompanyName</t>
-  </si>
-  <si>
     <t>DFM A/S</t>
   </si>
   <si>
-    <t>DFM_CalLab_Email</t>
-  </si>
-  <si>
     <t>Administration@dfm.dk</t>
   </si>
   <si>
-    <t>DFM_CalLab_Phone</t>
-  </si>
-  <si>
     <t>+45 7730 5800</t>
   </si>
   <si>
-    <t>DFM_CalLab_City</t>
-  </si>
-  <si>
     <t>Hørsholm</t>
   </si>
   <si>
-    <t>DFM_CalLab_Country</t>
-  </si>
-  <si>
     <t>DK</t>
   </si>
   <si>
-    <t>DFM_CalLab_PostalCode</t>
-  </si>
-  <si>
     <t>2970</t>
   </si>
   <si>
-    <t>DFM_CalLab_Street1</t>
-  </si>
-  <si>
-    <t>DFM_CalLab_Street_No</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
-    <t>DFM_CalLab_Webpage</t>
-  </si>
-  <si>
     <t>www.dfm.dk</t>
   </si>
   <si>
-    <t>DFM_SignedBy</t>
-  </si>
-  <si>
     <t>J. S. Nielsen</t>
   </si>
   <si>
-    <t>DFM_Customer_CompanyName</t>
-  </si>
-  <si>
     <t>Danish Measurement Company Ltd.</t>
   </si>
   <si>
-    <t>DFM_Customer_Email</t>
-  </si>
-  <si>
     <t>mm@dmc.dk</t>
   </si>
   <si>
-    <t>DFM_Customer_City</t>
-  </si>
-  <si>
     <t>Måløv</t>
   </si>
   <si>
-    <t>DFM_Customer_Country</t>
-  </si>
-  <si>
-    <t>DFM_Customer_PostalCode</t>
-  </si>
-  <si>
     <t>9899</t>
   </si>
   <si>
-    <t>DFM_Customer_CompanyStreet1</t>
-  </si>
-  <si>
     <t>Målervej</t>
   </si>
   <si>
-    <t>DFM_Customer_CompanyStreet_No</t>
-  </si>
-  <si>
     <t>16, 1. sal</t>
   </si>
   <si>
-    <t>DFM_Customer_Att</t>
-  </si>
-  <si>
     <t>Mads Målermand</t>
   </si>
   <si>
@@ -1073,12 +998,6 @@
   </si>
   <si>
     <t>Kogle Alle</t>
-  </si>
-  <si>
-    <t>DFM_Customer_Webpage</t>
-  </si>
-  <si>
-    <t>DFM_Customer_Phone</t>
   </si>
   <si>
     <t xml:space="preserve"> /dcc:digitalCalibrationCertificate/dcc:administrativeData/dcc:customer/dcc:attPerson</t>
@@ -1575,18 +1494,6 @@
     <t>13</t>
   </si>
   <si>
-    <t>item01</t>
-  </si>
-  <si>
-    <t>product name</t>
-  </si>
-  <si>
-    <t>prodcut number</t>
-  </si>
-  <si>
-    <t>issuer</t>
-  </si>
-  <si>
     <t>id1</t>
   </si>
   <si>
@@ -1639,6 +1546,135 @@
   </si>
   <si>
     <t>id2 heading lang2</t>
+  </si>
+  <si>
+    <t>humanHeading lang1</t>
+  </si>
+  <si>
+    <t>humanHeading lang2</t>
+  </si>
+  <si>
+    <t>Kalibreringspunkt</t>
+  </si>
+  <si>
+    <t>Referencetemperatur</t>
+  </si>
+  <si>
+    <t>Referencetemperatur i instrumentenheder</t>
+  </si>
+  <si>
+    <t>Instrumentvisning</t>
+  </si>
+  <si>
+    <t>Visningsfejl</t>
+  </si>
+  <si>
+    <t>Ekspanderet kalibreringsusikkerhed</t>
+  </si>
+  <si>
+    <t>Øvre tolerancegrænse</t>
+  </si>
+  <si>
+    <t>Nedre tolerancegrænse for visningsfejl</t>
+  </si>
+  <si>
+    <t>Recistans</t>
+  </si>
+  <si>
+    <t>Undtagelse fra akkreditering</t>
+  </si>
+  <si>
+    <t>Undtagelsesbemærkning</t>
+  </si>
+  <si>
+    <t>Basis for konformitetsudsagn</t>
+  </si>
+  <si>
+    <t>Anvendt reference</t>
+  </si>
+  <si>
+    <t>Kundens kode</t>
+  </si>
+  <si>
+    <t>CalLab_CompanyName</t>
+  </si>
+  <si>
+    <t>CalLab_Email</t>
+  </si>
+  <si>
+    <t>CalLab_Phone</t>
+  </si>
+  <si>
+    <t>CalLab_City</t>
+  </si>
+  <si>
+    <t>CalLab_Country</t>
+  </si>
+  <si>
+    <t>CalLab_PostalCode</t>
+  </si>
+  <si>
+    <t>CalLab_Street1</t>
+  </si>
+  <si>
+    <t>CalLab_Street_No</t>
+  </si>
+  <si>
+    <t>CalLab_Webpage</t>
+  </si>
+  <si>
+    <t>SignedBy</t>
+  </si>
+  <si>
+    <t>Customer_CompanyName</t>
+  </si>
+  <si>
+    <t>Customer_Att</t>
+  </si>
+  <si>
+    <t>Customer_Email</t>
+  </si>
+  <si>
+    <t>Customer_Phone</t>
+  </si>
+  <si>
+    <t>Customer_City</t>
+  </si>
+  <si>
+    <t>Customer_Country</t>
+  </si>
+  <si>
+    <t>Customer_PostalCode</t>
+  </si>
+  <si>
+    <t>Customer_CompanyStreet1</t>
+  </si>
+  <si>
+    <t>Customer_CompanyStreet_No</t>
+  </si>
+  <si>
+    <t>Customer_Webpage</t>
+  </si>
+  <si>
+    <t>Software_Name</t>
+  </si>
+  <si>
+    <t>Software_Version</t>
+  </si>
+  <si>
+    <t>Unique_ID</t>
+  </si>
+  <si>
+    <t>OrderNo</t>
+  </si>
+  <si>
+    <t>ArrivalDate</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
   </si>
 </sst>
 </file>
@@ -1717,7 +1753,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1781,6 +1817,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1869,7 +1911,7 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -1981,8 +2023,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
@@ -3093,45 +3137,6 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:H6" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:H6"/>
-  <tableColumns count="8">
-    <tableColumn id="1" name="swID"/>
-    <tableColumn id="2" name="name"/>
-    <tableColumn id="3" name="release "/>
-    <tableColumn id="4" name="type"/>
-    <tableColumn id="5" name="description"/>
-    <tableColumn id="6" name="content"/>
-    <tableColumn id="7" name="file"/>
-    <tableColumn id="8" name="formula"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table167" displayName="Table167" ref="A1:M6" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:M6"/>
-  <tableColumns count="13">
-    <tableColumn id="11" name="Category"/>
-    <tableColumn id="1" name="id"/>
-    <tableColumn id="10" name="Name1"/>
-    <tableColumn id="13" name="Name2"/>
-    <tableColumn id="2" name="Street1"/>
-    <tableColumn id="3" name="StreetNo"/>
-    <tableColumn id="14" name="Column1"/>
-    <tableColumn id="4" name="City"/>
-    <tableColumn id="5" name="PostCode"/>
-    <tableColumn id="6" name="PO-BOX"/>
-    <tableColumn id="7" name="CountryCode"/>
-    <tableColumn id="8" name="further"/>
-    <tableColumn id="9" name="p"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="B1:P6" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="B1:P6"/>
   <tableColumns count="15">
@@ -3150,6 +3155,45 @@
     <tableColumn id="16" name="id2 issuer"/>
     <tableColumn id="17" name="id2 heading lang1"/>
     <tableColumn id="18" name="id2 heading lang2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:H6" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:H6"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="swID"/>
+    <tableColumn id="2" name="name"/>
+    <tableColumn id="3" name="release "/>
+    <tableColumn id="4" name="type"/>
+    <tableColumn id="5" name="description"/>
+    <tableColumn id="6" name="content"/>
+    <tableColumn id="7" name="file"/>
+    <tableColumn id="8" name="formula"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table167" displayName="Table167" ref="A1:M6" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:M6"/>
+  <tableColumns count="13">
+    <tableColumn id="11" name="Category"/>
+    <tableColumn id="1" name="id"/>
+    <tableColumn id="10" name="Name1"/>
+    <tableColumn id="13" name="Name2"/>
+    <tableColumn id="2" name="Street1"/>
+    <tableColumn id="3" name="StreetNo"/>
+    <tableColumn id="14" name="Column1"/>
+    <tableColumn id="4" name="City"/>
+    <tableColumn id="5" name="PostCode"/>
+    <tableColumn id="6" name="PO-BOX"/>
+    <tableColumn id="7" name="CountryCode"/>
+    <tableColumn id="8" name="further"/>
+    <tableColumn id="9" name="p"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3485,39 +3529,39 @@
         <v>31</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>376</v>
+        <v>349</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>382</v>
+        <v>355</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>392</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="B2" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="D2" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="F2" t="s">
-        <v>377</v>
+        <v>350</v>
       </c>
       <c r="G2" t="s">
+        <v>340</v>
+      </c>
+      <c r="I2" t="s">
         <v>367</v>
-      </c>
-      <c r="I2" t="s">
-        <v>394</v>
       </c>
       <c r="L2" s="2"/>
     </row>
@@ -3529,19 +3573,19 @@
         <v>24</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="G3" t="s">
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>436</v>
+        <v>409</v>
       </c>
       <c r="L3" s="2"/>
     </row>
@@ -3553,16 +3597,16 @@
         <v>23</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
       <c r="D4" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
       <c r="F4" t="s">
-        <v>378</v>
+        <v>351</v>
       </c>
       <c r="I4" t="s">
-        <v>437</v>
+        <v>410</v>
       </c>
       <c r="L4" s="2"/>
     </row>
@@ -3571,37 +3615,37 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>474</v>
+        <v>447</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="D5" t="s">
-        <v>265</v>
+        <v>240</v>
       </c>
       <c r="F5" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="I5" t="s">
-        <v>438</v>
+        <v>411</v>
       </c>
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>452</v>
+        <v>425</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="D6" t="s">
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="F6" t="s">
-        <v>379</v>
+        <v>352</v>
       </c>
       <c r="I6" t="s">
         <v>0</v>
@@ -3611,16 +3655,16 @@
     <row r="7" spans="1:12">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>473</v>
+        <v>446</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>137</v>
+        <v>112</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>380</v>
+        <v>353</v>
       </c>
       <c r="I7" t="s">
         <v>19</v>
@@ -3632,16 +3676,16 @@
         <v>3</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="D8" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="F8" t="s">
-        <v>381</v>
+        <v>354</v>
       </c>
       <c r="I8" t="s">
-        <v>424</v>
+        <v>397</v>
       </c>
       <c r="L8" s="2"/>
     </row>
@@ -3650,16 +3694,16 @@
         <v>4</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="D9" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
       <c r="F9" t="s">
-        <v>418</v>
+        <v>391</v>
       </c>
       <c r="I9" t="s">
-        <v>393</v>
+        <v>366</v>
       </c>
       <c r="L9" s="2"/>
     </row>
@@ -3668,16 +3712,16 @@
         <v>5</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="D10" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
       <c r="F10" t="s">
-        <v>424</v>
+        <v>397</v>
       </c>
       <c r="I10" t="s">
-        <v>351</v>
+        <v>324</v>
       </c>
       <c r="L10" s="2"/>
     </row>
@@ -3686,13 +3730,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="D11" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
       <c r="I11" t="s">
-        <v>396</v>
+        <v>369</v>
       </c>
       <c r="L11" s="2"/>
     </row>
@@ -3701,10 +3745,10 @@
         <v>22</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="D12" t="s">
-        <v>271</v>
+        <v>246</v>
       </c>
       <c r="L12" s="2"/>
     </row>
@@ -3713,10 +3757,10 @@
         <v>39</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="D13" t="s">
-        <v>272</v>
+        <v>247</v>
       </c>
       <c r="L13" s="2"/>
     </row>
@@ -3725,10 +3769,10 @@
         <v>40</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="D14" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
       <c r="L14" s="2"/>
     </row>
@@ -3737,113 +3781,113 @@
         <v>43</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="D15" t="s">
-        <v>274</v>
+        <v>249</v>
       </c>
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12">
       <c r="C16" s="30" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="D16" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="3:4">
       <c r="C17" s="30" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="D17" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="3:4">
       <c r="C18" s="30" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="D18" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="3:4">
       <c r="C19" s="30" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="D19" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
     </row>
     <row r="20" spans="3:4">
       <c r="C20" s="30" t="s">
-        <v>453</v>
+        <v>426</v>
       </c>
       <c r="D20" t="s">
-        <v>279</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" spans="3:4">
       <c r="C21" s="30" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="D21" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
     </row>
     <row r="22" spans="3:4">
       <c r="C22" s="30" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="D22" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="3:4">
       <c r="C23" s="30" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="D23" t="s">
-        <v>282</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="3:4">
       <c r="C24" s="30" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="D24" t="s">
-        <v>283</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" spans="3:4">
       <c r="C25" s="30" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="D25" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
     </row>
     <row r="26" spans="3:4">
       <c r="C26" s="30" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="D26" t="s">
-        <v>285</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="3:4">
       <c r="C27" s="30" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="D27" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
     </row>
     <row r="28" spans="3:4">
       <c r="C28" s="30" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="D28" t="s">
         <v>28</v>
@@ -3851,39 +3895,39 @@
     </row>
     <row r="29" spans="3:4">
       <c r="C29" s="30" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="D29" t="s">
-        <v>287</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="3:4">
       <c r="C30" s="30" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="D30" t="s">
-        <v>288</v>
+        <v>263</v>
       </c>
     </row>
     <row r="31" spans="3:4">
       <c r="C31" s="30" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="D31" t="s">
-        <v>289</v>
+        <v>264</v>
       </c>
     </row>
     <row r="32" spans="3:4">
       <c r="C32" s="30" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="D32" t="s">
-        <v>290</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33" spans="3:4">
       <c r="C33" s="30" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="D33" t="s">
         <v>27</v>
@@ -3891,634 +3935,634 @@
     </row>
     <row r="34" spans="3:4">
       <c r="C34" s="30" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="D34" t="s">
-        <v>291</v>
+        <v>266</v>
       </c>
     </row>
     <row r="35" spans="3:4">
       <c r="C35" s="30" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
       <c r="D35" t="s">
-        <v>292</v>
+        <v>267</v>
       </c>
     </row>
     <row r="36" spans="3:4">
       <c r="C36" s="30" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="D36" t="s">
-        <v>293</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" spans="3:4">
       <c r="C37" s="30" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="D37" t="s">
-        <v>294</v>
+        <v>269</v>
       </c>
     </row>
     <row r="38" spans="3:4">
       <c r="C38" s="30" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="D38" t="s">
-        <v>295</v>
+        <v>270</v>
       </c>
     </row>
     <row r="39" spans="3:4">
       <c r="C39" s="30" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="D39" t="s">
-        <v>296</v>
+        <v>271</v>
       </c>
     </row>
     <row r="40" spans="3:4">
       <c r="C40" s="30" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="D40" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41" spans="3:4">
       <c r="C41" s="30" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="D41" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
     </row>
     <row r="42" spans="3:4">
       <c r="C42" s="30" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="D42" t="s">
-        <v>299</v>
+        <v>274</v>
       </c>
     </row>
     <row r="43" spans="3:4">
       <c r="C43" s="30" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="D43" t="s">
-        <v>300</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44" spans="3:4">
       <c r="C44" s="30" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="D44" t="s">
-        <v>301</v>
+        <v>276</v>
       </c>
     </row>
     <row r="45" spans="3:4">
       <c r="C45" s="30" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="D45" t="s">
-        <v>302</v>
+        <v>277</v>
       </c>
     </row>
     <row r="46" spans="3:4">
       <c r="C46" s="30" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="D46" t="s">
-        <v>303</v>
+        <v>278</v>
       </c>
     </row>
     <row r="47" spans="3:4">
       <c r="C47" s="30" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="D47" t="s">
-        <v>304</v>
+        <v>279</v>
       </c>
     </row>
     <row r="48" spans="3:4">
       <c r="C48" s="30" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="D48" t="s">
-        <v>305</v>
+        <v>280</v>
       </c>
     </row>
     <row r="49" spans="3:4">
       <c r="C49" s="30" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="D49" t="s">
-        <v>306</v>
+        <v>281</v>
       </c>
     </row>
     <row r="50" spans="3:4">
       <c r="C50" s="30" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="D50" t="s">
-        <v>307</v>
+        <v>282</v>
       </c>
     </row>
     <row r="51" spans="3:4">
       <c r="C51" s="30" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="D51" t="s">
-        <v>308</v>
+        <v>283</v>
       </c>
     </row>
     <row r="52" spans="3:4">
       <c r="C52" s="30" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="D52" t="s">
-        <v>309</v>
+        <v>284</v>
       </c>
     </row>
     <row r="53" spans="3:4">
       <c r="C53" s="30" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="D53" t="s">
-        <v>310</v>
+        <v>285</v>
       </c>
     </row>
     <row r="54" spans="3:4">
       <c r="C54" s="30" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="D54" t="s">
-        <v>311</v>
+        <v>286</v>
       </c>
     </row>
     <row r="55" spans="3:4">
       <c r="C55" s="30" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="D55" t="s">
-        <v>312</v>
+        <v>287</v>
       </c>
     </row>
     <row r="56" spans="3:4">
       <c r="C56" s="30" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="D56" t="s">
-        <v>313</v>
+        <v>288</v>
       </c>
     </row>
     <row r="57" spans="3:4">
       <c r="C57" s="30" t="s">
-        <v>186</v>
+        <v>161</v>
       </c>
       <c r="D57" t="s">
-        <v>314</v>
+        <v>289</v>
       </c>
     </row>
     <row r="58" spans="3:4">
       <c r="C58" s="30" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="D58" t="s">
-        <v>315</v>
+        <v>290</v>
       </c>
     </row>
     <row r="59" spans="3:4">
       <c r="C59" s="30" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="D59" t="s">
-        <v>316</v>
+        <v>291</v>
       </c>
     </row>
     <row r="60" spans="3:4">
       <c r="C60" s="30" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="D60" t="s">
-        <v>317</v>
+        <v>292</v>
       </c>
     </row>
     <row r="61" spans="3:4">
       <c r="C61" s="30" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="D61" t="s">
-        <v>318</v>
+        <v>293</v>
       </c>
     </row>
     <row r="62" spans="3:4">
       <c r="C62" s="30" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="D62" t="s">
-        <v>319</v>
+        <v>294</v>
       </c>
     </row>
     <row r="63" spans="3:4">
       <c r="C63" s="30" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="D63" t="s">
-        <v>320</v>
+        <v>295</v>
       </c>
     </row>
     <row r="64" spans="3:4">
       <c r="C64" s="30" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="D64" t="s">
-        <v>321</v>
+        <v>296</v>
       </c>
     </row>
     <row r="65" spans="3:4">
       <c r="C65" s="30" t="s">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="D65" t="s">
-        <v>322</v>
+        <v>297</v>
       </c>
     </row>
     <row r="66" spans="3:4">
       <c r="C66" s="30" t="s">
-        <v>195</v>
+        <v>170</v>
       </c>
       <c r="D66" t="s">
-        <v>323</v>
+        <v>298</v>
       </c>
     </row>
     <row r="67" spans="3:4">
       <c r="C67" s="30" t="s">
-        <v>196</v>
+        <v>171</v>
       </c>
       <c r="D67" t="s">
-        <v>324</v>
+        <v>299</v>
       </c>
     </row>
     <row r="68" spans="3:4">
       <c r="C68" s="30" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
     </row>
     <row r="69" spans="3:4">
       <c r="C69" s="30" t="s">
-        <v>198</v>
+        <v>173</v>
       </c>
     </row>
     <row r="70" spans="3:4">
       <c r="C70" s="30" t="s">
-        <v>199</v>
+        <v>174</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="30" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
     </row>
     <row r="72" spans="3:4">
       <c r="C72" s="30" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="30" t="s">
-        <v>202</v>
+        <v>177</v>
       </c>
     </row>
     <row r="74" spans="3:4">
       <c r="C74" s="30" t="s">
-        <v>203</v>
+        <v>178</v>
       </c>
     </row>
     <row r="75" spans="3:4">
       <c r="C75" s="30" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
     </row>
     <row r="76" spans="3:4">
       <c r="C76" s="30" t="s">
-        <v>205</v>
+        <v>180</v>
       </c>
     </row>
     <row r="77" spans="3:4">
       <c r="C77" s="30" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="30" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="30" t="s">
-        <v>208</v>
+        <v>183</v>
       </c>
     </row>
     <row r="80" spans="3:4">
       <c r="C80" s="30" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81" s="30" t="s">
-        <v>210</v>
+        <v>185</v>
       </c>
     </row>
     <row r="82" spans="3:3">
       <c r="C82" s="30" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83" s="30" t="s">
-        <v>212</v>
+        <v>187</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84" s="30" t="s">
-        <v>213</v>
+        <v>188</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85" s="30" t="s">
-        <v>214</v>
+        <v>189</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86" s="30" t="s">
-        <v>215</v>
+        <v>190</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87" s="30" t="s">
-        <v>216</v>
+        <v>191</v>
       </c>
     </row>
     <row r="88" spans="3:3">
       <c r="C88" s="30" t="s">
-        <v>217</v>
+        <v>192</v>
       </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89" s="30" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
     </row>
     <row r="90" spans="3:3">
       <c r="C90" s="30" t="s">
-        <v>219</v>
+        <v>194</v>
       </c>
     </row>
     <row r="91" spans="3:3">
       <c r="C91" s="30" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92" s="30" t="s">
-        <v>221</v>
+        <v>196</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93" s="30" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
     </row>
     <row r="94" spans="3:3">
       <c r="C94" s="30" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
     </row>
     <row r="95" spans="3:3">
       <c r="C95" s="30" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
     </row>
     <row r="96" spans="3:3">
       <c r="C96" s="30" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
     </row>
     <row r="97" spans="3:3">
       <c r="C97" s="30" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
     </row>
     <row r="98" spans="3:3">
       <c r="C98" s="30" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
     </row>
     <row r="99" spans="3:3">
       <c r="C99" s="30" t="s">
-        <v>228</v>
+        <v>203</v>
       </c>
     </row>
     <row r="100" spans="3:3">
       <c r="C100" s="30" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
     </row>
     <row r="101" spans="3:3">
       <c r="C101" s="30" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
     </row>
     <row r="102" spans="3:3">
       <c r="C102" s="30" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
     </row>
     <row r="103" spans="3:3">
       <c r="C103" s="30" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
     </row>
     <row r="104" spans="3:3">
       <c r="C104" s="30" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
     </row>
     <row r="105" spans="3:3">
       <c r="C105" s="30" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
     </row>
     <row r="106" spans="3:3">
       <c r="C106" s="30" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
     </row>
     <row r="107" spans="3:3">
       <c r="C107" s="30" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
     </row>
     <row r="108" spans="3:3">
       <c r="C108" s="30" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
     </row>
     <row r="109" spans="3:3">
       <c r="C109" s="30" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
     </row>
     <row r="110" spans="3:3">
       <c r="C110" s="30" t="s">
-        <v>239</v>
+        <v>214</v>
       </c>
     </row>
     <row r="111" spans="3:3">
       <c r="C111" s="30" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
     </row>
     <row r="112" spans="3:3">
       <c r="C112" s="30" t="s">
-        <v>241</v>
+        <v>216</v>
       </c>
     </row>
     <row r="113" spans="3:3">
       <c r="C113" s="30" t="s">
-        <v>242</v>
+        <v>217</v>
       </c>
     </row>
     <row r="114" spans="3:3">
       <c r="C114" s="30" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
     </row>
     <row r="115" spans="3:3">
       <c r="C115" s="30" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
     </row>
     <row r="116" spans="3:3">
       <c r="C116" s="30" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
     </row>
     <row r="117" spans="3:3">
       <c r="C117" s="30" t="s">
-        <v>246</v>
+        <v>221</v>
       </c>
     </row>
     <row r="118" spans="3:3">
       <c r="C118" s="30" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
     </row>
     <row r="119" spans="3:3">
       <c r="C119" s="30" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
     </row>
     <row r="120" spans="3:3">
       <c r="C120" s="30" t="s">
-        <v>249</v>
+        <v>224</v>
       </c>
     </row>
     <row r="121" spans="3:3">
       <c r="C121" s="30" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
     </row>
     <row r="122" spans="3:3">
       <c r="C122" s="30" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
     </row>
     <row r="123" spans="3:3">
       <c r="C123" s="30" t="s">
-        <v>252</v>
+        <v>227</v>
       </c>
     </row>
     <row r="124" spans="3:3">
       <c r="C124" s="30" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
     </row>
     <row r="125" spans="3:3">
       <c r="C125" s="30" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
     </row>
     <row r="126" spans="3:3">
       <c r="C126" s="30" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
     </row>
     <row r="127" spans="3:3">
       <c r="C127" s="30" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
     </row>
     <row r="128" spans="3:3">
       <c r="C128" s="30" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
     </row>
     <row r="129" spans="3:3">
       <c r="C129" s="30" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
     </row>
     <row r="130" spans="3:3">
       <c r="C130" s="30" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
     </row>
     <row r="131" spans="3:3">
       <c r="C131" s="30" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
     </row>
     <row r="132" spans="3:3">
       <c r="C132" s="30" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
     </row>
     <row r="133" spans="3:3">
       <c r="C133" s="30" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
     </row>
     <row r="134" spans="3:3">
       <c r="C134" s="30" t="s">
-        <v>449</v>
+        <v>422</v>
       </c>
     </row>
     <row r="135" spans="3:3">
       <c r="C135" t="s">
-        <v>331</v>
+        <v>306</v>
       </c>
     </row>
     <row r="136" spans="3:3">
       <c r="C136" t="s">
-        <v>332</v>
+        <v>307</v>
       </c>
     </row>
     <row r="137" spans="3:3">
       <c r="C137" t="s">
-        <v>333</v>
+        <v>308</v>
       </c>
     </row>
     <row r="138" spans="3:3">
       <c r="C138" t="s">
-        <v>334</v>
+        <v>309</v>
       </c>
     </row>
     <row r="139" spans="3:3">
       <c r="C139" t="s">
-        <v>335</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -4664,298 +4708,153 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="5" width="25.33203125" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" customWidth="1"/>
-    <col min="10" max="10" width="27.33203125" customWidth="1"/>
-    <col min="11" max="11" width="21.77734375" customWidth="1"/>
-    <col min="12" max="12" width="31" customWidth="1"/>
-    <col min="13" max="13" width="14.21875" customWidth="1"/>
-    <col min="14" max="14" width="26" customWidth="1"/>
-    <col min="15" max="15" width="19.109375" customWidth="1"/>
-    <col min="16" max="16" width="21.44140625" customWidth="1"/>
+    <col min="2" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="6" max="7" width="21.6640625" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" customWidth="1"/>
+    <col min="13" max="13" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:14">
       <c r="A1" s="3" t="s">
-        <v>462</v>
+        <v>348</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>416</v>
+        <v>72</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>97</v>
+        <v>358</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>414</v>
+        <v>359</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>415</v>
+        <v>380</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>369</v>
+        <v>339</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="I1" s="43" t="s">
-        <v>506</v>
-      </c>
-      <c r="J1" s="43" t="s">
-        <v>508</v>
-      </c>
-      <c r="K1" s="43" t="s">
-        <v>507</v>
-      </c>
-      <c r="L1" s="43" t="s">
-        <v>509</v>
-      </c>
-      <c r="M1" s="44" t="s">
-        <v>519</v>
-      </c>
-      <c r="N1" s="44" t="s">
-        <v>518</v>
-      </c>
-      <c r="O1" s="44" t="s">
-        <v>520</v>
-      </c>
-      <c r="P1" s="44" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+        <v>357</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" ht="43.2">
       <c r="A2" t="s">
-        <v>463</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>367</v>
-      </c>
-      <c r="C2" t="s">
-        <v>491</v>
-      </c>
-      <c r="D2" t="s">
-        <v>62</v>
+        <v>375</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>383</v>
       </c>
       <c r="E2" t="s">
-        <v>496</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>328</v>
-      </c>
-      <c r="G2" t="s">
-        <v>329</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>500</v>
-      </c>
-      <c r="I2" t="s">
-        <v>510</v>
-      </c>
-      <c r="J2" t="s">
-        <v>513</v>
+        <v>381</v>
+      </c>
+      <c r="H2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2">
+        <v>9218</v>
       </c>
       <c r="K2" t="s">
-        <v>515</v>
-      </c>
-      <c r="L2" t="s">
-        <v>516</v>
-      </c>
-      <c r="M2" t="s">
-        <v>330</v>
-      </c>
-      <c r="N2" t="s">
-        <v>368</v>
-      </c>
-      <c r="O2" t="s">
-        <v>522</v>
-      </c>
-      <c r="P2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>463</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="C3" t="s">
-        <v>492</v>
-      </c>
-      <c r="D3" t="s">
-        <v>362</v>
+        <v>382</v>
       </c>
       <c r="E3" t="s">
-        <v>497</v>
-      </c>
-      <c r="F3" t="s">
-        <v>328</v>
-      </c>
-      <c r="G3" t="s">
-        <v>363</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>501</v>
-      </c>
-      <c r="I3" t="s">
-        <v>511</v>
-      </c>
-      <c r="J3" t="s">
-        <v>513</v>
+        <v>379</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3">
+        <v>2970</v>
       </c>
       <c r="K3" t="s">
-        <v>515</v>
-      </c>
-      <c r="L3" t="s">
-        <v>516</v>
-      </c>
-      <c r="M3" t="s">
-        <v>364</v>
-      </c>
-      <c r="N3" t="s">
-        <v>368</v>
-      </c>
-      <c r="O3" t="s">
-        <v>522</v>
-      </c>
-      <c r="P3" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>463</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>367</v>
-      </c>
-      <c r="C4" t="s">
-        <v>493</v>
-      </c>
-      <c r="D4" t="s">
-        <v>371</v>
-      </c>
-      <c r="E4" t="s">
-        <v>498</v>
-      </c>
-      <c r="F4" t="s">
-        <v>328</v>
-      </c>
-      <c r="G4" t="s">
-        <v>372</v>
-      </c>
-      <c r="H4" t="s">
-        <v>373</v>
-      </c>
-      <c r="I4" t="s">
-        <v>361</v>
-      </c>
-      <c r="J4" t="s">
-        <v>513</v>
-      </c>
-      <c r="K4" t="s">
-        <v>515</v>
-      </c>
-      <c r="L4" t="s">
-        <v>516</v>
-      </c>
-      <c r="M4" t="s">
-        <v>374</v>
-      </c>
-      <c r="N4" t="s">
-        <v>368</v>
-      </c>
-      <c r="O4" t="s">
-        <v>522</v>
-      </c>
-      <c r="P4" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>463</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>494</v>
-      </c>
-      <c r="D5" t="s">
-        <v>482</v>
-      </c>
-      <c r="E5" t="s">
-        <v>499</v>
-      </c>
-      <c r="F5" t="s">
-        <v>483</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>484</v>
-      </c>
-      <c r="I5" t="s">
-        <v>512</v>
-      </c>
-      <c r="J5" t="s">
-        <v>513</v>
-      </c>
-      <c r="K5" t="s">
-        <v>514</v>
-      </c>
-      <c r="L5" t="s">
-        <v>517</v>
-      </c>
-      <c r="M5" t="s">
-        <v>490</v>
-      </c>
-      <c r="N5" t="s">
-        <v>368</v>
-      </c>
-      <c r="O5" t="s">
-        <v>522</v>
-      </c>
-      <c r="P5" t="s">
-        <v>521</v>
+        <v>378</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6 I6 M6">
-      <formula1>EquipmentCategories</formula1>
-    </dataValidation>
-  </dataValidations>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4966,47 +4865,7 @@
     <col min="6" max="6" width="15.21875" customWidth="1"/>
     <col min="7" max="7" width="12.44140625" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="B2" t="s">
-        <v>502</v>
-      </c>
-      <c r="C2" t="s">
-        <v>414</v>
-      </c>
-      <c r="D2" t="s">
-        <v>415</v>
-      </c>
-      <c r="E2" t="s">
-        <v>368</v>
-      </c>
-      <c r="F2" t="s">
-        <v>503</v>
-      </c>
-      <c r="G2" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="B5" t="s">
-        <v>360</v>
-      </c>
-      <c r="C5" t="s">
-        <v>414</v>
-      </c>
-      <c r="D5" t="s">
-        <v>415</v>
-      </c>
-      <c r="E5" t="s">
-        <v>505</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5016,8 +4875,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5030,359 +4889,359 @@
     <row r="1" spans="1:4">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
-        <v>458</v>
+        <v>431</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>50</v>
+        <v>529</v>
       </c>
       <c r="C2" t="s">
-        <v>445</v>
+        <v>418</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>51</v>
+        <v>530</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>53</v>
+        <v>531</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>469</v>
+        <v>442</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>54</v>
+        <v>532</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>343</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>56</v>
+        <v>533</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>58</v>
+        <v>534</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="s">
-        <v>60</v>
+        <v>535</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>345</v>
+        <v>318</v>
       </c>
       <c r="D9" t="s">
-        <v>346</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="s">
-        <v>340</v>
+        <v>313</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>342</v>
+        <v>315</v>
       </c>
       <c r="D10" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="B11" t="s">
+      <c r="B11" s="45" t="s">
+        <v>509</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="45" t="s">
+        <v>510</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" s="45" t="s">
+        <v>511</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" s="45" t="s">
+        <v>512</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" s="45" t="s">
+        <v>513</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" s="45" t="s">
+        <v>514</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="45" t="s">
+        <v>515</v>
+      </c>
+      <c r="C17" t="s">
+        <v>311</v>
+      </c>
+      <c r="D17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="45" t="s">
+        <v>516</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="45" t="s">
+        <v>517</v>
+      </c>
+      <c r="C19" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="45" t="s">
+        <v>518</v>
+      </c>
+      <c r="C20" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="D11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="B12" t="s">
+      <c r="D20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="46" t="s">
+        <v>519</v>
+      </c>
+      <c r="C21" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="D21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="46" t="s">
+        <v>520</v>
+      </c>
+      <c r="C22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="46" t="s">
+        <v>521</v>
+      </c>
+      <c r="C23" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="D12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="B13" t="s">
+      <c r="D23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="46" t="s">
+        <v>522</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>432</v>
+      </c>
+      <c r="D24" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="46" t="s">
+        <v>523</v>
+      </c>
+      <c r="C25" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="D25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="46" t="s">
+        <v>524</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="46" t="s">
+        <v>525</v>
+      </c>
+      <c r="C27" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="B14" t="s">
+      <c r="D27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="46" t="s">
+        <v>526</v>
+      </c>
+      <c r="C28" t="s">
         <v>69</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="46" t="s">
+        <v>527</v>
+      </c>
+      <c r="C29" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="B15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="B16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" t="s">
-        <v>336</v>
-      </c>
-      <c r="D17" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" t="s">
-        <v>95</v>
-      </c>
-      <c r="C22" t="s">
-        <v>96</v>
-      </c>
-      <c r="D22" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" t="s">
-        <v>338</v>
-      </c>
-      <c r="C24" s="40" t="s">
-        <v>459</v>
-      </c>
-      <c r="D24" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" t="s">
-        <v>88</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" t="s">
-        <v>89</v>
-      </c>
-      <c r="C27" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="D27" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" t="s">
-        <v>91</v>
-      </c>
-      <c r="C28" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" s="27" t="s">
-        <v>94</v>
-      </c>
       <c r="D29" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="2:4">
-      <c r="B30" t="s">
-        <v>337</v>
+      <c r="B30" s="46" t="s">
+        <v>528</v>
       </c>
       <c r="C30" s="27"/>
       <c r="D30" t="s">
-        <v>461</v>
+        <v>434</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="3" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="C31" t="s">
-        <v>435</v>
+        <v>408</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="B32" s="3" t="s">
-        <v>421</v>
+        <v>394</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="3" t="s">
-        <v>420</v>
+        <v>393</v>
       </c>
       <c r="C33" t="s">
-        <v>347</v>
+        <v>320</v>
       </c>
     </row>
     <row r="34" spans="2:3">
       <c r="B34" s="3" t="s">
-        <v>419</v>
+        <v>392</v>
       </c>
       <c r="C34">
         <v>255</v>
@@ -5390,7 +5249,7 @@
     </row>
     <row r="35" spans="2:3">
       <c r="B35" s="3" t="s">
-        <v>422</v>
+        <v>395</v>
       </c>
       <c r="C35">
         <v>17025</v>
@@ -5398,7 +5257,7 @@
     </row>
     <row r="36" spans="2:3">
       <c r="B36" s="3" t="s">
-        <v>423</v>
+        <v>396</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -5461,25 +5320,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>465</v>
+        <v>438</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>416</v>
+        <v>389</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="E1" s="32" t="s">
         <v>414</v>
       </c>
-      <c r="E1" s="32" t="s">
-        <v>441</v>
-      </c>
       <c r="F1" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>415</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>442</v>
       </c>
       <c r="H1" s="3"/>
     </row>
@@ -5489,175 +5348,175 @@
     </row>
     <row r="3" spans="1:8" ht="28.8">
       <c r="A3" t="s">
-        <v>463</v>
+        <v>436</v>
       </c>
       <c r="B3" t="s">
-        <v>377</v>
+        <v>350</v>
       </c>
       <c r="C3" t="s">
-        <v>397</v>
+        <v>370</v>
       </c>
       <c r="D3" t="s">
-        <v>356</v>
+        <v>329</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>355</v>
+        <v>328</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>357</v>
+        <v>330</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>358</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="111.75" customHeight="1">
       <c r="A4" t="s">
-        <v>463</v>
+        <v>436</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>377</v>
+        <v>350</v>
       </c>
       <c r="C4" t="s">
-        <v>480</v>
+        <v>453</v>
       </c>
       <c r="D4" t="s">
-        <v>401</v>
+        <v>374</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>400</v>
+        <v>373</v>
       </c>
       <c r="F4" t="s">
-        <v>401</v>
+        <v>374</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>399</v>
+        <v>372</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8">
       <c r="A5" t="s">
-        <v>463</v>
+        <v>436</v>
       </c>
       <c r="B5" t="s">
-        <v>378</v>
+        <v>351</v>
       </c>
       <c r="C5" t="s">
-        <v>411</v>
+        <v>384</v>
       </c>
       <c r="D5" t="s">
-        <v>412</v>
+        <v>385</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>470</v>
+        <v>443</v>
       </c>
       <c r="F5" t="s">
-        <v>413</v>
+        <v>386</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>471</v>
+        <v>444</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="57.6">
       <c r="A6" t="s">
-        <v>463</v>
+        <v>436</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>377</v>
+        <v>350</v>
       </c>
       <c r="C6" t="s">
-        <v>481</v>
+        <v>454</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>478</v>
+        <v>451</v>
       </c>
       <c r="F6" t="s">
-        <v>477</v>
+        <v>450</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>479</v>
+        <v>452</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="43.2">
       <c r="A7" t="s">
-        <v>463</v>
+        <v>436</v>
       </c>
       <c r="B7" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="C7" t="s">
-        <v>472</v>
+        <v>445</v>
       </c>
       <c r="D7" t="s">
-        <v>466</v>
+        <v>439</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>353</v>
+        <v>326</v>
       </c>
       <c r="F7" t="s">
-        <v>467</v>
+        <v>440</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>468</v>
+        <v>441</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>463</v>
+        <v>436</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>377</v>
+        <v>350</v>
       </c>
       <c r="C8" t="s">
-        <v>398</v>
+        <v>371</v>
       </c>
       <c r="G8" s="33"/>
     </row>
     <row r="9" spans="1:8" ht="230.4">
       <c r="A9" s="38" t="s">
-        <v>463</v>
+        <v>436</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>418</v>
+        <v>391</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>425</v>
+        <v>398</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>427</v>
+        <v>400</v>
       </c>
       <c r="E9" s="39" t="s">
-        <v>433</v>
+        <v>406</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>428</v>
+        <v>401</v>
       </c>
       <c r="G9" s="39" t="s">
-        <v>434</v>
+        <v>407</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8">
       <c r="A10" s="38" t="s">
-        <v>463</v>
+        <v>436</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>424</v>
+        <v>397</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>426</v>
+        <v>399</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>429</v>
+        <v>402</v>
       </c>
       <c r="E10" s="39" t="s">
-        <v>431</v>
+        <v>404</v>
       </c>
       <c r="F10" s="39" t="s">
-        <v>430</v>
+        <v>403</v>
       </c>
       <c r="G10" s="39" t="s">
-        <v>432</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -5696,57 +5555,57 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>464</v>
+        <v>437</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1" t="s">
         <v>414</v>
       </c>
-      <c r="D1" t="s">
-        <v>441</v>
-      </c>
       <c r="E1" t="s">
+        <v>388</v>
+      </c>
+      <c r="F1" t="s">
         <v>415</v>
       </c>
-      <c r="F1" t="s">
-        <v>442</v>
-      </c>
       <c r="G1" t="s">
-        <v>443</v>
+        <v>416</v>
       </c>
       <c r="H1" t="s">
-        <v>360</v>
+        <v>333</v>
       </c>
       <c r="I1" t="s">
         <v>31</v>
       </c>
       <c r="J1" t="s">
-        <v>444</v>
+        <v>417</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>463</v>
+        <v>436</v>
       </c>
       <c r="B2" t="s">
-        <v>359</v>
+        <v>332</v>
       </c>
       <c r="C2" t="s">
-        <v>485</v>
+        <v>458</v>
       </c>
       <c r="D2" t="s">
-        <v>486</v>
+        <v>459</v>
       </c>
       <c r="E2" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="F2" t="s">
-        <v>488</v>
+        <v>461</v>
       </c>
       <c r="G2" t="s">
-        <v>489</v>
+        <v>462</v>
       </c>
       <c r="H2">
         <v>-0.5</v>
@@ -5780,30 +5639,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>465</v>
+        <v>438</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>421</v>
+        <v>394</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>420</v>
+        <v>393</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>419</v>
+        <v>392</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>422</v>
+        <v>395</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>423</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>463</v>
+        <v>436</v>
       </c>
       <c r="B2" t="str">
         <f>AdministrativeData!C31</f>
@@ -5868,7 +5727,7 @@
         <v>29</v>
       </c>
       <c r="G1" s="42" t="s">
-        <v>365</v>
+        <v>338</v>
       </c>
       <c r="H1" s="42"/>
       <c r="I1" s="42"/>
@@ -5877,26 +5736,26 @@
     </row>
     <row r="2" spans="1:19" ht="17.25" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>350</v>
+        <v>323</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>457</v>
+        <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="26" t="s">
-        <v>348</v>
+        <v>321</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>326</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="26" t="s">
-        <v>349</v>
+        <v>322</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>456</v>
+        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -5929,7 +5788,7 @@
         <v>44</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>21</v>
@@ -5956,31 +5815,31 @@
         <v>18</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>452</v>
+        <v>425</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>452</v>
+        <v>425</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>452</v>
+        <v>425</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>452</v>
+        <v>425</v>
       </c>
       <c r="P9" s="12" t="s">
-        <v>452</v>
+        <v>425</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>452</v>
+        <v>425</v>
       </c>
       <c r="R9" s="12" t="s">
-        <v>452</v>
+        <v>425</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>452</v>
+        <v>425</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="21.6">
@@ -5988,7 +5847,7 @@
         <v>46</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>23</v>
@@ -6012,10 +5871,10 @@
         <v>39</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="L10" s="12" t="s">
         <v>24</v>
@@ -6047,58 +5906,58 @@
         <v>45</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>449</v>
+        <v>422</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>449</v>
+        <v>422</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>449</v>
+        <v>422</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>449</v>
+        <v>422</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>449</v>
+        <v>422</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>449</v>
+        <v>422</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>449</v>
+        <v>422</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>449</v>
+        <v>422</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="O11" s="11" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>453</v>
+        <v>426</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>453</v>
+        <v>426</v>
       </c>
       <c r="R11" s="11" t="s">
-        <v>331</v>
+        <v>306</v>
       </c>
       <c r="S11" s="11" t="s">
-        <v>331</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="21.6">
@@ -6106,117 +5965,117 @@
         <v>31</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>450</v>
+        <v>423</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>450</v>
+        <v>423</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>450</v>
+        <v>423</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>450</v>
+        <v>423</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>450</v>
+        <v>423</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>451</v>
+        <v>424</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>451</v>
+        <v>424</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>451</v>
+        <v>424</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>455</v>
+        <v>428</v>
       </c>
       <c r="M12" s="15" t="s">
-        <v>455</v>
+        <v>428</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>454</v>
+        <v>427</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>454</v>
+        <v>427</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>451</v>
+        <v>424</v>
       </c>
       <c r="Q12" s="14" t="s">
-        <v>451</v>
+        <v>424</v>
       </c>
       <c r="R12" s="14" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
       <c r="S12" s="14" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="35" t="s">
-        <v>392</v>
+        <v>365</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="I13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>396</v>
+        <v>369</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>437</v>
+        <v>410</v>
       </c>
       <c r="L13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="M13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="N13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="O13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="P13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="Q13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="R13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="S13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -6224,7 +6083,7 @@
         <v>30</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>325</v>
+        <v>300</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
@@ -6249,7 +6108,7 @@
         <v>32</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>446</v>
+        <v>419</v>
       </c>
       <c r="C15" s="17">
         <v>1000</v>
@@ -6276,7 +6135,7 @@
         <v>33</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>447</v>
+        <v>420</v>
       </c>
       <c r="C16" s="17">
         <v>5000</v>
@@ -6303,7 +6162,7 @@
         <v>34</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>448</v>
+        <v>421</v>
       </c>
       <c r="C17" s="17">
         <v>10000</v>
@@ -6383,10 +6242,298 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:P5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="5" width="25.33203125" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="10" max="10" width="27.33203125" customWidth="1"/>
+    <col min="11" max="11" width="21.77734375" customWidth="1"/>
+    <col min="12" max="12" width="31" customWidth="1"/>
+    <col min="13" max="13" width="14.21875" customWidth="1"/>
+    <col min="14" max="14" width="26" customWidth="1"/>
+    <col min="15" max="15" width="19.109375" customWidth="1"/>
+    <col min="16" max="16" width="21.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="I1" s="43" t="s">
+        <v>475</v>
+      </c>
+      <c r="J1" s="43" t="s">
+        <v>477</v>
+      </c>
+      <c r="K1" s="43" t="s">
+        <v>476</v>
+      </c>
+      <c r="L1" s="43" t="s">
+        <v>478</v>
+      </c>
+      <c r="M1" s="44" t="s">
+        <v>488</v>
+      </c>
+      <c r="N1" s="44" t="s">
+        <v>487</v>
+      </c>
+      <c r="O1" s="44" t="s">
+        <v>489</v>
+      </c>
+      <c r="P1" s="44" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>436</v>
+      </c>
+      <c r="B2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C2" t="s">
+        <v>464</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>469</v>
+      </c>
+      <c r="F2" t="s">
+        <v>303</v>
+      </c>
+      <c r="G2" t="s">
+        <v>304</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>473</v>
+      </c>
+      <c r="I2" t="s">
+        <v>479</v>
+      </c>
+      <c r="J2" t="s">
+        <v>482</v>
+      </c>
+      <c r="K2" t="s">
+        <v>484</v>
+      </c>
+      <c r="L2" t="s">
+        <v>485</v>
+      </c>
+      <c r="M2" t="s">
+        <v>305</v>
+      </c>
+      <c r="N2" t="s">
+        <v>341</v>
+      </c>
+      <c r="O2" t="s">
+        <v>491</v>
+      </c>
+      <c r="P2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>436</v>
+      </c>
+      <c r="B3" t="s">
+        <v>340</v>
+      </c>
+      <c r="C3" t="s">
+        <v>465</v>
+      </c>
+      <c r="D3" t="s">
+        <v>335</v>
+      </c>
+      <c r="E3" t="s">
+        <v>470</v>
+      </c>
+      <c r="F3" t="s">
+        <v>303</v>
+      </c>
+      <c r="G3" t="s">
+        <v>336</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>474</v>
+      </c>
+      <c r="I3" t="s">
+        <v>480</v>
+      </c>
+      <c r="J3" t="s">
+        <v>482</v>
+      </c>
+      <c r="K3" t="s">
+        <v>484</v>
+      </c>
+      <c r="L3" t="s">
+        <v>485</v>
+      </c>
+      <c r="M3" t="s">
+        <v>337</v>
+      </c>
+      <c r="N3" t="s">
+        <v>341</v>
+      </c>
+      <c r="O3" t="s">
+        <v>491</v>
+      </c>
+      <c r="P3" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>436</v>
+      </c>
+      <c r="B4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C4" t="s">
+        <v>466</v>
+      </c>
+      <c r="D4" t="s">
+        <v>344</v>
+      </c>
+      <c r="E4" t="s">
+        <v>471</v>
+      </c>
+      <c r="F4" t="s">
+        <v>303</v>
+      </c>
+      <c r="G4" t="s">
+        <v>345</v>
+      </c>
+      <c r="H4" t="s">
+        <v>346</v>
+      </c>
+      <c r="I4" t="s">
+        <v>334</v>
+      </c>
+      <c r="J4" t="s">
+        <v>482</v>
+      </c>
+      <c r="K4" t="s">
+        <v>484</v>
+      </c>
+      <c r="L4" t="s">
+        <v>485</v>
+      </c>
+      <c r="M4" t="s">
+        <v>347</v>
+      </c>
+      <c r="N4" t="s">
+        <v>341</v>
+      </c>
+      <c r="O4" t="s">
+        <v>491</v>
+      </c>
+      <c r="P4" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>436</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>467</v>
+      </c>
+      <c r="D5" t="s">
+        <v>455</v>
+      </c>
+      <c r="E5" t="s">
+        <v>472</v>
+      </c>
+      <c r="F5" t="s">
+        <v>456</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>457</v>
+      </c>
+      <c r="I5" t="s">
+        <v>481</v>
+      </c>
+      <c r="J5" t="s">
+        <v>482</v>
+      </c>
+      <c r="K5" t="s">
+        <v>483</v>
+      </c>
+      <c r="L5" t="s">
+        <v>486</v>
+      </c>
+      <c r="M5" t="s">
+        <v>463</v>
+      </c>
+      <c r="N5" t="s">
+        <v>341</v>
+      </c>
+      <c r="O5" t="s">
+        <v>491</v>
+      </c>
+      <c r="P5" t="s">
+        <v>490</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6 I6 M6">
+      <formula1>EquipmentCategories</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6411,7 +6558,7 @@
         <v>29</v>
       </c>
       <c r="G1" s="42" t="s">
-        <v>365</v>
+        <v>338</v>
       </c>
       <c r="H1" s="42"/>
       <c r="I1" s="42"/>
@@ -6421,26 +6568,26 @@
     </row>
     <row r="2" spans="1:17" ht="17.25" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>350</v>
+        <v>323</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>327</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="26" t="s">
-        <v>348</v>
+        <v>321</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="26" t="s">
-        <v>349</v>
+        <v>322</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>359</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -6473,7 +6620,7 @@
         <v>44</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>20</v>
@@ -6509,16 +6656,16 @@
         <v>21</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="P9" s="11" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="21.6">
@@ -6526,7 +6673,7 @@
         <v>46</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>23</v>
@@ -6553,7 +6700,7 @@
         <v>2</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>474</v>
+        <v>447</v>
       </c>
       <c r="L10" s="11" t="s">
         <v>4</v>
@@ -6562,7 +6709,7 @@
         <v>5</v>
       </c>
       <c r="N10" s="11" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="O10" s="11" t="s">
         <v>39</v>
@@ -6579,52 +6726,52 @@
         <v>45</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="O11" s="11" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -6632,7 +6779,7 @@
         <v>31</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>27</v>
@@ -6662,83 +6809,83 @@
         <v>27</v>
       </c>
       <c r="L12" s="14" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="M12" s="15" t="s">
         <v>28</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
       <c r="Q12" s="14" t="s">
-        <v>440</v>
+        <v>413</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="35" t="s">
-        <v>392</v>
+        <v>365</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="I13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="L13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="M13" s="34" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
       <c r="N13" s="34" t="s">
-        <v>424</v>
+        <v>397</v>
       </c>
       <c r="O13" s="34" t="s">
-        <v>351</v>
+        <v>324</v>
       </c>
       <c r="P13" s="34" t="s">
-        <v>396</v>
+        <v>369</v>
       </c>
       <c r="Q13" s="34" t="s">
-        <v>436</v>
+        <v>409</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="31.8">
       <c r="A14" s="22" t="s">
-        <v>30</v>
+        <v>493</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>325</v>
+        <v>300</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>17</v>
@@ -6762,10 +6909,10 @@
         <v>42</v>
       </c>
       <c r="J14" s="22" t="s">
-        <v>476</v>
+        <v>449</v>
       </c>
       <c r="K14" s="22" t="s">
-        <v>475</v>
+        <v>448</v>
       </c>
       <c r="L14" s="22" t="s">
         <v>4</v>
@@ -6774,96 +6921,94 @@
         <v>47</v>
       </c>
       <c r="N14" s="22" t="s">
-        <v>439</v>
+        <v>412</v>
       </c>
       <c r="O14" s="22" t="s">
-        <v>352</v>
+        <v>325</v>
       </c>
       <c r="P14" s="22" t="s">
-        <v>395</v>
+        <v>368</v>
       </c>
       <c r="Q14" s="22" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="A15" s="5" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="31.8">
+      <c r="A15" s="22" t="s">
+        <v>494</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>508</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>495</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>496</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>497</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>498</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>499</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>500</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="J15" s="22" t="s">
+        <v>501</v>
+      </c>
+      <c r="K15" s="22" t="s">
+        <v>502</v>
+      </c>
+      <c r="L15" s="22" t="s">
+        <v>450</v>
+      </c>
+      <c r="M15" s="23" t="s">
+        <v>503</v>
+      </c>
+      <c r="N15" s="22" t="s">
+        <v>504</v>
+      </c>
+      <c r="O15" s="22" t="s">
+        <v>505</v>
+      </c>
+      <c r="P15" s="22" t="s">
+        <v>506</v>
+      </c>
+      <c r="Q15" s="22" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B16" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C16" s="17">
         <v>0</v>
       </c>
-      <c r="D15" s="18">
-        <f>ROUND(E15+273.15,2)</f>
+      <c r="D16" s="18">
+        <f>ROUND(E16+273.15,2)</f>
         <v>273.14999999999998</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E16" s="18">
         <v>0</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F16" s="9">
         <v>-0.1</v>
       </c>
-      <c r="G15" s="9">
-        <f>ROUND(F15-E15,1)</f>
+      <c r="G16" s="9">
+        <f>ROUND(F16-E16,1)</f>
         <v>-0.1</v>
-      </c>
-      <c r="H15" s="24">
-        <v>0.05</v>
-      </c>
-      <c r="I15" s="25">
-        <v>2</v>
-      </c>
-      <c r="J15" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="K15" s="9">
-        <v>-0.2</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="M15" s="8">
-        <v>1</v>
-      </c>
-      <c r="N15" s="9" t="s">
-        <v>398</v>
-      </c>
-      <c r="O15" s="9" t="s">
-        <v>472</v>
-      </c>
-      <c r="P15" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="Q15" s="9" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="17">
-        <v>15</v>
-      </c>
-      <c r="D16" s="18">
-        <f t="shared" ref="D16:D19" si="0">ROUND(E16+273.15,2)</f>
-        <v>288.14999999999998</v>
-      </c>
-      <c r="E16" s="18">
-        <v>15.000999999999999</v>
-      </c>
-      <c r="F16" s="9">
-        <v>15.1</v>
-      </c>
-      <c r="G16" s="9">
-        <f t="shared" ref="G16:G19" si="1">ROUND(F16-E16,1)</f>
-        <v>0.1</v>
       </c>
       <c r="H16" s="24">
         <v>0.05</v>
@@ -6881,197 +7026,248 @@
         <v>25</v>
       </c>
       <c r="M16" s="8">
+        <v>1</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="17">
+        <v>15</v>
+      </c>
+      <c r="D17" s="18">
+        <f t="shared" ref="D17:D20" si="0">ROUND(E17+273.15,2)</f>
+        <v>288.14999999999998</v>
+      </c>
+      <c r="E17" s="18">
+        <v>15.000999999999999</v>
+      </c>
+      <c r="F17" s="9">
+        <v>15.1</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" ref="G17:G20" si="1">ROUND(F17-E17,1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="I17" s="25">
         <v>2</v>
       </c>
-      <c r="N16" s="9" t="s">
-        <v>398</v>
-      </c>
-      <c r="O16" s="9" t="s">
-        <v>398</v>
-      </c>
-      <c r="P16" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="Q16" s="9" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="A17" s="5" t="s">
+      <c r="J17" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="K17" s="9">
+        <v>-0.2</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="8">
+        <v>2</v>
+      </c>
+      <c r="N17" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="O17" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q17" s="9" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B18" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C18" s="17">
         <v>25</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D18" s="18">
         <f t="shared" si="0"/>
         <v>298.14999999999998</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E18" s="18">
         <v>25.001999999999999</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F18" s="9">
         <v>25.2</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G18" s="9">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="H17" s="24">
+      <c r="H18" s="24">
         <v>0.05</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I18" s="25">
         <v>2</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J18" s="9">
         <v>0.2</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K18" s="9">
         <v>-0.2</v>
       </c>
-      <c r="L17" s="9" t="s">
+      <c r="L18" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M17" s="8">
+      <c r="M18" s="8">
         <v>3</v>
       </c>
-      <c r="N17" s="9" t="s">
-        <v>426</v>
-      </c>
-      <c r="O17" s="9" t="s">
-        <v>398</v>
-      </c>
-      <c r="P17" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="Q17" s="9" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18" s="6" t="s">
+      <c r="N18" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="P18" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q18" s="9" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B19" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C19" s="17">
         <v>15</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D19" s="18">
         <f t="shared" si="0"/>
         <v>288.14999999999998</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E19" s="18">
         <v>15</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F19" s="9">
         <v>15.3</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G19" s="9">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="H18" s="24">
+      <c r="H19" s="24">
         <v>0.05</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I19" s="25">
         <v>2</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J19" s="9">
         <v>0.2</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K19" s="9">
         <v>-0.2</v>
       </c>
-      <c r="L18" s="9" t="s">
+      <c r="L19" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="M18" s="8">
+      <c r="M19" s="8">
         <v>4</v>
       </c>
-      <c r="N18" s="9" t="s">
-        <v>398</v>
-      </c>
-      <c r="O18" s="9" t="s">
-        <v>472</v>
-      </c>
-      <c r="P18" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="Q18" s="9" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19" s="5" t="s">
+      <c r="N19" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="O19" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="P19" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q19" s="9" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B20" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C20" s="20">
         <v>0</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D20" s="18">
         <f t="shared" si="0"/>
         <v>273.14999999999998</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E20" s="21">
         <v>-1E-3</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F20" s="7">
         <v>0</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G20" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H19" s="24">
+      <c r="H20" s="24">
         <v>0.05</v>
       </c>
-      <c r="I19" s="25">
+      <c r="I20" s="25">
         <v>2</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J20" s="7">
         <v>0.2</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K20" s="9">
         <v>-0.2</v>
       </c>
-      <c r="L19" s="9" t="s">
+      <c r="L20" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M19" s="4">
+      <c r="M20" s="4">
         <v>5</v>
       </c>
-      <c r="N19" s="7" t="s">
-        <v>398</v>
-      </c>
-      <c r="O19" s="7" t="s">
-        <v>472</v>
-      </c>
-      <c r="P19" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="Q19" s="9" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
+      <c r="N20" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="P20" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q20" s="9" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="26"/>
@@ -7092,6 +7288,10 @@
     <row r="28" spans="1:17">
       <c r="A28" s="26"/>
       <c r="B28" s="26"/>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -7118,7 +7318,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:I1"/>
@@ -7141,28 +7341,28 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="I1" s="3"/>
     </row>
@@ -7172,147 +7372,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P46" sqref="P46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="2" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
-    <col min="6" max="7" width="21.6640625" customWidth="1"/>
-    <col min="8" max="8" width="25.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" customWidth="1"/>
-    <col min="13" max="13" width="18.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>366</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="N1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" ht="43.2">
-      <c r="A2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" t="s">
-        <v>402</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>410</v>
-      </c>
-      <c r="E2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" t="s">
-        <v>408</v>
-      </c>
-      <c r="H2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I2">
-        <v>9218</v>
-      </c>
-      <c r="K2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" t="s">
-        <v>403</v>
-      </c>
-      <c r="C3" t="s">
-        <v>409</v>
-      </c>
-      <c r="E3" t="s">
-        <v>406</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>70</v>
-      </c>
-      <c r="I3">
-        <v>2970</v>
-      </c>
-      <c r="K3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B5" t="s">
-        <v>405</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add MedicoSupport Example. Update search function
</commit_message>
<xml_diff>
--- a/Examples/DCC_temperature.xlsx
+++ b/Examples/DCC_temperature.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\MS\4006-03 AI metrologi\Software\DCCtables\master\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tesla\Data\MS\4006-03 AI metrologi\Software\DCCtables\master\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86897254-300B-41D7-AA5F-8215F1B47668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21396" activeTab="1"/>
+    <workbookView xWindow="1650" yWindow="975" windowWidth="37200" windowHeight="17310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -21,8 +22,8 @@
     <sheet name="Equipment" sheetId="12" r:id="rId7"/>
     <sheet name="Table_TempCal" sheetId="14" r:id="rId8"/>
     <sheet name="Software" sheetId="8" state="hidden" r:id="rId9"/>
-    <sheet name="Locations" sheetId="13" state="hidden" r:id="rId10"/>
-    <sheet name="Sheet1" sheetId="15" r:id="rId11"/>
+    <sheet name="Locations" sheetId="15" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="16" r:id="rId11"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId12"/>
@@ -41,7 +42,7 @@
     <definedName name="statementCategories">Definitions!$F$2:$F$10</definedName>
     <definedName name="UsedReference">metaDataType</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="531">
   <si>
     <t>customerTag</t>
   </si>
@@ -295,9 +296,6 @@
     <t>norm</t>
   </si>
   <si>
-    <t>location</t>
-  </si>
-  <si>
     <t>XPATH</t>
   </si>
   <si>
@@ -1081,9 +1079,6 @@
     <t>LABORATORY</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>item</t>
   </si>
   <si>
@@ -1132,31 +1127,7 @@
     <t>Equipment Categories</t>
   </si>
   <si>
-    <t>StreetNo</t>
-  </si>
-  <si>
     <t>City</t>
-  </si>
-  <si>
-    <t>Name1</t>
-  </si>
-  <si>
-    <t>Name2</t>
-  </si>
-  <si>
-    <t>PostCode</t>
-  </si>
-  <si>
-    <t>PO-BOX</t>
-  </si>
-  <si>
-    <t>CountryCode</t>
-  </si>
-  <si>
-    <t>further</t>
-  </si>
-  <si>
-    <t>p</t>
   </si>
   <si>
     <t>metaDataType</t>
@@ -1196,25 +1167,7 @@
     <t>lab</t>
   </si>
   <si>
-    <t>field1</t>
-  </si>
-  <si>
-    <t>field2</t>
-  </si>
-  <si>
-    <t>kogle alle</t>
-  </si>
-  <si>
     <t>Street1</t>
-  </si>
-  <si>
-    <t>16, 1. tv</t>
-  </si>
-  <si>
-    <t>DFM</t>
-  </si>
-  <si>
-    <t>Danish Professional Company</t>
   </si>
   <si>
     <t>meth01</t>
@@ -1675,12 +1628,45 @@
   </si>
   <si>
     <t>EndDate</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>Street_No</t>
+  </si>
+  <si>
+    <t>Webpage</t>
+  </si>
+  <si>
+    <t>Street2</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Att</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -2020,13 +2006,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
@@ -2034,24 +2020,7 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <b/>
@@ -2123,7 +2092,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Definitions"/>
@@ -2971,7 +2940,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Januar"/>
@@ -3123,77 +3092,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table135" displayName="Table135" ref="C1:G8" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="C1:G8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table135" displayName="Table135" ref="C1:G8" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="C1:G8" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="id"/>
-    <tableColumn id="3" name="heading lang1"/>
-    <tableColumn id="4" name="body lang1" dataDxfId="4"/>
-    <tableColumn id="5" name="heading lang2"/>
-    <tableColumn id="6" name="body lang2" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="heading lang1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="body lang1" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="heading lang2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="body lang2" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table16" displayName="Table16" ref="B1:P6" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B1:P6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table16" displayName="Table16" ref="B1:P6" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="B1:P6" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="15">
-    <tableColumn id="11" name="category"/>
-    <tableColumn id="1" name="id"/>
-    <tableColumn id="4" name="heading lang1"/>
-    <tableColumn id="3" name="heading lang2"/>
-    <tableColumn id="6" name="manufacturer"/>
-    <tableColumn id="7" name="productName"/>
-    <tableColumn id="8" name="productNumber"/>
-    <tableColumn id="10" name="id1"/>
-    <tableColumn id="12" name="id1 issuer"/>
-    <tableColumn id="13" name="id1 heading lang1"/>
-    <tableColumn id="14" name="id1 heading lang2"/>
-    <tableColumn id="15" name="id2"/>
-    <tableColumn id="16" name="id2 issuer"/>
-    <tableColumn id="17" name="id2 heading lang1"/>
-    <tableColumn id="18" name="id2 heading lang2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="category"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="id"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="heading lang1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="heading lang2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="manufacturer"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="productName"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="productNumber"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="id1"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="id1 issuer"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="id1 heading lang1"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="id1 heading lang2"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="id2"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="id2 issuer"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="id2 heading lang1"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="id2 heading lang2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:H6" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:H6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:H6" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:H6" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="swID"/>
-    <tableColumn id="2" name="name"/>
-    <tableColumn id="3" name="release "/>
-    <tableColumn id="4" name="type"/>
-    <tableColumn id="5" name="description"/>
-    <tableColumn id="6" name="content"/>
-    <tableColumn id="7" name="file"/>
-    <tableColumn id="8" name="formula"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table167" displayName="Table167" ref="A1:M6" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:M6"/>
-  <tableColumns count="13">
-    <tableColumn id="11" name="Category"/>
-    <tableColumn id="1" name="id"/>
-    <tableColumn id="10" name="Name1"/>
-    <tableColumn id="13" name="Name2"/>
-    <tableColumn id="2" name="Street1"/>
-    <tableColumn id="3" name="StreetNo"/>
-    <tableColumn id="14" name="Column1"/>
-    <tableColumn id="4" name="City"/>
-    <tableColumn id="5" name="PostCode"/>
-    <tableColumn id="6" name="PO-BOX"/>
-    <tableColumn id="7" name="CountryCode"/>
-    <tableColumn id="8" name="further"/>
-    <tableColumn id="9" name="p"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="swID"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="release "/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="type"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="description"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="content"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="file"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="formula"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3495,7 +3442,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L139"/>
   <sheetViews>
@@ -3503,15 +3450,15 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" customWidth="1"/>
-    <col min="2" max="2" width="32.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="3" width="62" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3532,36 +3479,36 @@
         <v>73</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>355</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="B2" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="D2" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="F2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="I2" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="L2" s="2"/>
     </row>
@@ -3573,10 +3520,10 @@
         <v>24</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F3" t="s">
         <v>76</v>
@@ -3585,7 +3532,7 @@
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="L3" s="2"/>
     </row>
@@ -3597,16 +3544,16 @@
         <v>23</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="I4" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="L4" s="2"/>
     </row>
@@ -3615,37 +3562,37 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I5" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="I6" t="s">
         <v>0</v>
@@ -3655,16 +3602,16 @@
     <row r="7" spans="1:12">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="I7" t="s">
         <v>19</v>
@@ -3676,16 +3623,16 @@
         <v>3</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="I8" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="L8" s="2"/>
     </row>
@@ -3694,16 +3641,16 @@
         <v>4</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F9" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="I9" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="L9" s="2"/>
     </row>
@@ -3712,16 +3659,16 @@
         <v>5</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F10" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="I10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L10" s="2"/>
     </row>
@@ -3730,13 +3677,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I11" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="L11" s="2"/>
     </row>
@@ -3745,10 +3692,10 @@
         <v>22</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L12" s="2"/>
     </row>
@@ -3757,10 +3704,10 @@
         <v>39</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L13" s="2"/>
     </row>
@@ -3769,10 +3716,10 @@
         <v>40</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L14" s="2"/>
     </row>
@@ -3781,113 +3728,113 @@
         <v>43</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12">
       <c r="C16" s="30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L16" s="2"/>
     </row>
     <row r="17" spans="3:4">
       <c r="C17" s="30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" spans="3:4">
       <c r="C18" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="19" spans="3:4">
       <c r="C19" s="30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="3:4">
       <c r="C20" s="30" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
       <c r="D20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="21" spans="3:4">
       <c r="C21" s="30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D21" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="22" spans="3:4">
       <c r="C22" s="30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="3:4">
       <c r="C23" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" spans="3:4">
       <c r="C24" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="25" spans="3:4">
       <c r="C25" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="3:4">
       <c r="C26" s="30" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="3:4">
       <c r="C27" s="30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D27" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="3:4">
       <c r="C28" s="30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D28" t="s">
         <v>28</v>
@@ -3895,39 +3842,39 @@
     </row>
     <row r="29" spans="3:4">
       <c r="C29" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D29" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" spans="3:4">
       <c r="C30" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D30" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" spans="3:4">
       <c r="C31" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="3:4">
       <c r="C32" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D32" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="3:4">
       <c r="C33" s="30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D33" t="s">
         <v>27</v>
@@ -3935,771 +3882,771 @@
     </row>
     <row r="34" spans="3:4">
       <c r="C34" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D34" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="35" spans="3:4">
       <c r="C35" s="30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D35" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="36" spans="3:4">
       <c r="C36" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D36" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="37" spans="3:4">
       <c r="C37" s="30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D37" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="3:4">
       <c r="C38" s="30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D38" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="39" spans="3:4">
       <c r="C39" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D39" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="40" spans="3:4">
       <c r="C40" s="30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D40" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="41" spans="3:4">
       <c r="C41" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D41" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="42" spans="3:4">
       <c r="C42" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D42" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="43" spans="3:4">
       <c r="C43" s="30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D43" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="44" spans="3:4">
       <c r="C44" s="30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D44" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="45" spans="3:4">
       <c r="C45" s="30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="46" spans="3:4">
       <c r="C46" s="30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D46" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="47" spans="3:4">
       <c r="C47" s="30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D47" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="48" spans="3:4">
       <c r="C48" s="30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D48" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49" spans="3:4">
       <c r="C49" s="30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D49" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="50" spans="3:4">
       <c r="C50" s="30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D50" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="51" spans="3:4">
       <c r="C51" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D51" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="52" spans="3:4">
       <c r="C52" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D52" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="53" spans="3:4">
       <c r="C53" s="30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D53" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="54" spans="3:4">
       <c r="C54" s="30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D54" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="55" spans="3:4">
       <c r="C55" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="56" spans="3:4">
       <c r="C56" s="30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D56" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="57" spans="3:4">
       <c r="C57" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D57" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="58" spans="3:4">
       <c r="C58" s="30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D58" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="59" spans="3:4">
       <c r="C59" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D59" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="60" spans="3:4">
       <c r="C60" s="30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D60" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="61" spans="3:4">
       <c r="C61" s="30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="62" spans="3:4">
       <c r="C62" s="30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D62" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="63" spans="3:4">
       <c r="C63" s="30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D63" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="64" spans="3:4">
       <c r="C64" s="30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D64" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="65" spans="3:4">
       <c r="C65" s="30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D65" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="66" spans="3:4">
       <c r="C66" s="30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D66" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="67" spans="3:4">
       <c r="C67" s="30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D67" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="68" spans="3:4">
       <c r="C68" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="69" spans="3:4">
       <c r="C69" s="30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="70" spans="3:4">
       <c r="C70" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="72" spans="3:4">
       <c r="C72" s="30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="74" spans="3:4">
       <c r="C74" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="75" spans="3:4">
       <c r="C75" s="30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="76" spans="3:4">
       <c r="C76" s="30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" spans="3:4">
       <c r="C77" s="30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="30" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="80" spans="3:4">
       <c r="C80" s="30" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="82" spans="3:3">
       <c r="C82" s="30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85" s="30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87" s="30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="88" spans="3:3">
       <c r="C88" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="90" spans="3:3">
       <c r="C90" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="91" spans="3:3">
       <c r="C91" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92" s="30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93" s="30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="94" spans="3:3">
       <c r="C94" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95" spans="3:3">
       <c r="C95" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="96" spans="3:3">
       <c r="C96" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="97" spans="3:3">
       <c r="C97" s="30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="98" spans="3:3">
       <c r="C98" s="30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="99" spans="3:3">
       <c r="C99" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="100" spans="3:3">
       <c r="C100" s="30" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="101" spans="3:3">
       <c r="C101" s="30" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="102" spans="3:3">
       <c r="C102" s="30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="103" spans="3:3">
       <c r="C103" s="30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="104" spans="3:3">
       <c r="C104" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="105" spans="3:3">
       <c r="C105" s="30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="106" spans="3:3">
       <c r="C106" s="30" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="107" spans="3:3">
       <c r="C107" s="30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="108" spans="3:3">
       <c r="C108" s="30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="109" spans="3:3">
       <c r="C109" s="30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="110" spans="3:3">
       <c r="C110" s="30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="111" spans="3:3">
       <c r="C111" s="30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="112" spans="3:3">
       <c r="C112" s="30" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="113" spans="3:3">
       <c r="C113" s="30" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="114" spans="3:3">
       <c r="C114" s="30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="115" spans="3:3">
       <c r="C115" s="30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="116" spans="3:3">
       <c r="C116" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="117" spans="3:3">
       <c r="C117" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="118" spans="3:3">
       <c r="C118" s="30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="119" spans="3:3">
       <c r="C119" s="30" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="120" spans="3:3">
       <c r="C120" s="30" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="121" spans="3:3">
       <c r="C121" s="30" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="122" spans="3:3">
       <c r="C122" s="30" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="123" spans="3:3">
       <c r="C123" s="30" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="124" spans="3:3">
       <c r="C124" s="30" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="125" spans="3:3">
       <c r="C125" s="30" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="126" spans="3:3">
       <c r="C126" s="30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="127" spans="3:3">
       <c r="C127" s="30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="128" spans="3:3">
       <c r="C128" s="30" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="129" spans="3:3">
       <c r="C129" s="30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="130" spans="3:3">
       <c r="C130" s="30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="131" spans="3:3">
       <c r="C131" s="30" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="132" spans="3:3">
       <c r="C132" s="30" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="133" spans="3:3">
       <c r="C133" s="30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="134" spans="3:3">
       <c r="C134" s="30" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
     </row>
     <row r="135" spans="3:3">
       <c r="C135" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="136" spans="3:3">
       <c r="C136" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="137" spans="3:3">
       <c r="C137" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="138" spans="3:3">
       <c r="C138" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="139" spans="3:3">
       <c r="C139" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="https://www.metrology.net/wiki/testprocess-measure-conductance/"/>
-    <hyperlink ref="C4" r:id="rId2" display="https://www.metrology.net/wiki/testprocess-measure-conductivity/"/>
-    <hyperlink ref="C5" r:id="rId3" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac/"/>
-    <hyperlink ref="C6" r:id="rId4" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-sinewave/"/>
-    <hyperlink ref="C7" r:id="rId5" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-squarewave/"/>
-    <hyperlink ref="C8" r:id="rId6" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-trianglewave/"/>
-    <hyperlink ref="C9" r:id="rId7" display="https://www.metrology.net/wiki/testprocess-measure-current-dc/"/>
-    <hyperlink ref="C10" r:id="rId8" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-gas/"/>
-    <hyperlink ref="C11" r:id="rId9" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-liquid/"/>
-    <hyperlink ref="C12" r:id="rId10" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-solid/"/>
-    <hyperlink ref="C13" r:id="rId11" display="https://www.metrology.net/wiki/testprocess-measure-force/"/>
-    <hyperlink ref="C14" r:id="rId12" display="https://www.metrology.net/wiki/testprocess-measure-frequency/"/>
-    <hyperlink ref="C15" r:id="rId13" display="https://www.metrology.net/wiki/testprocess-measure-frequency-amplitudemodulation-rate/"/>
-    <hyperlink ref="C16" r:id="rId14" display="https://www.metrology.net/wiki/testprocess-measure-frequency-frequencymodulation-deviation/"/>
-    <hyperlink ref="C17" r:id="rId15" display="https://www.metrology.net/wiki/testprocess-measure-frequency-frequencymodulation-rate/"/>
-    <hyperlink ref="C18" r:id="rId16" display="https://www.metrology.net/wiki/testprocess-measure-frequency-phasemodulation-rate/"/>
-    <hyperlink ref="C19" r:id="rId17" display="https://www.metrology.net/wiki/testprocess-measure-humidity-absolute/"/>
-    <hyperlink ref="C21" r:id="rId18" display="https://www.metrology.net/wiki/testprocess-measure-impedance/"/>
-    <hyperlink ref="C22" r:id="rId19" display="https://www.metrology.net/wiki/testprocess-measure-inductance/"/>
-    <hyperlink ref="C23" r:id="rId20" display="https://www.metrology.net/wiki/testprocess-measure-length/"/>
-    <hyperlink ref="C24" r:id="rId21" display="https://www.metrology.net/wiki/testprocess-measure-length-circumference/"/>
-    <hyperlink ref="C25" r:id="rId22" display="https://www.metrology.net/wiki/testprocess-measure-length-diameter/"/>
-    <hyperlink ref="C26" r:id="rId23" display="https://www.metrology.net/wiki/testprocess-measure-length-form-flatness/"/>
-    <hyperlink ref="C27" r:id="rId24" display="https://www.metrology.net/wiki/testprocess-measure-length-form-parallelism/"/>
-    <hyperlink ref="C28" r:id="rId25" display="https://www.metrology.net/wiki/testprocess-measure-length-form-perpendicularity/"/>
-    <hyperlink ref="C29" r:id="rId26" display="https://www.metrology.net/wiki/testprocess-measure-length-form-roughness/"/>
-    <hyperlink ref="C30" r:id="rId27" display="https://www.metrology.net/wiki/testprocess-measure-length-form-roundness/"/>
-    <hyperlink ref="C31" r:id="rId28" display="https://www.metrology.net/wiki/testprocess-measure-length-form-sphericity/"/>
-    <hyperlink ref="C32" r:id="rId29" display="https://www.metrology.net/wiki/testprocess-measure-length-form-straightness-axis/"/>
-    <hyperlink ref="C33" r:id="rId30" display="https://www.metrology.net/wiki/testprocess-measure-length-form-straightness-surface/"/>
-    <hyperlink ref="C34" r:id="rId31" display="https://www.metrology.net/wiki/testprocess-measure-length-radius/"/>
-    <hyperlink ref="C35" r:id="rId32" display="https://www.metrology.net/wiki/testprocess-measure-mass-apparent/"/>
-    <hyperlink ref="C36" r:id="rId33" display="https://www.metrology.net/wiki/testprocess-measure-mass-conventional/"/>
-    <hyperlink ref="C37" r:id="rId34" display="https://www.metrology.net/wiki/testprocess-measure-mass-true/"/>
-    <hyperlink ref="C38" r:id="rId35" display="https://www.metrology.net/wiki/testprocess-measure-phase-phasemodulation/"/>
-    <hyperlink ref="C39" r:id="rId36" display="https://www.metrology.net/wiki/testprocess-measure-phase-reflectioncoefficent-rf/"/>
-    <hyperlink ref="C40" r:id="rId37" display="https://www.metrology.net/wiki/testprocess-measure-phase-reflectioncoefficent/"/>
-    <hyperlink ref="C41" r:id="rId38" display="https://www.metrology.net/wiki/testprocess-measure-phasenoise-sideband/"/>
-    <hyperlink ref="C42" r:id="rId39" display="https://www.metrology.net/wiki/testprocess-measure-power-rf-sinewave/"/>
-    <hyperlink ref="C43" r:id="rId40" display="https://www.metrology.net/wiki/testprocess-measure-pressure-hydraulic-static/"/>
-    <hyperlink ref="C44" r:id="rId41" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-absolute-static/"/>
-    <hyperlink ref="C45" r:id="rId42" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-differential-static/"/>
-    <hyperlink ref="C46" r:id="rId43" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-gage-static/"/>
-    <hyperlink ref="C47" r:id="rId44" display="https://www.metrology.net/wiki/testprocess-measure-ratio-amplitudemodulation/"/>
-    <hyperlink ref="C48" r:id="rId45" display="https://www.metrology.net/wiki/testprocess-measure-ratio-density-mass/"/>
-    <hyperlink ref="C49" r:id="rId46" display="https://www.metrology.net/wiki/testprocess-measure-ratio-humidity-relative/"/>
-    <hyperlink ref="C50" r:id="rId47" display="https://www.metrology.net/wiki/testprocess-measure-ratio-humidity-specific/"/>
-    <hyperlink ref="C51" r:id="rId48" display="https://www.metrology.net/wiki/testprocess-measure-ratio-reflectioncoefficent-rf/"/>
-    <hyperlink ref="C52" r:id="rId49" display="https://www.metrology.net/wiki/testprocess-measure-ratio-power-rf-sinewave-delta-frequency/"/>
-    <hyperlink ref="C53" r:id="rId50" display="https://www.metrology.net/wiki/testprocess-measure-ratio-power-rf-sinewave-delta-power/"/>
-    <hyperlink ref="C54" r:id="rId51" display="https://www.metrology.net/wiki/testprocess-measure-ratio-transmissioncoefficent/"/>
-    <hyperlink ref="C55" r:id="rId52" display="https://www.metrology.net/wiki/testprocess-measure-ratio-torque/"/>
-    <hyperlink ref="C56" r:id="rId53" display="https://www.metrology.net/wiki/testprocess-measure-ratio-voltage-ac-ripple-ondc/"/>
-    <hyperlink ref="C57" r:id="rId54" display="https://www.metrology.net/wiki/testprocess-measure-ratio-voltage-ac-sinewave-delta-frequency/"/>
-    <hyperlink ref="C58" r:id="rId55" display="https://www.metrology.net/wiki/testprocess-measure-ratio-volts-ac-sinewave-delta-volts/"/>
-    <hyperlink ref="C59" r:id="rId56" display="https://www.metrology.net/wiki/testprocess-measure-ohms/"/>
-    <hyperlink ref="C60" r:id="rId57" display="https://www.metrology.net/wiki/testprocess-measure-temperature/"/>
-    <hyperlink ref="C61" r:id="rId58" display="https://www.metrology.net/wiki/testprocess-measure-temperature-radiometric/"/>
-    <hyperlink ref="C62" r:id="rId59" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-prt/"/>
-    <hyperlink ref="C63" r:id="rId60" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-rtd/"/>
-    <hyperlink ref="C64" r:id="rId61" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-thermocouple/"/>
-    <hyperlink ref="C65" r:id="rId62" display="https://www.metrology.net/wiki/testprocess-measure-time-pulsetransition/"/>
-    <hyperlink ref="C66" r:id="rId63" display="https://www.metrology.net/wiki/testprocess-measure-time-absolute/"/>
-    <hyperlink ref="C67" r:id="rId64" display="https://www.metrology.net/wiki/testprocess-measure-torque/"/>
-    <hyperlink ref="C68" r:id="rId65" display="https://www.metrology.net/wiki/testprocess-measure-torque-hydraulicpressure/"/>
-    <hyperlink ref="C69" r:id="rId66" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac/"/>
-    <hyperlink ref="C70" r:id="rId67" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-noise-ondc/"/>
-    <hyperlink ref="C71" r:id="rId68" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-sinewave/"/>
-    <hyperlink ref="C72" r:id="rId69" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-squarewave/"/>
-    <hyperlink ref="C73" r:id="rId70" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-trianglewave/"/>
-    <hyperlink ref="C74" r:id="rId71" display="https://www.metrology.net/wiki/testprocess-measure-voltage-dc/"/>
-    <hyperlink ref="C75" r:id="rId72" display="https://www.metrology.net/wiki/testprocess-measure-weight/"/>
-    <hyperlink ref="C76" r:id="rId73" display="https://www.metrology.net/wiki/testprocess-source-capacitance/"/>
-    <hyperlink ref="C77" r:id="rId74" display="https://www.metrology.net/wiki/testprocess-source-conductance/"/>
-    <hyperlink ref="C78" r:id="rId75" display="https://www.metrology.net/wiki/testprocess-source-conductivity/"/>
-    <hyperlink ref="C79" r:id="rId76" display="https://www.metrology.net/wiki/testprocess-source-current-ac-sinewave/"/>
-    <hyperlink ref="C80" r:id="rId77" display="https://www.metrology.net/wiki/testprocess-source-current-ac-squarewave/"/>
-    <hyperlink ref="C81" r:id="rId78" display="https://www.metrology.net/wiki/testprocess-source-current-ac-triangle/"/>
-    <hyperlink ref="C82" r:id="rId79" display="https://www.metrology.net/wiki/testprocess-source-current-dc/"/>
-    <hyperlink ref="C83" r:id="rId80" display="https://www.metrology.net/wiki/testprocess-source-density-mass-gas/"/>
-    <hyperlink ref="C84" r:id="rId81" display="https://www.metrology.net/wiki/testprocess-source-density-mass-liquid/"/>
-    <hyperlink ref="C85" r:id="rId82" display="https://www.metrology.net/wiki/testprocess-source-density-mass-solid/"/>
-    <hyperlink ref="C86" r:id="rId83" display="https://www.metrology.net/wiki/testprocess-source-force/"/>
-    <hyperlink ref="C87" r:id="rId84" display="https://www.metrology.net/wiki/testprocess-source-frequency-ac-squarewave/"/>
-    <hyperlink ref="C88" r:id="rId85" display="https://www.metrology.net/wiki/testprocess-source-frequency-arbitrary-cardiograph/"/>
-    <hyperlink ref="C89" r:id="rId86" display="https://www.metrology.net/wiki/testprocess-source-humidity-absolute/"/>
-    <hyperlink ref="C90" r:id="rId87" display="https://www.metrology.net/wiki/testprocess-source-impedance/"/>
-    <hyperlink ref="C91" r:id="rId88" display="https://www.metrology.net/wiki/testprocess-source-inductance/"/>
-    <hyperlink ref="C92" r:id="rId89" display="https://www.metrology.net/wiki/testprocess-source-length/"/>
-    <hyperlink ref="C93" r:id="rId90" display="https://www.metrology.net/wiki/testprocess-source-length-circumference/"/>
-    <hyperlink ref="C94" r:id="rId91" display="https://www.metrology.net/wiki/testprocess-source-length-diameter/"/>
-    <hyperlink ref="C95" r:id="rId92" display="https://www.metrology.net/wiki/testprocess-source-length-form-perpendicularity/"/>
-    <hyperlink ref="C96" r:id="rId93" display="https://www.metrology.net/wiki/testprocess-source-length-form-roundness/"/>
-    <hyperlink ref="C97" r:id="rId94" display="https://www.metrology.net/wiki/testprocess-source-length-form-sphericity/"/>
-    <hyperlink ref="C98" r:id="rId95" display="https://www.metrology.net/wiki/testprocess-source-length-form-straightness-surrface/"/>
-    <hyperlink ref="C99" r:id="rId96" display="https://www.metrology.net/wiki/testprocess-source-length-radius/"/>
-    <hyperlink ref="C100" r:id="rId97" display="https://www.metrology.net/wiki/testprocess-source-mass-apparent/"/>
-    <hyperlink ref="C101" r:id="rId98" display="https://www.metrology.net/wiki/testprocess-source-mass-conventional/"/>
-    <hyperlink ref="C102" r:id="rId99" display="https://www.metrology.net/wiki/testprocess-source-mass-true/"/>
-    <hyperlink ref="C103" r:id="rId100" display="https://www.metrology.net/wiki/testprocess-source-period-marker/"/>
-    <hyperlink ref="C104" r:id="rId101" display="https://www.metrology.net/wiki/testprocess-source-period-squarewave/"/>
-    <hyperlink ref="C105" r:id="rId102" display="https://www.metrology.net/wiki/testprocess-source-power-ac-sinewave/"/>
-    <hyperlink ref="C106" r:id="rId103" display="https://www.metrology.net/wiki/testprocess-source-power-ac-sinewave-simulated/"/>
-    <hyperlink ref="C107" r:id="rId104" display="https://www.metrology.net/wiki/testprocess-source-power-dc-simulated/"/>
-    <hyperlink ref="C108" r:id="rId105" display="https://www.metrology.net/wiki/testprocess-source-power-noise-terminated/"/>
-    <hyperlink ref="C109" r:id="rId106" display="https://www.metrology.net/wiki/testprocess-source-power-rf-sinewave/"/>
-    <hyperlink ref="C110" r:id="rId107" display="https://www.metrology.net/wiki/testprocess-source-pressure-hydraulic-static/"/>
-    <hyperlink ref="C111" r:id="rId108" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-absolute-static/"/>
-    <hyperlink ref="C112" r:id="rId109" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-differential-static/"/>
-    <hyperlink ref="C113" r:id="rId110" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-gage-static/"/>
-    <hyperlink ref="C114" r:id="rId111" display="https://www.metrology.net/wiki/testprocess-source-ratio-amplitudemodulation/"/>
-    <hyperlink ref="C115" r:id="rId112" display="https://www.metrology.net/wiki/testprocess-source-ratio-humidity-relative/"/>
-    <hyperlink ref="C116" r:id="rId113" display="https://www.metrology.net/wiki/testprocess-source-ratio-humidity-specific/"/>
-    <hyperlink ref="C117" r:id="rId114" display="https://www.metrology.net/wiki/testprocess-source-ratio-rf-sinusoidal-delta-frequency/"/>
-    <hyperlink ref="C118" r:id="rId115" display="https://www.metrology.net/wiki/source-voltage-ac-sinewave-delta-frequency/"/>
-    <hyperlink ref="C119" r:id="rId116" display="https://www.metrology.net/wiki/testprocess-source-voltage-ac-sinewave-delta-voltage/"/>
-    <hyperlink ref="C120" r:id="rId117" display="https://www.metrology.net/wiki/testprocess-source-resistance/"/>
-    <hyperlink ref="C121" r:id="rId118" display="https://www.metrology.net/wiki/testprocess-source-temperature/"/>
-    <hyperlink ref="C122" r:id="rId119" display="https://www.metrology.net/wiki/testprocess-source-temperature-fixedpoint/"/>
-    <hyperlink ref="C123" r:id="rId120" display="https://www.metrology.net/wiki/testprocess-source-temperature-radiometric/"/>
-    <hyperlink ref="C124" r:id="rId121" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-prt/"/>
-    <hyperlink ref="C125" r:id="rId122" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-rtd/"/>
-    <hyperlink ref="C126" r:id="rId123" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-thermocouple/"/>
-    <hyperlink ref="C127" r:id="rId124" display="https://www.metrology.net/wiki/source-time-marker/"/>
-    <hyperlink ref="C128" r:id="rId125" display="https://www.metrology.net/wiki/testprocess-source-torque/"/>
-    <hyperlink ref="C129" r:id="rId126" display="https://www.metrology.net/wiki/source-voltage-ac-sinewave/"/>
-    <hyperlink ref="C130" r:id="rId127" display="https://www.metrology.net/wiki/testprocess-source-voltage-dc/"/>
-    <hyperlink ref="C131" r:id="rId128" display="https://www.metrology.net/wiki/source-voltage-dc-delta/"/>
-    <hyperlink ref="C132" r:id="rId129" display="https://www.metrology.net/wiki/testprocess-source-voltage-noise-terminated/"/>
-    <hyperlink ref="C133" r:id="rId130" display="https://www.metrology.net/wiki/testprocess-source-voltage-shorted/"/>
-    <hyperlink ref="C134" r:id="rId131" display="https://www.metrology.net/wiki/testprocess-source-weight/"/>
-    <hyperlink ref="C20" r:id="rId132" display="https://www.metrology.net/wiki/testprocess-measure-humidity-absolute/"/>
+    <hyperlink ref="C3" r:id="rId1" display="https://www.metrology.net/wiki/testprocess-measure-conductance/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" display="https://www.metrology.net/wiki/testprocess-measure-conductivity/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId3" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac/" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C6" r:id="rId4" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C7" r:id="rId5" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-squarewave/" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C8" r:id="rId6" display="https://www.metrology.net/wiki/testprocess-measure-amps-ac-trianglewave/" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C9" r:id="rId7" display="https://www.metrology.net/wiki/testprocess-measure-current-dc/" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C10" r:id="rId8" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-gas/" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C11" r:id="rId9" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-liquid/" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C12" r:id="rId10" display="https://www.metrology.net/wiki/testprocess-measure-density-mass-solid/" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C13" r:id="rId11" display="https://www.metrology.net/wiki/testprocess-measure-force/" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C14" r:id="rId12" display="https://www.metrology.net/wiki/testprocess-measure-frequency/" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C15" r:id="rId13" display="https://www.metrology.net/wiki/testprocess-measure-frequency-amplitudemodulation-rate/" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C16" r:id="rId14" display="https://www.metrology.net/wiki/testprocess-measure-frequency-frequencymodulation-deviation/" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C17" r:id="rId15" display="https://www.metrology.net/wiki/testprocess-measure-frequency-frequencymodulation-rate/" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C18" r:id="rId16" display="https://www.metrology.net/wiki/testprocess-measure-frequency-phasemodulation-rate/" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C19" r:id="rId17" display="https://www.metrology.net/wiki/testprocess-measure-humidity-absolute/" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C21" r:id="rId18" display="https://www.metrology.net/wiki/testprocess-measure-impedance/" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C22" r:id="rId19" display="https://www.metrology.net/wiki/testprocess-measure-inductance/" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C23" r:id="rId20" display="https://www.metrology.net/wiki/testprocess-measure-length/" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C24" r:id="rId21" display="https://www.metrology.net/wiki/testprocess-measure-length-circumference/" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C25" r:id="rId22" display="https://www.metrology.net/wiki/testprocess-measure-length-diameter/" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C26" r:id="rId23" display="https://www.metrology.net/wiki/testprocess-measure-length-form-flatness/" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C27" r:id="rId24" display="https://www.metrology.net/wiki/testprocess-measure-length-form-parallelism/" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C28" r:id="rId25" display="https://www.metrology.net/wiki/testprocess-measure-length-form-perpendicularity/" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C29" r:id="rId26" display="https://www.metrology.net/wiki/testprocess-measure-length-form-roughness/" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C30" r:id="rId27" display="https://www.metrology.net/wiki/testprocess-measure-length-form-roundness/" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C31" r:id="rId28" display="https://www.metrology.net/wiki/testprocess-measure-length-form-sphericity/" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C32" r:id="rId29" display="https://www.metrology.net/wiki/testprocess-measure-length-form-straightness-axis/" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C33" r:id="rId30" display="https://www.metrology.net/wiki/testprocess-measure-length-form-straightness-surface/" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C34" r:id="rId31" display="https://www.metrology.net/wiki/testprocess-measure-length-radius/" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C35" r:id="rId32" display="https://www.metrology.net/wiki/testprocess-measure-mass-apparent/" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C36" r:id="rId33" display="https://www.metrology.net/wiki/testprocess-measure-mass-conventional/" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C37" r:id="rId34" display="https://www.metrology.net/wiki/testprocess-measure-mass-true/" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C38" r:id="rId35" display="https://www.metrology.net/wiki/testprocess-measure-phase-phasemodulation/" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C39" r:id="rId36" display="https://www.metrology.net/wiki/testprocess-measure-phase-reflectioncoefficent-rf/" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C40" r:id="rId37" display="https://www.metrology.net/wiki/testprocess-measure-phase-reflectioncoefficent/" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C41" r:id="rId38" display="https://www.metrology.net/wiki/testprocess-measure-phasenoise-sideband/" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C42" r:id="rId39" display="https://www.metrology.net/wiki/testprocess-measure-power-rf-sinewave/" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="C43" r:id="rId40" display="https://www.metrology.net/wiki/testprocess-measure-pressure-hydraulic-static/" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C44" r:id="rId41" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-absolute-static/" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="C45" r:id="rId42" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-differential-static/" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C46" r:id="rId43" display="https://www.metrology.net/wiki/testprocess-measure-pressure-pneumatic-gage-static/" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C47" r:id="rId44" display="https://www.metrology.net/wiki/testprocess-measure-ratio-amplitudemodulation/" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C48" r:id="rId45" display="https://www.metrology.net/wiki/testprocess-measure-ratio-density-mass/" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C49" r:id="rId46" display="https://www.metrology.net/wiki/testprocess-measure-ratio-humidity-relative/" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C50" r:id="rId47" display="https://www.metrology.net/wiki/testprocess-measure-ratio-humidity-specific/" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C51" r:id="rId48" display="https://www.metrology.net/wiki/testprocess-measure-ratio-reflectioncoefficent-rf/" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="C52" r:id="rId49" display="https://www.metrology.net/wiki/testprocess-measure-ratio-power-rf-sinewave-delta-frequency/" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="C53" r:id="rId50" display="https://www.metrology.net/wiki/testprocess-measure-ratio-power-rf-sinewave-delta-power/" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="C54" r:id="rId51" display="https://www.metrology.net/wiki/testprocess-measure-ratio-transmissioncoefficent/" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C55" r:id="rId52" display="https://www.metrology.net/wiki/testprocess-measure-ratio-torque/" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="C56" r:id="rId53" display="https://www.metrology.net/wiki/testprocess-measure-ratio-voltage-ac-ripple-ondc/" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="C57" r:id="rId54" display="https://www.metrology.net/wiki/testprocess-measure-ratio-voltage-ac-sinewave-delta-frequency/" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="C58" r:id="rId55" display="https://www.metrology.net/wiki/testprocess-measure-ratio-volts-ac-sinewave-delta-volts/" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="C59" r:id="rId56" display="https://www.metrology.net/wiki/testprocess-measure-ohms/" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="C60" r:id="rId57" display="https://www.metrology.net/wiki/testprocess-measure-temperature/" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="C61" r:id="rId58" display="https://www.metrology.net/wiki/testprocess-measure-temperature-radiometric/" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="C62" r:id="rId59" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-prt/" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="C63" r:id="rId60" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-rtd/" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="C64" r:id="rId61" display="https://www.metrology.net/wiki/testprocess-measure-temperature-simulated-thermocouple/" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="C65" r:id="rId62" display="https://www.metrology.net/wiki/testprocess-measure-time-pulsetransition/" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="C66" r:id="rId63" display="https://www.metrology.net/wiki/testprocess-measure-time-absolute/" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="C67" r:id="rId64" display="https://www.metrology.net/wiki/testprocess-measure-torque/" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="C68" r:id="rId65" display="https://www.metrology.net/wiki/testprocess-measure-torque-hydraulicpressure/" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="C69" r:id="rId66" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac/" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="C70" r:id="rId67" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-noise-ondc/" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="C71" r:id="rId68" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="C72" r:id="rId69" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-squarewave/" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="C73" r:id="rId70" display="https://www.metrology.net/wiki/testprocess-measure-voltage-ac-trianglewave/" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="C74" r:id="rId71" display="https://www.metrology.net/wiki/testprocess-measure-voltage-dc/" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="C75" r:id="rId72" display="https://www.metrology.net/wiki/testprocess-measure-weight/" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="C76" r:id="rId73" display="https://www.metrology.net/wiki/testprocess-source-capacitance/" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="C77" r:id="rId74" display="https://www.metrology.net/wiki/testprocess-source-conductance/" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="C78" r:id="rId75" display="https://www.metrology.net/wiki/testprocess-source-conductivity/" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="C79" r:id="rId76" display="https://www.metrology.net/wiki/testprocess-source-current-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="C80" r:id="rId77" display="https://www.metrology.net/wiki/testprocess-source-current-ac-squarewave/" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="C81" r:id="rId78" display="https://www.metrology.net/wiki/testprocess-source-current-ac-triangle/" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="C82" r:id="rId79" display="https://www.metrology.net/wiki/testprocess-source-current-dc/" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="C83" r:id="rId80" display="https://www.metrology.net/wiki/testprocess-source-density-mass-gas/" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="C84" r:id="rId81" display="https://www.metrology.net/wiki/testprocess-source-density-mass-liquid/" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="C85" r:id="rId82" display="https://www.metrology.net/wiki/testprocess-source-density-mass-solid/" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="C86" r:id="rId83" display="https://www.metrology.net/wiki/testprocess-source-force/" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="C87" r:id="rId84" display="https://www.metrology.net/wiki/testprocess-source-frequency-ac-squarewave/" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="C88" r:id="rId85" display="https://www.metrology.net/wiki/testprocess-source-frequency-arbitrary-cardiograph/" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="C89" r:id="rId86" display="https://www.metrology.net/wiki/testprocess-source-humidity-absolute/" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="C90" r:id="rId87" display="https://www.metrology.net/wiki/testprocess-source-impedance/" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="C91" r:id="rId88" display="https://www.metrology.net/wiki/testprocess-source-inductance/" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="C92" r:id="rId89" display="https://www.metrology.net/wiki/testprocess-source-length/" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="C93" r:id="rId90" display="https://www.metrology.net/wiki/testprocess-source-length-circumference/" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="C94" r:id="rId91" display="https://www.metrology.net/wiki/testprocess-source-length-diameter/" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="C95" r:id="rId92" display="https://www.metrology.net/wiki/testprocess-source-length-form-perpendicularity/" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="C96" r:id="rId93" display="https://www.metrology.net/wiki/testprocess-source-length-form-roundness/" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="C97" r:id="rId94" display="https://www.metrology.net/wiki/testprocess-source-length-form-sphericity/" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="C98" r:id="rId95" display="https://www.metrology.net/wiki/testprocess-source-length-form-straightness-surrface/" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="C99" r:id="rId96" display="https://www.metrology.net/wiki/testprocess-source-length-radius/" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="C100" r:id="rId97" display="https://www.metrology.net/wiki/testprocess-source-mass-apparent/" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="C101" r:id="rId98" display="https://www.metrology.net/wiki/testprocess-source-mass-conventional/" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="C102" r:id="rId99" display="https://www.metrology.net/wiki/testprocess-source-mass-true/" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="C103" r:id="rId100" display="https://www.metrology.net/wiki/testprocess-source-period-marker/" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="C104" r:id="rId101" display="https://www.metrology.net/wiki/testprocess-source-period-squarewave/" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="C105" r:id="rId102" display="https://www.metrology.net/wiki/testprocess-source-power-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="C106" r:id="rId103" display="https://www.metrology.net/wiki/testprocess-source-power-ac-sinewave-simulated/" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="C107" r:id="rId104" display="https://www.metrology.net/wiki/testprocess-source-power-dc-simulated/" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="C108" r:id="rId105" display="https://www.metrology.net/wiki/testprocess-source-power-noise-terminated/" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="C109" r:id="rId106" display="https://www.metrology.net/wiki/testprocess-source-power-rf-sinewave/" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="C110" r:id="rId107" display="https://www.metrology.net/wiki/testprocess-source-pressure-hydraulic-static/" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="C111" r:id="rId108" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-absolute-static/" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="C112" r:id="rId109" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-differential-static/" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="C113" r:id="rId110" display="https://www.metrology.net/wiki/testprocess-source-pressure-pneumatic-gage-static/" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="C114" r:id="rId111" display="https://www.metrology.net/wiki/testprocess-source-ratio-amplitudemodulation/" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="C115" r:id="rId112" display="https://www.metrology.net/wiki/testprocess-source-ratio-humidity-relative/" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="C116" r:id="rId113" display="https://www.metrology.net/wiki/testprocess-source-ratio-humidity-specific/" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="C117" r:id="rId114" display="https://www.metrology.net/wiki/testprocess-source-ratio-rf-sinusoidal-delta-frequency/" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="C118" r:id="rId115" display="https://www.metrology.net/wiki/source-voltage-ac-sinewave-delta-frequency/" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="C119" r:id="rId116" display="https://www.metrology.net/wiki/testprocess-source-voltage-ac-sinewave-delta-voltage/" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="C120" r:id="rId117" display="https://www.metrology.net/wiki/testprocess-source-resistance/" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="C121" r:id="rId118" display="https://www.metrology.net/wiki/testprocess-source-temperature/" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="C122" r:id="rId119" display="https://www.metrology.net/wiki/testprocess-source-temperature-fixedpoint/" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="C123" r:id="rId120" display="https://www.metrology.net/wiki/testprocess-source-temperature-radiometric/" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="C124" r:id="rId121" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-prt/" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="C125" r:id="rId122" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-rtd/" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="C126" r:id="rId123" display="https://www.metrology.net/wiki/testprocess-source-temperature-simulated-thermocouple/" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="C127" r:id="rId124" display="https://www.metrology.net/wiki/source-time-marker/" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="C128" r:id="rId125" display="https://www.metrology.net/wiki/testprocess-source-torque/" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="C129" r:id="rId126" display="https://www.metrology.net/wiki/source-voltage-ac-sinewave/" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="C130" r:id="rId127" display="https://www.metrology.net/wiki/testprocess-source-voltage-dc/" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="C131" r:id="rId128" display="https://www.metrology.net/wiki/source-voltage-dc-delta/" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="C132" r:id="rId129" display="https://www.metrology.net/wiki/testprocess-source-voltage-noise-terminated/" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="C133" r:id="rId130" display="https://www.metrology.net/wiki/testprocess-source-voltage-shorted/" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="C134" r:id="rId131" display="https://www.metrology.net/wiki/testprocess-source-weight/" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="C20" r:id="rId132" display="https://www.metrology.net/wiki/testprocess-measure-humidity-absolute/" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId133"/>
@@ -4707,561 +4654,540 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A2:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P46" sqref="P46"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
-    <col min="6" max="7" width="21.6640625" customWidth="1"/>
-    <col min="8" max="8" width="25.33203125" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" customWidth="1"/>
-    <col min="13" max="13" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="N1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" ht="43.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>529</v>
       </c>
       <c r="B2" t="s">
-        <v>375</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>383</v>
-      </c>
-      <c r="E2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C3" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>520</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>530</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>521</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>522</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>523</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>524</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>367</v>
+      </c>
+      <c r="B11" t="s">
+        <v>310</v>
+      </c>
+      <c r="C11" t="s">
         <v>69</v>
       </c>
-      <c r="F2" t="s">
-        <v>381</v>
-      </c>
-      <c r="H2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2">
-        <v>9218</v>
-      </c>
-      <c r="K2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" t="s">
-        <v>376</v>
-      </c>
-      <c r="C3" t="s">
-        <v>382</v>
-      </c>
-      <c r="E3" t="s">
-        <v>379</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3">
-        <v>2970</v>
-      </c>
-      <c r="K3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" t="s">
-        <v>378</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>525</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>526</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B13" r:id="rId1" display="www.dfm.dk" xr:uid="{3BB2CF1F-FE9A-4CBB-BF1E-27B2EBB8D33F}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{B9461125-82C7-4F93-9F8D-F76525FEFD1F}"/>
+    <hyperlink ref="B14" r:id="rId3" xr:uid="{8DCFB803-FEC4-46C5-AD28-84133941B376}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{B3E71855-D1B6-45BA-A530-2035E91DF7FE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00544486-CB0D-4F43-A82E-E46C84ABB3B9}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>529</v>
+        <v>513</v>
       </c>
       <c r="C2" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="B3" t="s">
-        <v>530</v>
+        <v>514</v>
       </c>
       <c r="C3" t="s">
         <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>531</v>
+        <v>515</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>442</v>
+        <v>426</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="B5" t="s">
-        <v>532</v>
+        <v>516</v>
       </c>
       <c r="C5" s="27" t="s">
         <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="B6" t="s">
-        <v>533</v>
+        <v>517</v>
       </c>
       <c r="C6" s="27" t="s">
         <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="B7" t="s">
-        <v>534</v>
+        <v>518</v>
       </c>
       <c r="C7" s="27" t="s">
         <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="B8" t="s">
-        <v>535</v>
+        <v>519</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="B9" t="s">
+        <v>316</v>
+      </c>
+      <c r="C9" s="27" t="s">
         <v>317</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="D9" t="s">
         <v>318</v>
-      </c>
-      <c r="D9" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="B10" t="s">
+        <v>312</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>314</v>
+      </c>
+      <c r="D10" t="s">
         <v>313</v>
       </c>
-      <c r="C10" s="31" t="s">
-        <v>315</v>
-      </c>
-      <c r="D10" t="s">
-        <v>314</v>
-      </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="B11" s="45" t="s">
-        <v>509</v>
+      <c r="B11" s="44" t="s">
+        <v>493</v>
       </c>
       <c r="C11" t="s">
         <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="B12" s="45" t="s">
-        <v>510</v>
+      <c r="B12" s="44" t="s">
+        <v>494</v>
       </c>
       <c r="C12" s="28" t="s">
         <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="B13" s="45" t="s">
-        <v>511</v>
+      <c r="B13" s="44" t="s">
+        <v>495</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="B14" s="45" t="s">
-        <v>512</v>
+      <c r="B14" s="44" t="s">
+        <v>496</v>
       </c>
       <c r="C14" t="s">
         <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="B15" s="45" t="s">
-        <v>513</v>
+      <c r="B15" s="44" t="s">
+        <v>497</v>
       </c>
       <c r="C15" t="s">
         <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="B16" s="45" t="s">
-        <v>514</v>
+      <c r="B16" s="44" t="s">
+        <v>498</v>
       </c>
       <c r="C16" s="27" t="s">
         <v>61</v>
       </c>
       <c r="D16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="44" t="s">
+        <v>499</v>
+      </c>
+      <c r="C17" t="s">
+        <v>310</v>
+      </c>
+      <c r="D17" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="45" t="s">
-        <v>515</v>
-      </c>
-      <c r="C17" t="s">
-        <v>311</v>
-      </c>
-      <c r="D17" t="s">
-        <v>91</v>
-      </c>
-    </row>
     <row r="18" spans="2:4">
-      <c r="B18" s="45" t="s">
-        <v>516</v>
+      <c r="B18" s="44" t="s">
+        <v>500</v>
       </c>
       <c r="C18" s="29" t="s">
         <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" s="45" t="s">
-        <v>517</v>
+      <c r="B19" s="44" t="s">
+        <v>501</v>
       </c>
       <c r="C19" s="28" t="s">
         <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" s="45" t="s">
-        <v>518</v>
+      <c r="B20" s="44" t="s">
+        <v>502</v>
       </c>
       <c r="C20" s="27" t="s">
         <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" s="46" t="s">
-        <v>519</v>
+      <c r="B21" s="45" t="s">
+        <v>503</v>
       </c>
       <c r="C21" t="s">
         <v>65</v>
       </c>
       <c r="D21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:4">
-      <c r="B22" s="46" t="s">
-        <v>520</v>
+      <c r="B22" s="45" t="s">
+        <v>504</v>
       </c>
       <c r="C22" t="s">
         <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="23" spans="2:4">
-      <c r="B23" s="46" t="s">
-        <v>521</v>
+      <c r="B23" s="45" t="s">
+        <v>505</v>
       </c>
       <c r="C23" s="28" t="s">
         <v>66</v>
       </c>
       <c r="D23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="2:4">
-      <c r="B24" s="46" t="s">
-        <v>522</v>
+      <c r="B24" s="45" t="s">
+        <v>506</v>
       </c>
       <c r="C24" s="40" t="s">
-        <v>432</v>
+        <v>416</v>
       </c>
       <c r="D24" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
     </row>
     <row r="25" spans="2:4">
-      <c r="B25" s="46" t="s">
-        <v>523</v>
+      <c r="B25" s="45" t="s">
+        <v>507</v>
       </c>
       <c r="C25" s="27" t="s">
         <v>67</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="2:4">
-      <c r="B26" s="46" t="s">
-        <v>524</v>
+      <c r="B26" s="45" t="s">
+        <v>508</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="2:4">
-      <c r="B27" s="46" t="s">
-        <v>525</v>
+      <c r="B27" s="45" t="s">
+        <v>509</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>68</v>
       </c>
       <c r="D27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="2:4">
-      <c r="B28" s="46" t="s">
-        <v>526</v>
+      <c r="B28" s="45" t="s">
+        <v>510</v>
       </c>
       <c r="C28" t="s">
         <v>69</v>
       </c>
       <c r="D28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="2:4">
-      <c r="B29" s="46" t="s">
-        <v>527</v>
+      <c r="B29" s="45" t="s">
+        <v>511</v>
       </c>
       <c r="C29" s="27" t="s">
         <v>70</v>
       </c>
       <c r="D29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="2:4">
-      <c r="B30" s="46" t="s">
-        <v>528</v>
+      <c r="B30" s="45" t="s">
+        <v>512</v>
       </c>
       <c r="C30" s="27"/>
       <c r="D30" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
     </row>
     <row r="31" spans="2:4">
-      <c r="B31" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" t="s">
-        <v>408</v>
-      </c>
+      <c r="B31" s="3"/>
     </row>
     <row r="32" spans="2:4">
-      <c r="B32" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="C32" t="s">
-        <v>60</v>
-      </c>
+      <c r="B32" s="3"/>
     </row>
     <row r="33" spans="2:3">
-      <c r="B33" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="C33" t="s">
-        <v>320</v>
-      </c>
+      <c r="B33" s="3"/>
     </row>
     <row r="34" spans="2:3">
-      <c r="B34" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="C34">
-        <v>255</v>
-      </c>
+      <c r="B34" s="3"/>
     </row>
     <row r="35" spans="2:3">
-      <c r="B35" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="C35">
-        <v>17025</v>
-      </c>
+      <c r="B35" s="3"/>
     </row>
     <row r="36" spans="2:3">
-      <c r="B36" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
+      <c r="B36" s="3"/>
     </row>
     <row r="38" spans="2:3">
       <c r="C38" s="27"/>
@@ -5289,56 +5215,56 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C18" r:id="rId1" display="www.dfm.dk"/>
-    <hyperlink ref="C12" r:id="rId2"/>
-    <hyperlink ref="C19" r:id="rId3"/>
-    <hyperlink ref="C23" r:id="rId4"/>
+    <hyperlink ref="C18" r:id="rId1" display="www.dfm.dk" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C12" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="C19" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C23" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="56.33203125" style="33" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="68.109375" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="56.28515625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="68.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>438</v>
+        <v>422</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
       <c r="H1" s="3"/>
     </row>
@@ -5346,183 +5272,183 @@
       <c r="B2" s="36"/>
       <c r="G2" s="33"/>
     </row>
-    <row r="3" spans="1:8" ht="28.8">
+    <row r="3" spans="1:8" ht="30">
       <c r="A3" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="B3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C3" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="D3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>327</v>
+      </c>
+      <c r="F3" s="33" t="s">
         <v>329</v>
       </c>
-      <c r="E3" s="33" t="s">
-        <v>328</v>
-      </c>
-      <c r="F3" s="33" t="s">
+      <c r="G3" s="33" t="s">
         <v>330</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="111.75" customHeight="1">
       <c r="A4" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C4" t="s">
-        <v>453</v>
+        <v>437</v>
       </c>
       <c r="D4" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="F4" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="28.8">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30">
       <c r="A5" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="B5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C5" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="D5" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>443</v>
+        <v>427</v>
       </c>
       <c r="F5" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="57.6">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60">
       <c r="A6" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C6" t="s">
-        <v>454</v>
+        <v>438</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>451</v>
+        <v>435</v>
       </c>
       <c r="F6" t="s">
-        <v>450</v>
+        <v>434</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="43.2">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45">
       <c r="A7" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="B7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C7" t="s">
-        <v>445</v>
+        <v>429</v>
       </c>
       <c r="D7" t="s">
-        <v>439</v>
+        <v>423</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F7" t="s">
-        <v>440</v>
+        <v>424</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C8" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="G8" s="33"/>
     </row>
-    <row r="9" spans="1:8" ht="230.4">
+    <row r="9" spans="1:8" ht="255">
       <c r="A9" s="38" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="B9" s="38" t="s">
+        <v>375</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>382</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>384</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>390</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>385</v>
+      </c>
+      <c r="G9" s="39" t="s">
         <v>391</v>
       </c>
-      <c r="C9" s="38" t="s">
-        <v>398</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>400</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>406</v>
-      </c>
-      <c r="F9" s="38" t="s">
-        <v>401</v>
-      </c>
-      <c r="G9" s="39" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="28.8">
+    </row>
+    <row r="10" spans="1:8" ht="45">
       <c r="A10" s="38" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
       <c r="E10" s="39" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="F10" s="39" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="G10" s="39" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B10" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>statementCategories</formula1>
     </dataValidation>
   </dataValidations>
@@ -5535,7 +5461,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -5543,69 +5469,69 @@
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
-    <col min="6" max="6" width="55.33203125" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="55.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
       <c r="B1" t="s">
         <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="D1" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="E1" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="F1" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
       <c r="G1" t="s">
-        <v>416</v>
+        <v>400</v>
       </c>
       <c r="H1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I1" t="s">
         <v>31</v>
       </c>
       <c r="J1" t="s">
-        <v>417</v>
+        <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="B2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C2" t="s">
-        <v>458</v>
+        <v>442</v>
       </c>
       <c r="D2" t="s">
-        <v>459</v>
+        <v>443</v>
       </c>
       <c r="E2" t="s">
-        <v>460</v>
+        <v>444</v>
       </c>
       <c r="F2" t="s">
-        <v>461</v>
+        <v>445</v>
       </c>
       <c r="G2" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
       <c r="H2">
         <v>-0.5</v>
@@ -5618,74 +5544,68 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" customWidth="1"/>
-    <col min="6" max="6" width="72.5546875" customWidth="1"/>
-    <col min="7" max="7" width="25.88671875" customWidth="1"/>
+    <col min="1" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="72.5703125" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
     <col min="8" max="8" width="75" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="26.88671875" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>438</v>
+        <v>422</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>436</v>
-      </c>
-      <c r="B2" t="str">
-        <f>AdministrativeData!C31</f>
-        <v>DFM255</v>
-      </c>
-      <c r="C2" t="str">
-        <f>AdministrativeData!C32</f>
-        <v>DK</v>
-      </c>
-      <c r="D2" t="str">
-        <f>AdministrativeData!C33</f>
-        <v>DANAK</v>
+        <v>420</v>
+      </c>
+      <c r="B2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>319</v>
       </c>
       <c r="E2">
-        <f>AdministrativeData!C34</f>
         <v>255</v>
       </c>
       <c r="F2">
-        <f>AdministrativeData!C35</f>
         <v>17025</v>
       </c>
       <c r="G2">
-        <f>AdministrativeData!C36</f>
         <v>2</v>
       </c>
     </row>
@@ -5696,7 +5616,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:S26"/>
   <sheetViews>
@@ -5704,58 +5624,58 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" customWidth="1"/>
-    <col min="11" max="11" width="15.44140625" customWidth="1"/>
-    <col min="12" max="12" width="12.88671875" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" customWidth="1"/>
-    <col min="16" max="16" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="42" t="s">
-        <v>338</v>
-      </c>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
+      <c r="G1" s="46" t="s">
+        <v>337</v>
+      </c>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
     </row>
     <row r="2" spans="1:19" ht="17.25" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="26" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -5783,12 +5703,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" ht="23.25">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>21</v>
@@ -5815,39 +5735,39 @@
         <v>18</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="P9" s="12" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="R9" s="12" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="21.6">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="23.25">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>23</v>
@@ -5871,10 +5791,10 @@
         <v>39</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="L10" s="12" t="s">
         <v>24</v>
@@ -5901,181 +5821,181 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="42">
+    <row r="11" spans="1:19" ht="45.75">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O11" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
       <c r="R11" s="11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="S11" s="11" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="21.6">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="23.25">
       <c r="A12" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>423</v>
+        <v>407</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>423</v>
+        <v>407</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>423</v>
+        <v>407</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>423</v>
+        <v>407</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>423</v>
+        <v>407</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="M12" s="15" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>427</v>
+        <v>411</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>427</v>
+        <v>411</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
       <c r="Q12" s="14" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
       <c r="R12" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="S12" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:19">
       <c r="A13" s="35" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="I13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="L13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="M13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="N13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="O13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="P13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="Q13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="R13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="S13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -6083,7 +6003,7 @@
         <v>30</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
@@ -6108,7 +6028,7 @@
         <v>32</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>419</v>
+        <v>403</v>
       </c>
       <c r="C15" s="17">
         <v>1000</v>
@@ -6135,7 +6055,7 @@
         <v>33</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="C16" s="17">
         <v>5000</v>
@@ -6162,7 +6082,7 @@
         <v>34</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>421</v>
+        <v>405</v>
       </c>
       <c r="C17" s="17">
         <v>10000</v>
@@ -6222,16 +6142,16 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:S11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:S11" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>MeasurandType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:S9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:S9" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>ColType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:S10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:S10" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>MetaType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:S13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:S13" xr:uid="{00000000-0002-0000-0500-000003000000}">
       <formula1>metaDataType</formula1>
     </dataValidation>
   </dataValidations>
@@ -6241,282 +6161,282 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="5" width="25.33203125" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" customWidth="1"/>
-    <col min="10" max="10" width="27.33203125" customWidth="1"/>
-    <col min="11" max="11" width="21.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
     <col min="12" max="12" width="31" customWidth="1"/>
-    <col min="13" max="13" width="14.21875" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
     <col min="14" max="14" width="26" customWidth="1"/>
-    <col min="15" max="15" width="19.109375" customWidth="1"/>
-    <col min="16" max="16" width="21.44140625" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" customWidth="1"/>
+    <col min="16" max="16" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="3" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="I1" s="43" t="s">
-        <v>475</v>
-      </c>
-      <c r="J1" s="43" t="s">
-        <v>477</v>
-      </c>
-      <c r="K1" s="43" t="s">
+      <c r="I1" s="42" t="s">
+        <v>459</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>461</v>
+      </c>
+      <c r="K1" s="42" t="s">
+        <v>460</v>
+      </c>
+      <c r="L1" s="42" t="s">
+        <v>462</v>
+      </c>
+      <c r="M1" s="43" t="s">
+        <v>472</v>
+      </c>
+      <c r="N1" s="43" t="s">
+        <v>471</v>
+      </c>
+      <c r="O1" s="43" t="s">
+        <v>473</v>
+      </c>
+      <c r="P1" s="43" t="s">
         <v>476</v>
-      </c>
-      <c r="L1" s="43" t="s">
-        <v>478</v>
-      </c>
-      <c r="M1" s="44" t="s">
-        <v>488</v>
-      </c>
-      <c r="N1" s="44" t="s">
-        <v>487</v>
-      </c>
-      <c r="O1" s="44" t="s">
-        <v>489</v>
-      </c>
-      <c r="P1" s="44" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="B2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C2" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
       <c r="D2" t="s">
         <v>55</v>
       </c>
       <c r="E2" t="s">
+        <v>453</v>
+      </c>
+      <c r="F2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G2" t="s">
+        <v>303</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>457</v>
+      </c>
+      <c r="I2" t="s">
+        <v>463</v>
+      </c>
+      <c r="J2" t="s">
+        <v>466</v>
+      </c>
+      <c r="K2" t="s">
+        <v>468</v>
+      </c>
+      <c r="L2" t="s">
         <v>469</v>
       </c>
-      <c r="F2" t="s">
-        <v>303</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="M2" t="s">
         <v>304</v>
       </c>
-      <c r="H2" s="27" t="s">
-        <v>473</v>
-      </c>
-      <c r="I2" t="s">
-        <v>479</v>
-      </c>
-      <c r="J2" t="s">
-        <v>482</v>
-      </c>
-      <c r="K2" t="s">
-        <v>484</v>
-      </c>
-      <c r="L2" t="s">
-        <v>485</v>
-      </c>
-      <c r="M2" t="s">
-        <v>305</v>
-      </c>
       <c r="N2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="O2" t="s">
-        <v>491</v>
+        <v>475</v>
       </c>
       <c r="P2" t="s">
-        <v>490</v>
+        <v>474</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="B3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C3" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="D3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E3" t="s">
+        <v>454</v>
+      </c>
+      <c r="F3" t="s">
+        <v>302</v>
+      </c>
+      <c r="G3" t="s">
         <v>335</v>
       </c>
-      <c r="E3" t="s">
-        <v>470</v>
-      </c>
-      <c r="F3" t="s">
-        <v>303</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" s="27" t="s">
+        <v>458</v>
+      </c>
+      <c r="I3" t="s">
+        <v>464</v>
+      </c>
+      <c r="J3" t="s">
+        <v>466</v>
+      </c>
+      <c r="K3" t="s">
+        <v>468</v>
+      </c>
+      <c r="L3" t="s">
+        <v>469</v>
+      </c>
+      <c r="M3" t="s">
         <v>336</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="N3" t="s">
+        <v>339</v>
+      </c>
+      <c r="O3" t="s">
+        <v>475</v>
+      </c>
+      <c r="P3" t="s">
         <v>474</v>
-      </c>
-      <c r="I3" t="s">
-        <v>480</v>
-      </c>
-      <c r="J3" t="s">
-        <v>482</v>
-      </c>
-      <c r="K3" t="s">
-        <v>484</v>
-      </c>
-      <c r="L3" t="s">
-        <v>485</v>
-      </c>
-      <c r="M3" t="s">
-        <v>337</v>
-      </c>
-      <c r="N3" t="s">
-        <v>341</v>
-      </c>
-      <c r="O3" t="s">
-        <v>491</v>
-      </c>
-      <c r="P3" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="B4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C4" t="s">
+        <v>450</v>
+      </c>
+      <c r="D4" t="s">
+        <v>342</v>
+      </c>
+      <c r="E4" t="s">
+        <v>455</v>
+      </c>
+      <c r="F4" t="s">
+        <v>302</v>
+      </c>
+      <c r="G4" t="s">
+        <v>343</v>
+      </c>
+      <c r="H4" t="s">
+        <v>344</v>
+      </c>
+      <c r="I4" t="s">
+        <v>333</v>
+      </c>
+      <c r="J4" t="s">
         <v>466</v>
       </c>
-      <c r="D4" t="s">
-        <v>344</v>
-      </c>
-      <c r="E4" t="s">
-        <v>471</v>
-      </c>
-      <c r="F4" t="s">
-        <v>303</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="K4" t="s">
+        <v>468</v>
+      </c>
+      <c r="L4" t="s">
+        <v>469</v>
+      </c>
+      <c r="M4" t="s">
         <v>345</v>
       </c>
-      <c r="H4" t="s">
-        <v>346</v>
-      </c>
-      <c r="I4" t="s">
-        <v>334</v>
-      </c>
-      <c r="J4" t="s">
-        <v>482</v>
-      </c>
-      <c r="K4" t="s">
-        <v>484</v>
-      </c>
-      <c r="L4" t="s">
-        <v>485</v>
-      </c>
-      <c r="M4" t="s">
-        <v>347</v>
-      </c>
       <c r="N4" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="O4" t="s">
-        <v>491</v>
+        <v>475</v>
       </c>
       <c r="P4" t="s">
-        <v>490</v>
+        <v>474</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
       <c r="C5" t="s">
+        <v>451</v>
+      </c>
+      <c r="D5" t="s">
+        <v>439</v>
+      </c>
+      <c r="E5" t="s">
+        <v>456</v>
+      </c>
+      <c r="F5" t="s">
+        <v>440</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>441</v>
+      </c>
+      <c r="I5" t="s">
+        <v>465</v>
+      </c>
+      <c r="J5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K5" t="s">
         <v>467</v>
       </c>
-      <c r="D5" t="s">
-        <v>455</v>
-      </c>
-      <c r="E5" t="s">
-        <v>472</v>
-      </c>
-      <c r="F5" t="s">
-        <v>456</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>457</v>
-      </c>
-      <c r="I5" t="s">
-        <v>481</v>
-      </c>
-      <c r="J5" t="s">
-        <v>482</v>
-      </c>
-      <c r="K5" t="s">
-        <v>483</v>
-      </c>
       <c r="L5" t="s">
-        <v>486</v>
+        <v>470</v>
       </c>
       <c r="M5" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="N5" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="O5" t="s">
-        <v>491</v>
+        <v>475</v>
       </c>
       <c r="P5" t="s">
-        <v>490</v>
+        <v>474</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6 I6 M6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6 I6 M6" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>EquipmentCategories</formula1>
     </dataValidation>
   </dataValidations>
@@ -6529,65 +6449,65 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" customWidth="1"/>
-    <col min="10" max="12" width="14.5546875" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
-    <col min="14" max="14" width="16.88671875" customWidth="1"/>
-    <col min="17" max="17" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="12" width="14.5703125" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="42" t="s">
-        <v>338</v>
-      </c>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
+      <c r="G1" s="46" t="s">
+        <v>337</v>
+      </c>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
       <c r="L1" s="41"/>
     </row>
     <row r="2" spans="1:17" ht="17.25" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="26" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -6620,7 +6540,7 @@
         <v>44</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>20</v>
@@ -6656,24 +6576,24 @@
         <v>21</v>
       </c>
       <c r="N9" s="11" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="O9" s="11" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="P9" s="11" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="Q9" s="11" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="21.6">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="23.25">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>23</v>
@@ -6700,16 +6620,16 @@
         <v>2</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
       <c r="L10" s="11" t="s">
         <v>4</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="N10" s="11" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="O10" s="11" t="s">
         <v>39</v>
@@ -6721,57 +6641,57 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="21.6">
+    <row r="11" spans="1:17" ht="23.25">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M11" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="O11" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="N11" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="O11" s="11" t="s">
-        <v>164</v>
-      </c>
       <c r="P11" s="11" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -6779,7 +6699,7 @@
         <v>31</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>27</v>
@@ -6809,83 +6729,83 @@
         <v>27</v>
       </c>
       <c r="L12" s="14" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="M12" s="15" t="s">
         <v>28</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="O12" s="14" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="Q12" s="14" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="23.25">
       <c r="A13" s="35" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="I13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="L13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="M13" s="34" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="N13" s="34" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="O13" s="34" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="P13" s="34" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="Q13" s="34" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="31.8">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="34.5">
       <c r="A14" s="22" t="s">
-        <v>493</v>
+        <v>477</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>17</v>
@@ -6909,10 +6829,10 @@
         <v>42</v>
       </c>
       <c r="J14" s="22" t="s">
-        <v>449</v>
+        <v>433</v>
       </c>
       <c r="K14" s="22" t="s">
-        <v>448</v>
+        <v>432</v>
       </c>
       <c r="L14" s="22" t="s">
         <v>4</v>
@@ -6921,69 +6841,69 @@
         <v>47</v>
       </c>
       <c r="N14" s="22" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="O14" s="22" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="P14" s="22" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="Q14" s="22" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="31.8">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="34.5">
       <c r="A15" s="22" t="s">
-        <v>494</v>
+        <v>478</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>508</v>
+        <v>492</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>495</v>
+        <v>479</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>496</v>
+        <v>480</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>497</v>
+        <v>481</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>498</v>
+        <v>482</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>499</v>
+        <v>483</v>
       </c>
       <c r="H15" s="23" t="s">
-        <v>500</v>
+        <v>484</v>
       </c>
       <c r="I15" s="23" t="s">
         <v>42</v>
       </c>
       <c r="J15" s="22" t="s">
-        <v>501</v>
+        <v>485</v>
       </c>
       <c r="K15" s="22" t="s">
-        <v>502</v>
+        <v>486</v>
       </c>
       <c r="L15" s="22" t="s">
-        <v>450</v>
+        <v>434</v>
       </c>
       <c r="M15" s="23" t="s">
-        <v>503</v>
+        <v>487</v>
       </c>
       <c r="N15" s="22" t="s">
-        <v>504</v>
+        <v>488</v>
       </c>
       <c r="O15" s="22" t="s">
-        <v>505</v>
+        <v>489</v>
       </c>
       <c r="P15" s="22" t="s">
-        <v>506</v>
+        <v>490</v>
       </c>
       <c r="Q15" s="22" t="s">
-        <v>507</v>
+        <v>491</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -7029,16 +6949,16 @@
         <v>1</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>445</v>
+        <v>429</v>
       </c>
       <c r="P16" s="9" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="Q16" s="9" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -7084,16 +7004,16 @@
         <v>2</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="P17" s="9" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="Q17" s="9" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -7139,16 +7059,16 @@
         <v>3</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="P18" s="9" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="Q18" s="9" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -7194,16 +7114,16 @@
         <v>4</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>445</v>
+        <v>429</v>
       </c>
       <c r="P19" s="9" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="Q19" s="9" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -7249,16 +7169,16 @@
         <v>5</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="O20" s="7" t="s">
-        <v>445</v>
+        <v>429</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="Q20" s="9" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -7300,16 +7220,16 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:Q13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:Q13" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>metaDataType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:Q10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:Q10" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>MetaType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:Q9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:Q9" xr:uid="{00000000-0002-0000-0700-000002000000}">
       <formula1>ColType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:Q11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:Q11" xr:uid="{00000000-0002-0000-0700-000003000000}">
       <formula1>MeasurandType</formula1>
     </dataValidation>
   </dataValidations>
@@ -7319,7 +7239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -7327,42 +7247,42 @@
       <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.88671875" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="I1" s="3"/>
     </row>

</xml_diff>